<commit_message>
fixed the formatting of image and text in overview tab (the text still needs some small tweaks)
</commit_message>
<xml_diff>
--- a/data-raw/texts.xlsx
+++ b/data-raw/texts.xlsx
@@ -71,7 +71,7 @@
 The Belgian fishing fleet is composed of 65 active vessels, primarily beam trawlers both above and below 24 m in length.
 Few vessels are smaller than 12 m. Most of the catch is demersal species; sole is the dominant species in value, and plaice
 the dominant species in volume. Other important species include Norway lobster, anglerfish, turbot, shrimp, lemon sole,
-common cuttlefish, squid, rays, and cod.
+common cuttlefish, squid, rays, and cod.&lt;br&gt;&lt;br&gt;
 &lt;b&gt;Denmark&lt;/b&gt;&lt;br&gt;
 The Danish fleet in 2019 had 717 vessels operating in the Greater North Sea, representing around half of the entire Danish
 fleet (1560 vessels). The size of the fleet has been generally decreasing over the last decade and in 2010 there were 968
@@ -92,7 +92,7 @@
 northern shrimp, and Nephrops using predominantly bottom trawls with some seine activity. This pattern has been
 consistent over the last ten years. The most important pelagic fisheries target herring and mackerel for human
 consumption, and sandeel, sprat, and Norway pout for reduction purposes (i.e. fish meal and oils), which is also consistent
-for the period.
+for the period.&lt;br&gt;&lt;br&gt;
 &lt;b&gt;France&lt;/b&gt;&lt;br&gt;
 The French fleet in the North Sea is composed of more than 600 vessels. The demersal fisheries operate mainly in the
 eastern English Channel and southern North Sea and catch a variety of finfish and shellfish species. Up until 2016, the
@@ -102,7 +102,7 @@
 Division 7.d and the southern part of Division 4.c. Smaller boats operate different gears throughout the year and target 
 different species assemblages. There is also a fleet of six large demersal trawlers ( &gt;40 m) that target saithe in the northern
 North Sea and to the west of Scotland. The pelagic fishery is prosecuted by three active vessels catching herring, mackerel,
-and horse-mackerel.
+and horse-mackerel.&lt;br&gt;&lt;br&gt;
 &lt;B&gt;Germany&lt;/b&gt;&lt;br&gt;
 The German North Sea fishing fleet comprises more than 200 vessels. Small beam trawlers of 12–24 m length constitute
 the largest fleet component (around 175 vessels in 2019) and almost exclusively target brown shrimp in the southern North
@@ -116,14 +116,14 @@
 Overall, a reduction in the number of vessels was recorded for the German North Sea fishing fleet during the last ten years.
 Especially the number of smaller beam trawlers (12–18 m length, 35 fewer vessels or −25%) and demersal otter trawlers
 (18–24 m length, 14 fewer vessels or −50%) decreased. The number of large pelagic trawlers stayed stable with five vessels
-for the last ten years.
+for the last ten years.&lt;br&gt;&lt;br&gt;
 &lt;b&gt;Netherlands&lt;/b&gt;&lt;br&gt;
 The Dutch fleet in the Greater North Sea consists of about 500 vessels. The main demersal fleet is the beam trawl fleet
 (275 vessels, of which 85 are &gt; 24 m and 190 are &lt; 24 m) that operates in the southern and central North Sea, targeting
 sole (dominant in value) and plaice (dominant in volume) as well as other flatfish species. Until the recent EU-wide ban on
 pulse trawling most of the &gt; 24 m beam trawlers have used pulse trawls. Most of the smaller beam trawlers (“Eurocutters”)
 seasonally target shrimp or flatfish. Pelagic freezer trawlers (seven vessels, &gt; 60 m) target pelagic species, mainly herring,
-mackerel, and horse mackerel.
+mackerel, and horse mackerel.&lt;br&gt;&lt;br&gt;
 &lt;b&gt;Norway&lt;/b&gt;&lt;br&gt;
 The Norwegian North Sea fleet is composed of about 1500 vessels. Approximately 94% of these catch demersal species,
 including fish, crustaceans, and elasmobranchs, while 33% catch pelagic species, including herring, blue whiting, mackerel,
@@ -140,7 +140,7 @@
 Ten years ago, larger vessels accounted for over 20% of the fleet (9% 24–40 m; 13% &gt; 40m), which factors in both the
 increase of the number of small vessels and a slight decrease in the number of vessels &gt; 24 m (−13%). The largest vessels
 among them ( &gt;40 m) are mostly pelagic trawlers and purse-seiners that operate offshore and account for more than 80%
-of the total landings (up from 75% in ten years; +40% in absolute landing tonnage).
+of the total landings (up from 75% in ten years; +40% in absolute landing tonnage).&lt;br&gt;&lt;br&gt;
 &lt;b&gt;Sweden&lt;/b&gt;&lt;br&gt;
 The Swedish fleet in the Greater North Sea comprises more than 400 vessels. Most vessels operate in the Skagerrak and
 Kattegat, but around 25 of them also fish in the North Sea. In total around 130 vessels are involved in demersal trawl
@@ -155,7 +155,7 @@
 fleet are reduced fishing opportunities, poor profitability, scrapping campaigns, and the introduction of annually
 transferable fishing rights in the demersal fleets in 2017. The fleet reduction is most pronounced in the Skagerrak and
 Kattegat, whereas the pelagic fleet and the demersal vessels fishing in the North Sea have been rather stable in terms of
-number of vessels over the last decade.
+number of vessels over the last decade.&lt;br&gt;&lt;br&gt;
 &lt;b&gt;UK (England)&lt;/b&gt;&lt;br&gt;
 The English fleet operating in the Greater North Sea ecoregion during 2019 was comprised of 1133 vessels, with a decrease
 of 33 vessels from 2018. The decrease is part of a longer running trend across many sectors, but most noticeably in the
@@ -170,7 +170,7 @@
 in recent years. This sector predominantly targets cockle and edible crab, with only around 12 vessels targeting
 demersal finfish.
  There were 12 English vessels over 40 m operating in the North Sea in 2019 and this number has been virtually
-unchanged since 2009. This largest category of vessel targets finfish, mostly demersal but some pelagic.
+unchanged since 2009. This largest category of vessel targets finfish, mostly demersal but some pelagic.&lt;br&gt;&lt;br&gt;
 &lt;b&gt;UK (Scotland)&lt;/b&gt;&lt;br&gt;
 The Scottish North Sea fleet comprises around 1000 vessels. More than 120 demersal trawlers (almost all &gt; 10 m) fish for
 mixed gadoids (cod, haddock, whiting, saithe, and hake,) and for groundfish such as anglerfish and megrim. A fleet of 139
@@ -178,7 +178,7 @@
 91 ( &gt; 10 m) operate over various offshore grounds. Pot or creel fishing is prosecuted by over 650 vessels (mostly &lt; 10 m)
 targeting lobsters and various crab species on harder inshore grounds. Scallop fishing is carried out by around 80 dredgers
 (mostly &gt; 10 m). Limited amounts of longlining and gillnetting are also conducted by Scottish vessels. Significant catches of
-pelagic species are harvested by 18 large vessels, primarily using pelagic trawls.
+pelagic species are harvested by 18 large vessels, primarily using pelagic trawls.&lt;br&gt;&lt;br&gt;
 The Faroe Islands also fish in the Greater North Sea, but ICES does not have information on this fleet.</t>
   </si>
 </sst>

</xml_diff>

<commit_message>
Update layout of bycatch and landings tabs. Adding text in sidebars
</commit_message>
<xml_diff>
--- a/data-raw/texts.xlsx
+++ b/data-raw/texts.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilm\Projects\fisheriesXplorer\data-raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22816777-6EF0-4493-BC0A-1441772498D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="28800" windowHeight="15030" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="overview"/>
+    <sheet name="overview" sheetId="1" r:id="rId1"/>
+    <sheet name="landings_discards" sheetId="2" r:id="rId2"/>
+    <sheet name="bycatch" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>section</t>
   </si>
@@ -25,36 +33,13 @@
     <t>executive_summary</t>
   </si>
   <si>
-    <t>Around 6600 fishing vessels are active in the Greater North Sea. Total landings peaked in the 1970s at 4 million tonnes and have since declined to about 2 million tonnes. Total fishing effort has declined substantially since 2003. Pelagic fish landings are greater than demersal fish landings. Herring and mackerel, caught using pelagic trawls and seines, account for the largest portion of the pelagic landings, while sandeel and haddock, caught using otter trawls/seines, account for the largest fraction of the demersal landings. Catches are taken from more than 100 stocks. Discards are highest in the demersal and benthic fisheries. The spatial distribution of fishing gear varies across the Greater North Sea. Static gear is used most frequently in the English Channel, the eastern part of the Southern Bight, the Danish banks, and in the waters east of Shetland. Bottom trawls are used throughout the North Sea, with lower use in the shallower southern North Sea, where beam trawls are most commonly used. Pelagic gears are used throughout the North Sea. &lt;br&gt;&lt;br&gt;In terms of weight of catch, fish stocks harvested from the North Sea are being fished at levels consistent with achieving good environmental status (GES) under the EU’s Marine Strategy Framework Directive; however, the reproductive capacity of the stocks has not generally reached this level. Almost all the fisheries in the North Sea catch more than one species; controlling fishing on one species therefore affects other species as well. ICES has developed a number of scenarios for fishing opportunities that take account of these technical interactions. Each of these scenarios results in different outcomes for the fish stocks. Managers may need to take these scenarios into account when deciding upon fishing opportunities. Furthermore, biological interactions occur between species (e.g. predation), and fishing on one stock may affect the population dynamics of another. Scenarios that take account of these various interactions can be used to evaluate the possible consequences of policy decisions. The greatest physical disturbances of the seabed caused by fishing activity in the North Sea is caused by mobile bottom-contacting gear in the eastern English Channel, in nearshore areas in the southeastern North Sea and in the central Skagerrak. Incidental bycatches of protected, endangered, and threatened species occur in several North Sea fisheries, and the bycatch of common dolphin in the western English Channel may be unsustainable in terms of population. &lt;br&gt;&lt;br&gt;Supporting data used in the Greater North Sea fisheries overview is accessible at &lt;a href="https://doi.org/10.17895/ices.advice.21641360"&gt;ICES Library&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>introduction</t>
   </si>
   <si>
-    <t xml:space="preserve">The Greater North Sea ecoregion includes the North Sea, English Channel, Skagerrak, and Kattegat. The Greater North Sea
-is a relatively shallow sea area on the European continental shelf, with the exception of the Norwegian Trench that extends
-parallel to the Norwegian shoreline. Pelag+B3ic species (primarily herring and mackerel) account for a significant portion of
-the total commercial fish landings in the region. Landings of benthic and demersal finfish species (primarily haddock,
-sandeel, flatfish, and cod) are also significant. &lt;br&gt;&lt;br&gt; 
-All of the Greater North Sea ecoregion lies within FAO Major Fishing Area 27; the prefix “27” in the ICES statistical area
-codes is therefore omitted in the following. This overview covers ICES Division 3.a, most of divisions 4.a, 4.b, 4.c, 7.d, and
-part of Division 7.e, as well as Subdivision 3.b.23. This overview does not include the fisheries in the western English
-Channel (Division 7.e) and in the Sound (Division 3.b.23).
-Note that updates to the figures using data from the stock assessment graphs (SAG) include only advice published before
-10 October 2022. Therefore anf.27.3a46, meg.27.7b-k8abd, rjn.27.678abd, and the Norway lobster stocks refer to the
-advice current at this time (the advice applicable for 2022).&lt;br&gt;&lt;br&gt; 
-This overview provides:&lt;br&gt; 
-&lt;ol&gt;&lt;li&gt; a short description of each of the national commercial fishing fleets in the ecoregion, including their fishing gears,
-and spatial and temporal patterns of activity;
-&lt;li&gt; a summary of the status of the fisheries resources and the level of exploitation relative to agreed objectives and
-reference points;
-&lt;li&gt; mixed-fisheries considerations of relevance to the management of the fisheries; and
-&lt;li&gt; an evaluation of the effects of fishing gear on the ecosystem in terms of the seabed and on the bycatch of
-protected, endangered, and threatened species.&lt;/ol&gt;&lt;br&gt;&lt;br&gt; 
-The scientific names of all species described in this overview are listed in Table A2 in the Annex. </t>
-  </si>
-  <si>
     <t>who_is_fishing</t>
+  </si>
+  <si>
+    <t>Around 6600 fishing vessels are active in the Greater North Sea. Total landings peaked in the 1970s at 4 million tonnes and have since declined to about 2 million tonnes. Total fishing effort has declined substantially since 2003. Pelagic fish landings are greater than demersal fish landings. Herring and mackerel, caught using pelagic trawls and seines, account for the largest portion of the pelagic landings, while sandeel and haddock, caught using otter trawls/seines, account for the largest fraction of the demersal landings. Catches are taken from more than 100 stocks. Discards are highest in the demersal and benthic fisheries. The spatial distribution of fishing gear varies across the Greater North Sea. Static gear is used most frequently in the English Channel, the eastern part of the Southern Bight, the Danish banks, and in the waters east of Shetland. Bottom trawls are used throughout the North Sea, with lower use in the shallower southern North Sea, where beam trawls are most commonly used. Pelagic gears are used throughout the North Sea. &lt;br&gt;&lt;br&gt;In terms of weight of catch, fish stocks harvested from the North Sea are being fished at levels consistent with achieving good environmental status (GES) under the EU’s Marine Strategy Framework Directive; however, the reproductive capacity of the stocks has not generally reached this level. Almost all the fisheries in the North Sea catch more than one species; controlling fishing on one species therefore affects other species as well. ICES has developed a number of scenarios for fishing opportunities that take account of these technical interactions. Each of these scenarios results in different outcomes for the fish stocks. Managers may need to take these scenarios into account when deciding upon fishing opportunities. Furthermore, biological interactions occur between species (e.g. predation), and fishing on one stock may affect the population dynamics of another. Scenarios that take account of these various interactions can be used to evaluate the possible consequences of policy decisions. The greatest physical disturbances of the seabed caused by fishing activity in the North Sea is caused by mobile bottom-contacting gear in the eastern English Channel, in nearshore areas in the southeastern North Sea and in the central Skagerrak. Incidental bycatches of protected, endangered, and threatened species occur in several North Sea fisheries, and the bycatch of common dolphin in the western English Channel may be unsustainable in terms of population. &lt;br&gt;&lt;br&gt;Supporting data used in the Greater North Sea fisheries overview is accessible at &lt;a href="https://doi.org/10.17895/ices.advice.21641360"&gt;ICES Library&lt;/a&gt;&lt;br&gt;&lt;br&gt;</t>
   </si>
   <si>
     <t>Around 6600 vessels from nine nations operate in the Greater North Sea, with the largest numbers coming from UK,
@@ -179,14 +164,58 @@
 targeting lobsters and various crab species on harder inshore grounds. Scallop fishing is carried out by around 80 dredgers
 (mostly &gt; 10 m). Limited amounts of longlining and gillnetting are also conducted by Scottish vessels. Significant catches of
 pelagic species are harvested by 18 large vessels, primarily using pelagic trawls.&lt;br&gt;&lt;br&gt;
-The Faroe Islands also fish in the Greater North Sea, but ICES does not have information on this fleet.</t>
+The Faroe Islands also fish in the Greater North Sea, but ICES does not have information on this fleet.&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>The Greater North Sea ecoregion includes the North Sea, English Channel, Skagerrak, and Kattegat. The Greater North Sea
+is a relatively shallow sea area on the European continental shelf, with the exception of the Norwegian Trench that extends
+parallel to the Norwegian shoreline. Pelagic species (primarily herring and mackerel) account for a significant portion of
+the total commercial fish landings in the region. Landings of benthic and demersal finfish species (primarily haddock,
+sandeel, flatfish, and cod) are also significant. &lt;br&gt;&lt;br&gt; 
+All of the Greater North Sea ecoregion lies within FAO Major Fishing Area 27; the prefix “27” in the ICES statistical area
+codes is therefore omitted in the following. This overview covers ICES Division 3.a, most of divisions 4.a, 4.b, 4.c, 7.d, and
+part of Division 7.e, as well as Subdivision 3.b.23. This overview does not include the fisheries in the western English
+Channel (Division 7.e) and in the Sound (Division 3.b.23).
+Note that updates to the figures using data from the stock assessment graphs (SAG) include only advice published before
+10 October 2022. Therefore anf.27.3a46, meg.27.7b-k8abd, rjn.27.678abd, and the Norway lobster stocks refer to the
+advice current at this time (the advice applicable for 2022).&lt;br&gt;&lt;br&gt; 
+This overview provides:&lt;br&gt;&lt;br&gt;
+&lt;ol style="font-size: 14px"&gt;
+&lt;li style="font-size: 14px"&gt;a short description of each of the national commercial fishing fleets in the ecoregion, including their fishing gears,
+and spatial and temporal patterns of activity;&lt;/li&gt;&lt;br&gt;&lt;br&gt;
+&lt;li style="font-size: 14px"&gt;a summary of the status of the fisheries resources and the level of exploitation relative to agreed objectives and
+reference points;&lt;/li&gt;&lt;br&gt;&lt;br&gt;
+&lt;li style="font-size: 14px"&gt;mixed-fisheries considerations of relevance to the management of the fisheries; and&lt;/li&gt;&lt;br&gt;&lt;br&gt;
+&lt;li style="font-size: 14px"&gt;an evaluation of the effects of fishing gear on the ecosystem in terms of the seabed and on the bycatch of
+protected, endangered, and threatened species.&lt;/li&gt;&lt;/ol&gt;&lt;br&gt;
+The scientific names of all species described in this overview are listed in Table A2 in the Annex. &lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>landings</t>
+  </si>
+  <si>
+    <t>discards</t>
+  </si>
+  <si>
+    <t>sidebar</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Landings&lt;/b&gt;&lt;br&gt;&lt;br&gt;Fisheries in the Greater North Sea catch a large diversity of species. These have been categorized into species that are pelagic, demersal, benthic (e.g. flatfish), crustaceans, and elasmobranchs. &lt;br&gt;&lt;br&gt;Total landings from the Greater North Sea varied between 2 and 3 million tonnes during the 1950s, then rose to between 3 and 4 million tonnes from the late 1960s to the mid-1990s (Figure 2). High catches of both pelagic species (mackerel and herring) and demersal species (cod and haddock) accounted for the increase in total landings in the late 1960s (figures 3 and 4). 
+The landings shown in Figure 4 only include those species for which ICES gives advice. There are a number of stocks for which ICES does not give advice where landings may be substantial (e.g. Scallop, edible crab, brown shrimp, European lobster, blue mussel). Total landings declined after 1995 to a low of 1.4 million tonnes in 2012. This decline is attributed to overfishing and decreased productivity of important stocks such as cod and herring, but also to the successful reduction of fishing mortality to more sustainable levels after 2000. &lt;br&gt;&lt;br&gt;
+Since 2003, the pelagic fisheries using pelagic trawl and purse seines have accounted for the largest proportion of the total landings, followed by the demersal and benthic fisheries (Figure 3). Overall landings increased slightly from 2011 after a rise in herring landings and again, most recently (in 2015), from increased catches of anchovy, sardine, and hake.&lt;br&gt;&lt;br&gt;
+Recreational fisheries in the North Sea target a wide range of species, but few of these fisheries are monitored or evaluated. Recreational catches of seabass and salmon (including freshwater for the latter) are significant and are included in ICES assessment of these species. In contrast, the recreational fisheries of elasmobranchs is not widely monitored; however, the recreational harvest of these species (mainly dogfish and several species of skates and rays) appears to be negligible.&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Discards&lt;/b&gt;&lt;br&gt;&lt;br&gt;Discard data have been collected for some North Sea fisheries since the mid-1970s. Since 2000, discard data from North Sea commercial fisheries have been collected from various observer programmes implemented under the EU Data Collection Framework (DCF), and UK continued that commitment in retained law from 2020 after leaving the EU. However, complete discard data are only available from 2012 onwards. In 2015–2019, discard rates remained relatively stable. Discard rates of pelagic species were close to zero (Figure 6). Discard estimates for several species of elasmobranch are highly uncertain due to low encounter probabilities and so are not shown.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Bycatch of protected, endangered, and threatened species&lt;/b&gt;&lt;br&gt;&lt;br&gt; All fisheries have the potential to catch protected, endangered, or threatened species, such as seabirds and marine mammals, as non-targeted bycatch. Data submitted to ICES through annual data calls indicated that between 2017–2021 ten ICES Member Countries had fisheries operating in the Greater North Sea ecoregion (ICES, 2022a). During the same period approximately 13 000 monitoring days were undertaken, primarily by at-sea observers, in a variety of static and mobile gears and on vessels ranging from under 8 m to over 40 m. Most bycatch data collection in the ecoregion is carried out within multipurpose programmes under the DCF and through dedicated bycatch monitoring programmes.&lt;br&gt;&lt;br&gt;&lt;b&gt; Bycatch records in 2021&lt;/b&gt;&lt;br&gt;&lt;br&gt; In 2021, 47 marine mammals from at least four species were recorded as bycatch, mostly in net métiers. Forty-two seabirds from at least five species were recorded as bycatch in bottom trawl, longline, purse-seine and net fisheries (Table 1). Over 13 000 specimens of fish of potential conservation interest were recorded from a wide mix of static and mobile gears. Most of the fish records were tub gurnard (Chelidonichthys lucerna) in bottom trawls. No turtles were reported as bycatch.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -229,35 +258,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -268,10 +288,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -309,71 +329,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -401,7 +421,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -424,11 +444,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -437,13 +457,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -453,7 +473,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -462,7 +482,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -471,7 +491,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -479,10 +499,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -547,50 +567,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView topLeftCell="A3" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="255.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="162">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" ht="162" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="549" customFormat="1" s="3">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="1574.25" customFormat="1" s="3">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4E976-B447-4DEF-A85E-11D6D9966CA4}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="255.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE2A7A1-C07D-40E0-A9E9-3CF06E261156}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="159.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test sections for stock status, mixfish, vms
</commit_message>
<xml_diff>
--- a/data-raw/texts.xlsx
+++ b/data-raw/texts.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilm\Projects\fisheriesXplorer\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22816777-6EF0-4493-BC0A-1441772498D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F934F0D4-6429-41F7-900E-CB6E10AD2E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="28800" windowHeight="15030" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2745" yWindow="3645" windowWidth="28800" windowHeight="15030" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
     <sheet name="landings_discards" sheetId="2" r:id="rId2"/>
     <sheet name="bycatch" sheetId="3" r:id="rId3"/>
+    <sheet name="status" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>section</t>
   </si>
@@ -39,10 +41,55 @@
     <t>who_is_fishing</t>
   </si>
   <si>
-    <t>Around 6600 fishing vessels are active in the Greater North Sea. Total landings peaked in the 1970s at 4 million tonnes and have since declined to about 2 million tonnes. Total fishing effort has declined substantially since 2003. Pelagic fish landings are greater than demersal fish landings. Herring and mackerel, caught using pelagic trawls and seines, account for the largest portion of the pelagic landings, while sandeel and haddock, caught using otter trawls/seines, account for the largest fraction of the demersal landings. Catches are taken from more than 100 stocks. Discards are highest in the demersal and benthic fisheries. The spatial distribution of fishing gear varies across the Greater North Sea. Static gear is used most frequently in the English Channel, the eastern part of the Southern Bight, the Danish banks, and in the waters east of Shetland. Bottom trawls are used throughout the North Sea, with lower use in the shallower southern North Sea, where beam trawls are most commonly used. Pelagic gears are used throughout the North Sea. &lt;br&gt;&lt;br&gt;In terms of weight of catch, fish stocks harvested from the North Sea are being fished at levels consistent with achieving good environmental status (GES) under the EU’s Marine Strategy Framework Directive; however, the reproductive capacity of the stocks has not generally reached this level. Almost all the fisheries in the North Sea catch more than one species; controlling fishing on one species therefore affects other species as well. ICES has developed a number of scenarios for fishing opportunities that take account of these technical interactions. Each of these scenarios results in different outcomes for the fish stocks. Managers may need to take these scenarios into account when deciding upon fishing opportunities. Furthermore, biological interactions occur between species (e.g. predation), and fishing on one stock may affect the population dynamics of another. Scenarios that take account of these various interactions can be used to evaluate the possible consequences of policy decisions. The greatest physical disturbances of the seabed caused by fishing activity in the North Sea is caused by mobile bottom-contacting gear in the eastern English Channel, in nearshore areas in the southeastern North Sea and in the central Skagerrak. Incidental bycatches of protected, endangered, and threatened species occur in several North Sea fisheries, and the bycatch of common dolphin in the western English Channel may be unsustainable in terms of population. &lt;br&gt;&lt;br&gt;Supporting data used in the Greater North Sea fisheries overview is accessible at &lt;a href="https://doi.org/10.17895/ices.advice.21641360"&gt;ICES Library&lt;/a&gt;&lt;br&gt;&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>Around 6600 vessels from nine nations operate in the Greater North Sea, with the largest numbers coming from UK,
+    <t>landings</t>
+  </si>
+  <si>
+    <t>discards</t>
+  </si>
+  <si>
+    <t>sidebar</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Landings&lt;/b&gt;&lt;br&gt;&lt;br&gt;Fisheries in the Greater North Sea catch a large diversity of species. These have been categorized into species that are pelagic, demersal, benthic (e.g. flatfish), crustaceans, and elasmobranchs. &lt;br&gt;&lt;br&gt;Total landings from the Greater North Sea varied between 2 and 3 million tonnes during the 1950s, then rose to between 3 and 4 million tonnes from the late 1960s to the mid-1990s (Figure 2). High catches of both pelagic species (mackerel and herring) and demersal species (cod and haddock) accounted for the increase in total landings in the late 1960s (figures 3 and 4). 
+The landings shown in Figure 4 only include those species for which ICES gives advice. There are a number of stocks for which ICES does not give advice where landings may be substantial (e.g. Scallop, edible crab, brown shrimp, European lobster, blue mussel). Total landings declined after 1995 to a low of 1.4 million tonnes in 2012. This decline is attributed to overfishing and decreased productivity of important stocks such as cod and herring, but also to the successful reduction of fishing mortality to more sustainable levels after 2000. &lt;br&gt;&lt;br&gt;
+Since 2003, the pelagic fisheries using pelagic trawl and purse seines have accounted for the largest proportion of the total landings, followed by the demersal and benthic fisheries (Figure 3). Overall landings increased slightly from 2011 after a rise in herring landings and again, most recently (in 2015), from increased catches of anchovy, sardine, and hake.&lt;br&gt;&lt;br&gt;
+Recreational fisheries in the North Sea target a wide range of species, but few of these fisheries are monitored or evaluated. Recreational catches of seabass and salmon (including freshwater for the latter) are significant and are included in ICES assessment of these species. In contrast, the recreational fisheries of elasmobranchs is not widely monitored; however, the recreational harvest of these species (mainly dogfish and several species of skates and rays) appears to be negligible.&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Discards&lt;/b&gt;&lt;br&gt;&lt;br&gt;Discard data have been collected for some North Sea fisheries since the mid-1970s. Since 2000, discard data from North Sea commercial fisheries have been collected from various observer programmes implemented under the EU Data Collection Framework (DCF), and UK continued that commitment in retained law from 2020 after leaving the EU. However, complete discard data are only available from 2012 onwards. In 2015–2019, discard rates remained relatively stable. Discard rates of pelagic species were close to zero (Figure 6). Discard estimates for several species of elasmobranch are highly uncertain due to low encounter probabilities and so are not shown.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Bycatch of protected, endangered, and threatened species&lt;/b&gt;&lt;br&gt;&lt;br&gt; All fisheries have the potential to catch protected, endangered, or threatened species, such as seabirds and marine mammals, as non-targeted bycatch. Data submitted to ICES through annual data calls indicated that between 2017–2021 ten ICES Member Countries had fisheries operating in the Greater North Sea ecoregion (ICES, 2022a). During the same period approximately 13 000 monitoring days were undertaken, primarily by at-sea observers, in a variety of static and mobile gears and on vessels ranging from under 8 m to over 40 m. Most bycatch data collection in the ecoregion is carried out within multipurpose programmes under the DCF and through dedicated bycatch monitoring programmes.&lt;br&gt;&lt;br&gt;&lt;b&gt; Bycatch records in 2021&lt;/b&gt;&lt;br&gt;&lt;br&gt; In 2021, 47 marine mammals from at least four species were recorded as bycatch, mostly in net métiers. Forty-two seabirds from at least five species were recorded as bycatch in bottom trawl, longline, purse-seine and net fisheries (Table 1). Over 13 000 specimens of fish of potential conservation interest were recorded from a wide mix of static and mobile gears. Most of the fish records were tub gurnard (Chelidonichthys lucerna) in bottom trawls. No turtles were reported as bycatch.</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Around 6600 fishing vessels are active in the Greater North Sea. Total landings peaked in the 1970s at 4 million tonnes and have since declined to about 2 million tonnes. Total fishing effort has declined substantially since 2003. Pelagic fish landings are greater than demersal fish landings. Herring and mackerel, caught using pelagic trawls and seines, account for the largest portion of the pelagic landings, while sandeel and haddock, caught using otter trawls/seines, account for the largest fraction of the demersal landings. Catches are taken from more than 100 stocks. Discards are highest in the demersal and benthic fisheries. The spatial distribution of fishing gear varies across the Greater North Sea. Static gear is used most frequently in the English Channel, the eastern part of the Southern Bight, the Danish banks, and in the waters east of Shetland. Bottom trawls are used throughout the North Sea, with lower use in the shallower southern North Sea, where beam trawls are most commonly used. Pelagic gears are used throughout the North Sea. &lt;br&gt;&lt;br&gt;In terms of weight of catch, fish stocks harvested from the North Sea are being fished at levels consistent with achieving good environmental status (GES) under the EU’s Marine Strategy Framework Directive; however, the reproductive capacity of the stocks has not generally reached this level. Almost all the fisheries in the North Sea catch more than one species; controlling fishing on one species therefore affects other species as well. ICES has developed a number of scenarios for fishing opportunities that take account of these technical interactions. Each of these scenarios results in different outcomes for the fish stocks. Managers may need to take these scenarios into account when deciding upon fishing opportunities. Furthermore, biological interactions occur between species (e.g. predation), and fishing on one stock may affect the population dynamics of another. Scenarios that take account of these various interactions can be used to evaluate the possible consequences of policy decisions. The greatest physical disturbances of the seabed caused by fishing activity in the North Sea is caused by mobile bottom-contacting gear in the eastern English Channel, in nearshore areas in the southeastern North Sea and in the central Skagerrak. Incidental bycatches of protected, endangered, and threatened species occur in several North Sea fisheries, and the bycatch of common dolphin in the western English Channel may be unsustainable in terms of population. &lt;br&gt;&lt;br&gt;Supporting data used in the Greater North Sea fisheries overview is accessible at &lt;a href="https://doi.org/10.17895/ices.advice.21641360"&gt;ICES Library&lt;/a&gt;&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;The Greater North Sea ecoregion includes the North Sea, English Channel, Skagerrak, and Kattegat. The Greater North Sea
+is a relatively shallow sea area on the European continental shelf, with the exception of the Norwegian Trench that extends
+parallel to the Norwegian shoreline. Pelagic species (primarily herring and mackerel) account for a significant portion of
+the total commercial fish landings in the region. Landings of benthic and demersal finfish species (primarily haddock,
+sandeel, flatfish, and cod) are also significant. &lt;br&gt;&lt;br&gt; 
+All of the Greater North Sea ecoregion lies within FAO Major Fishing Area 27; the prefix “27” in the ICES statistical area
+codes is therefore omitted in the following. This overview covers ICES Division 3.a, most of divisions 4.a, 4.b, 4.c, 7.d, and
+part of Division 7.e, as well as Subdivision 3.b.23. This overview does not include the fisheries in the western English
+Channel (Division 7.e) and in the Sound (Division 3.b.23).
+Note that updates to the figures using data from the stock assessment graphs (SAG) include only advice published before
+10 October 2022. Therefore anf.27.3a46, meg.27.7b-k8abd, rjn.27.678abd, and the Norway lobster stocks refer to the
+advice current at this time (the advice applicable for 2022).&lt;br&gt;&lt;br&gt; 
+This overview provides:&lt;br&gt;&lt;br&gt;
+&lt;ol style="font-size: 14px"&gt;
+&lt;li style="font-size: 14px"&gt;a short description of each of the national commercial fishing fleets in the ecoregion, including their fishing gears,
+and spatial and temporal patterns of activity;&lt;/li&gt;&lt;br&gt;&lt;br&gt;
+&lt;li style="font-size: 14px"&gt;a summary of the status of the fisheries resources and the level of exploitation relative to agreed objectives and
+reference points;&lt;/li&gt;&lt;br&gt;&lt;br&gt;
+&lt;li style="font-size: 14px"&gt;mixed-fisheries considerations of relevance to the management of the fisheries; and&lt;/li&gt;&lt;br&gt;&lt;br&gt;
+&lt;li style="font-size: 14px"&gt;an evaluation of the effects of fishing gear on the ecosystem in terms of the seabed and on the bycatch of
+protected, endangered, and threatened species.&lt;/li&gt;&lt;/ol&gt;&lt;br&gt;
+The scientific names of all species described in this overview are listed in Table A2 in the Annex. &lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Around 6600 vessels from nine nations operate in the Greater North Sea, with the largest numbers coming from UK,
 Norway, Denmark, the Netherlands, and France. Total landings peaked in the early 1970s and have since declined. The
 proportion caught by each country of the total annual landings has varied over time (Figure 2). The following country
 paragraphs highlight features of the fleets and fisheries of each country but are not exhaustive descriptions.&lt;br&gt;&lt;br&gt;
@@ -167,49 +214,7 @@
 The Faroe Islands also fish in the Greater North Sea, but ICES does not have information on this fleet.&lt;br&gt;&lt;br&gt;</t>
   </si>
   <si>
-    <t>The Greater North Sea ecoregion includes the North Sea, English Channel, Skagerrak, and Kattegat. The Greater North Sea
-is a relatively shallow sea area on the European continental shelf, with the exception of the Norwegian Trench that extends
-parallel to the Norwegian shoreline. Pelagic species (primarily herring and mackerel) account for a significant portion of
-the total commercial fish landings in the region. Landings of benthic and demersal finfish species (primarily haddock,
-sandeel, flatfish, and cod) are also significant. &lt;br&gt;&lt;br&gt; 
-All of the Greater North Sea ecoregion lies within FAO Major Fishing Area 27; the prefix “27” in the ICES statistical area
-codes is therefore omitted in the following. This overview covers ICES Division 3.a, most of divisions 4.a, 4.b, 4.c, 7.d, and
-part of Division 7.e, as well as Subdivision 3.b.23. This overview does not include the fisheries in the western English
-Channel (Division 7.e) and in the Sound (Division 3.b.23).
-Note that updates to the figures using data from the stock assessment graphs (SAG) include only advice published before
-10 October 2022. Therefore anf.27.3a46, meg.27.7b-k8abd, rjn.27.678abd, and the Norway lobster stocks refer to the
-advice current at this time (the advice applicable for 2022).&lt;br&gt;&lt;br&gt; 
-This overview provides:&lt;br&gt;&lt;br&gt;
-&lt;ol style="font-size: 14px"&gt;
-&lt;li style="font-size: 14px"&gt;a short description of each of the national commercial fishing fleets in the ecoregion, including their fishing gears,
-and spatial and temporal patterns of activity;&lt;/li&gt;&lt;br&gt;&lt;br&gt;
-&lt;li style="font-size: 14px"&gt;a summary of the status of the fisheries resources and the level of exploitation relative to agreed objectives and
-reference points;&lt;/li&gt;&lt;br&gt;&lt;br&gt;
-&lt;li style="font-size: 14px"&gt;mixed-fisheries considerations of relevance to the management of the fisheries; and&lt;/li&gt;&lt;br&gt;&lt;br&gt;
-&lt;li style="font-size: 14px"&gt;an evaluation of the effects of fishing gear on the ecosystem in terms of the seabed and on the bycatch of
-protected, endangered, and threatened species.&lt;/li&gt;&lt;/ol&gt;&lt;br&gt;
-The scientific names of all species described in this overview are listed in Table A2 in the Annex. &lt;br&gt;&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>landings</t>
-  </si>
-  <si>
-    <t>discards</t>
-  </si>
-  <si>
-    <t>sidebar</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Landings&lt;/b&gt;&lt;br&gt;&lt;br&gt;Fisheries in the Greater North Sea catch a large diversity of species. These have been categorized into species that are pelagic, demersal, benthic (e.g. flatfish), crustaceans, and elasmobranchs. &lt;br&gt;&lt;br&gt;Total landings from the Greater North Sea varied between 2 and 3 million tonnes during the 1950s, then rose to between 3 and 4 million tonnes from the late 1960s to the mid-1990s (Figure 2). High catches of both pelagic species (mackerel and herring) and demersal species (cod and haddock) accounted for the increase in total landings in the late 1960s (figures 3 and 4). 
-The landings shown in Figure 4 only include those species for which ICES gives advice. There are a number of stocks for which ICES does not give advice where landings may be substantial (e.g. Scallop, edible crab, brown shrimp, European lobster, blue mussel). Total landings declined after 1995 to a low of 1.4 million tonnes in 2012. This decline is attributed to overfishing and decreased productivity of important stocks such as cod and herring, but also to the successful reduction of fishing mortality to more sustainable levels after 2000. &lt;br&gt;&lt;br&gt;
-Since 2003, the pelagic fisheries using pelagic trawl and purse seines have accounted for the largest proportion of the total landings, followed by the demersal and benthic fisheries (Figure 3). Overall landings increased slightly from 2011 after a rise in herring landings and again, most recently (in 2015), from increased catches of anchovy, sardine, and hake.&lt;br&gt;&lt;br&gt;
-Recreational fisheries in the North Sea target a wide range of species, but few of these fisheries are monitored or evaluated. Recreational catches of seabass and salmon (including freshwater for the latter) are significant and are included in ICES assessment of these species. In contrast, the recreational fisheries of elasmobranchs is not widely monitored; however, the recreational harvest of these species (mainly dogfish and several species of skates and rays) appears to be negligible.&lt;br&gt;&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Discards&lt;/b&gt;&lt;br&gt;&lt;br&gt;Discard data have been collected for some North Sea fisheries since the mid-1970s. Since 2000, discard data from North Sea commercial fisheries have been collected from various observer programmes implemented under the EU Data Collection Framework (DCF), and UK continued that commitment in retained law from 2020 after leaving the EU. However, complete discard data are only available from 2012 onwards. In 2015–2019, discard rates remained relatively stable. Discard rates of pelagic species were close to zero (Figure 6). Discard estimates for several species of elasmobranch are highly uncertain due to low encounter probabilities and so are not shown.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Bycatch of protected, endangered, and threatened species&lt;/b&gt;&lt;br&gt;&lt;br&gt; All fisheries have the potential to catch protected, endangered, or threatened species, such as seabirds and marine mammals, as non-targeted bycatch. Data submitted to ICES through annual data calls indicated that between 2017–2021 ten ICES Member Countries had fisheries operating in the Greater North Sea ecoregion (ICES, 2022a). During the same period approximately 13 000 monitoring days were undertaken, primarily by at-sea observers, in a variety of static and mobile gears and on vessels ranging from under 8 m to over 40 m. Most bycatch data collection in the ecoregion is carried out within multipurpose programmes under the DCF and through dedicated bycatch monitoring programmes.&lt;br&gt;&lt;br&gt;&lt;b&gt; Bycatch records in 2021&lt;/b&gt;&lt;br&gt;&lt;br&gt; In 2021, 47 marine mammals from at least four species were recorded as bycatch, mostly in net métiers. Forty-two seabirds from at least five species were recorded as bycatch in bottom trawl, longline, purse-seine and net fisheries (Table 1). Over 13 000 specimens of fish of potential conservation interest were recorded from a wide mix of static and mobile gears. Most of the fish records were tub gurnard (Chelidonichthys lucerna) in bottom trawls. No turtles were reported as bycatch.</t>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -573,7 +578,9 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -594,7 +601,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -602,7 +609,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -610,7 +617,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -641,18 +648,18 @@
     </row>
     <row r="2" spans="1:2" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -664,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE2A7A1-C07D-40E0-A9E9-3CF06E261156}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,13 +690,56 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D916A7BB-8321-4345-8DD6-BD18062EF575}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8086C30E-32C2-4F68-82C0-7284FD30F32C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: update texts.xlsx with new data for improved functionality
</commit_message>
<xml_diff>
--- a/data-raw/texts.xlsx
+++ b/data-raw/texts.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilm\Projects\fisheriesXplorer\data-raw\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AE5013-575E-4A22-8763-DC954D95EA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="3645" windowWidth="28800" windowHeight="15030" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="overview" sheetId="1" r:id="rId1"/>
-    <sheet name="landings_discards" sheetId="2" r:id="rId2"/>
-    <sheet name="status" sheetId="4" r:id="rId3"/>
-    <sheet name="mixfish" sheetId="5" r:id="rId4"/>
-    <sheet name="vms" sheetId="6" r:id="rId5"/>
-    <sheet name="bycatch" sheetId="3" r:id="rId6"/>
+    <sheet r:id="rId1" sheetId="1" name="overview_NrS"/>
+    <sheet r:id="rId2" sheetId="2" name="overview_NwS"/>
+    <sheet r:id="rId3" sheetId="3" name="landings_discards"/>
+    <sheet r:id="rId4" sheetId="4" name="status"/>
+    <sheet r:id="rId5" sheetId="5" name="mixfish"/>
+    <sheet r:id="rId6" sheetId="6" name="vms"/>
+    <sheet r:id="rId7" sheetId="7" name="bycatch"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>section</t>
   </si>
@@ -33,22 +28,16 @@
     <t>text</t>
   </si>
   <si>
-    <t>executive_summary</t>
-  </si>
-  <si>
-    <t>introduction</t>
-  </si>
-  <si>
-    <t>who_is_fishing</t>
+    <t>sidebar</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Bycatch of protected, endangered, and threatened species&lt;/b&gt;&lt;br&gt;&lt;br&gt; All fisheries have the potential to catch protected, endangered, or threatened species, such as seabirds and marine mammals, as non-targeted bycatch. Data submitted to ICES through annual data calls indicated that between 2017–2021 ten ICES Member Countries had fisheries operating in the Greater North Sea ecoregion (ICES, 2022a). During the same period approximately 13 000 monitoring days were undertaken, primarily by at-sea observers, in a variety of static and mobile gears and on vessels ranging from under 8 m to over 40 m. Most bycatch data collection in the ecoregion is carried out within multipurpose programmes under the DCF and through dedicated bycatch monitoring programmes.&lt;br&gt;&lt;br&gt;&lt;b&gt; Bycatch records in 2021&lt;/b&gt;&lt;br&gt;&lt;br&gt; In 2021, 47 marine mammals from at least four species were recorded as bycatch, mostly in net métiers. Forty-two seabirds from at least five species were recorded as bycatch in bottom trawl, longline, purse-seine and net fisheries (Table 1). Over 13 000 specimens of fish of potential conservation interest were recorded from a wide mix of static and mobile gears. Most of the fish records were tub gurnard (Chelidonichthys lucerna) in bottom trawls. No turtles were reported as bycatch.</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
   <si>
     <t>landings</t>
-  </si>
-  <si>
-    <t>discards</t>
-  </si>
-  <si>
-    <t>sidebar</t>
   </si>
   <si>
     <t>&lt;b&gt;Landings&lt;/b&gt;&lt;br&gt;&lt;br&gt;Fisheries in the Greater North Sea catch a large diversity of species. These have been categorized into species that are pelagic, demersal, benthic (e.g. flatfish), crustaceans, and elasmobranchs. &lt;br&gt;&lt;br&gt;Total landings from the Greater North Sea varied between 2 and 3 million tonnes during the 1950s, then rose to between 3 and 4 million tonnes from the late 1960s to the mid-1990s (Figure 2). High catches of both pelagic species (mackerel and herring) and demersal species (cod and haddock) accounted for the increase in total landings in the late 1960s (figures 3 and 4). 
@@ -57,10 +46,74 @@
 Recreational fisheries in the North Sea target a wide range of species, but few of these fisheries are monitored or evaluated. Recreational catches of seabass and salmon (including freshwater for the latter) are significant and are included in ICES assessment of these species. In contrast, the recreational fisheries of elasmobranchs is not widely monitored; however, the recreational harvest of these species (mainly dogfish and several species of skates and rays) appears to be negligible.&lt;br&gt;&lt;br&gt;</t>
   </si>
   <si>
+    <t>discards</t>
+  </si>
+  <si>
     <t>&lt;b&gt;Discards&lt;/b&gt;&lt;br&gt;&lt;br&gt;Discard data have been collected for some North Sea fisheries since the mid-1970s. Since 2000, discard data from North Sea commercial fisheries have been collected from various observer programmes implemented under the EU Data Collection Framework (DCF), and UK continued that commitment in retained law from 2020 after leaving the EU. However, complete discard data are only available from 2012 onwards. In 2015–2019, discard rates remained relatively stable. Discard rates of pelagic species were close to zero (Figure 6). Discard estimates for several species of elasmobranch are highly uncertain due to low encounter probabilities and so are not shown.</t>
   </si>
   <si>
-    <t>&lt;b&gt;Bycatch of protected, endangered, and threatened species&lt;/b&gt;&lt;br&gt;&lt;br&gt; All fisheries have the potential to catch protected, endangered, or threatened species, such as seabirds and marine mammals, as non-targeted bycatch. Data submitted to ICES through annual data calls indicated that between 2017–2021 ten ICES Member Countries had fisheries operating in the Greater North Sea ecoregion (ICES, 2022a). During the same period approximately 13 000 monitoring days were undertaken, primarily by at-sea observers, in a variety of static and mobile gears and on vessels ranging from under 8 m to over 40 m. Most bycatch data collection in the ecoregion is carried out within multipurpose programmes under the DCF and through dedicated bycatch monitoring programmes.&lt;br&gt;&lt;br&gt;&lt;b&gt; Bycatch records in 2021&lt;/b&gt;&lt;br&gt;&lt;br&gt; In 2021, 47 marine mammals from at least four species were recorded as bycatch, mostly in net métiers. Forty-two seabirds from at least five species were recorded as bycatch in bottom trawl, longline, purse-seine and net fisheries (Table 1). Over 13 000 specimens of fish of potential conservation interest were recorded from a wide mix of static and mobile gears. Most of the fish records were tub gurnard (Chelidonichthys lucerna) in bottom trawls. No turtles were reported as bycatch.</t>
+    <t>executive_summary</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;The largest landings in this ecoregion are by Norway, the Russian Federation (Russia henceforth), Faroe Islands, and Iceland, mainly by pelagic fisheries. Other nations also have fisheries in the area. The number of fishing vessels is declining while the size of the remaining vessels is increasing. The annual catch in the ecoregion has varied between 700 000 tonnes
+to over 2 million tonnes.&lt;br&gt;&lt;br&gt;
+The pelagic fisheries, using purse-seine and pelagic trawls, account for the largest catches by weight and target Norwegian spring-spawning (NSS) herring (her.27.1-24a514a), blue whiting (whb.27.1-91214), mackerel (mac.27.nea), and other pelagic species. The largest demersal fishery targets cod (cod.27.1-2), haddock (had.27.1-2), and saithe (pok.27.1-2) using bottom trawls, purse-seine, Danish seine and gillnets, and to a lesser extent hook and line gear. Smaller fisheries target other gadoid species, Greenland halibut (ghl.27.1-2), and beaked redfish (reb.27.1-2). Landings of pelagic species within the ecoregion in the last decades have been variable. The demersal fisheries, dominated by cod, display less pronounced fluctuations than the pelagic fisheries. Information about discards is sparse, but the total weight of discards is considered low in both the pelagic and the demersal fisheries. Harp seals and minke whales are hunted in the region.&lt;br&gt;&lt;br&gt;
+Status summaries of Norwegian Sea stocks relative to ICES maximum sustainable yield (MSY) approach and precautionary approach (PA) are known for about 42% of the 19 stocks assessed by ICES in this ecoregion. Only 21% of the stocks are fished below F MSY, accounting for less than 1% of the total catch. 21% of the stocks have a biomass above MSY Btrigger, accounting for 86% of the total catch. Demersal stocks have shown a trend of declining fishing mortality since the mid-1990s, followed by a sharp increase in 2019, largely driven by the exploitation pattern of redfish. In 2021 the average F/F MSY ratio was close to 1. The mean SSB/MSY Btrigger ratio of demersal stocks has been decreasing over the last decade, but mean SSB remains above MSY Btrigger and increased in 2021. The average F/F MSY ratio for pelagic stocks has fluctuated slightly above 1 since 2005. The mean SSB/MSY Btrigger ratio for pelagic species has been well above 1 the last two decades though followed by a recent sharp decline, but remains above 1.&lt;br&gt;&lt;br&gt;
+In addition to biomass removal, ecosystem effects of fisheries include abrasion, ghost fishing, and bycatch of protected, endangered, and threatened species.&lt;br&gt;&lt;br&gt;
+Supporting data used in the Norwegian Sea fisheries overview can be accessed at &lt;a href="https://doi.org/10.17895/ices.advice.27879897"&gt;ICES Library&lt;/a&gt;&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>introduction</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;The Norwegian Sea connects with the Faroes ecoregion to the southwest, the Icelandic Waters ecoregion and Greenland Sea to the west along the edge to the shallower Iceland Sea between the Faroe Islands, and northwards to Jan Mayen. To the south it borders to the shallower North Sea along the 62 ̊N parallel between Norway and the Faroe Islands, and to the northeast the shallower Barents Sea (Figure 1). The Norwegian Sea covers more than 1.1 million km2 , consisting of two deep basins (between 3000 m and 4000 m deep) – the Norwegian Basin and the Lofoten Basin – separated by the Vøring Plateau (between 1000 m and 3000 m deep). The Norwegian Sea is separated from the Greenland Sea to the north by the Mohn Ridge. To the west, the basin slope forms the transition to the somewhat shallower Iceland Sea. The warm North Atlantic Current ensures relatively stable and high water temperatures, so that unlike the Arctic seas, the Norwegian Sea is ice-free throughout the year.&lt;br&gt;&lt;br&gt; 
+Due to the temporary suspension of Russian Federation in ICES activities, ICES did not conduct assessments for the following stocks in 2022: cod.27.1-2, had.27.1-2, and reb.27.1-2. The results of the bilateral Norwegian−Russian
+assessments for these stocks are not included in this overview.&lt;br&gt;&lt;br&gt; 
+This overview provides:&lt;br&gt;&lt;br&gt;
+&lt;ol style="font-size: 14px"&gt;
+&lt;li style="font-size: 14px"&gt;a short description of each of the national commercial fishing fleets in the ecoregion, including their fishing gears, and spatial and temporal patterns of activity;&lt;/li&gt;&lt;br&gt;&lt;br&gt;
+&lt;li style="font-size: 14px"&gt;a summary of the status of the fisheries resources and the level of exploitation relative to agreed objectives and reference points;&lt;/li&gt;&lt;br&gt;&lt;br&gt;
+&lt;li style="font-size: 14px"&gt;a description of mixed fisheries interactions in the ecosystem, and&lt;/li&gt;&lt;br&gt;&lt;br&gt;
+&lt;li style="font-size: 14px"&gt;an evaluation of the effects of fishing gear on the ecosystem in terms of the seabed and on the bycatch of protected, endangered, and threatened species.&lt;/li&gt;&lt;/ol&gt;&lt;br&gt;
+The scientific names of all species described in this overview are listed in Table A2 in the Annex. &lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>who_is_fishing</t>
+  </si>
+  <si>
+    <t>&lt;br&gt;Many nations currently have fisheries targeting the marine stocks within this ecoregion. The largest landings are by Norway, Russia, Faroe Islands, and Iceland. Lesser amounts are landed by United Kingdom and others (Figure 2). Pelagic fishing by multinational fleets is the major activity in the ecoregion. The number of fishing vessels is declining while the size of the vessels is increasing.&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Norway&lt;/b&gt;&lt;br&gt;
+The Norwegian commercial fleet has the majority of its fishing activity in the shelf area, particularly along the coast of
+Norway and along the continental shelf edge. The Norwegian fleet fishing in the ecoregion consists of about 2300 active
+vessels fishing pelagic fish (mackerel and herring), demersal fish (cod, saithe, haddock, ling (lin.27.1-2), tusk (usk.27.1-2),
+Greenland halibut, and redfish), and shellfish (brown crab, king crab, and northern prawn). Small coastal vessels (the
+majority &lt; 15 m length) fishing with beach-seine, gillnets, and pots make up around 87% of the fleet, while the remaining
+are mainly ocean-going trawlers and purse-seiners &gt; 28 m in length. The highest catch volume (82% of the total catch) is
+taken by the bigger vessels, with pelagic fish constituting the largest part of the landings.&lt;br&gt;&lt;br&gt;
+Harp and hooded seals are hunted with between two and five large ice-going vessels. The minke whale hunt has been
+ongoing in all years since 1993, and approximately 10–15 vessels.&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Russia&lt;/b&gt;&lt;br&gt;
+The Russian commercial fleet in the Norwegian Sea ecoregion and adjacent waters is composed of about 30 large vessels
+(62–120 m in length) targeting pelagic species including NSS herring, blue whiting, and mackerel using pelagic trawls. The
+pelagic fleet conducts most of its fishing activities in international waters and fewer in the Norwegian EEZ. About 50 smaller
+vessels (&lt; 60 m) target demersal fish, including cod, haddock, saithe, redfish, Greenland halibut, and Atlantic wolffish, using
+mostly bottom trawls. Pelagic fish contribute most to the Russian fishery (about 90 % of the catches) in this ecoregion.&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Iceland&lt;/b&gt;&lt;br&gt;
+he Icelandic fleet operating in the Norwegian Sea ecoregion is composed of about 19 large vessels (&gt; 60 m length). They
+all target pelagic fish (NSS herring, mackerel, and blue whiting) with pelagic trawls. Two of the vessels freeze the catches
+on board while the others bring the catches ashore in refrigerated seawater (RSW) tanks&lt;br&gt;&lt;br&gt;
+&lt;b&gt;United Kingdom&lt;/b&gt;&lt;br&gt;
+The UK fishery operating in the Norwegian Sea ecoregion fishes mainly in ICES Division 2.a using bottom and midwater
+trawls with the occasional gillnetting and purse-seining. A small number of vessels operate in this area and catch a variety
+of demersal and pelagic species. In 2020, three bottom otter trawlers (40–90 m length) targeted cod, together with small
+amounts of saithe, haddock, redfish, and other species. The four midwater trawlers (75–120 m) fishing in 2020 targeted
+NSS herring, mackerel, and blue whiting.&lt;br&gt;&lt;br&gt;
+&lt;b&gt;Faroe Islands&lt;/b&gt;&lt;br&gt;The Faroese fleet in the ecoregion consists of 12 large (&gt; 55 m length) vessels targeting pelagic species (NSS herring,
+mackerel, and blue whiting) with pelagic trawl (mainly) or purse-seine. One of the vessels freeze the catch on board while
+the rest use RSW tanks to bring the catch ashore. In addition, a handful of smaller trawlers (35–50 m length without RSW
+tanks) deliver the catch (mackerel) to the larger vessels at sea; the number of vessels in this last category has decreased
+much over the last five-to-eight years. In the description of fisheries, some Faroese fisheries are mentioned in Subarea 2,
+but these all take place outside the Norwegian Sea ecoregion.&lt;br&gt;&lt;br&gt;</t>
   </si>
   <si>
     <t>&lt;br&gt;Around 6600 fishing vessels are active in the Greater North Sea. Total landings peaked in the 1970s at 4 million tonnes and have since declined to about 2 million tonnes. Total fishing effort has declined substantially since 2003. Pelagic fish landings are greater than demersal fish landings. Herring and mackerel, caught using pelagic trawls and seines, account for the largest portion of the pelagic landings, while sandeel and haddock, caught using otter trawls/seines, account for the largest fraction of the demersal landings. Catches are taken from more than 100 stocks. Discards are highest in the demersal and benthic fisheries. The spatial distribution of fishing gear varies across the Greater North Sea. Static gear is used most frequently in the English Channel, the eastern part of the Southern Bight, the Danish banks, and in the waters east of Shetland. Bottom trawls are used throughout the North Sea, with lower use in the shallower southern North Sea, where beam trawls are most commonly used. Pelagic gears are used throughout the North Sea. &lt;br&gt;&lt;br&gt;In terms of weight of catch, fish stocks harvested from the North Sea are being fished at levels consistent with achieving good environmental status (GES) under the EU’s Marine Strategy Framework Directive; however, the reproductive capacity of the stocks has not generally reached this level. Almost all the fisheries in the North Sea catch more than one species; controlling fishing on one species therefore affects other species as well. ICES has developed a number of scenarios for fishing opportunities that take account of these technical interactions. Each of these scenarios results in different outcomes for the fish stocks. Managers may need to take these scenarios into account when deciding upon fishing opportunities. Furthermore, biological interactions occur between species (e.g. predation), and fishing on one stock may affect the population dynamics of another. Scenarios that take account of these various interactions can be used to evaluate the possible consequences of policy decisions. The greatest physical disturbances of the seabed caused by fishing activity in the North Sea is caused by mobile bottom-contacting gear in the eastern English Channel, in nearshore areas in the southeastern North Sea and in the central Skagerrak. Incidental bycatches of protected, endangered, and threatened species occur in several North Sea fisheries, and the bycatch of common dolphin in the western English Channel may be unsustainable in terms of population. &lt;br&gt;&lt;br&gt;Supporting data used in the Greater North Sea fisheries overview is accessible at &lt;a href="https://doi.org/10.17895/ices.advice.21641360"&gt;ICES Library&lt;/a&gt;&lt;br&gt;&lt;br&gt;</t>
@@ -214,15 +267,13 @@
 pelagic species are harvested by 18 large vessels, primarily using pelagic trawls.&lt;br&gt;&lt;br&gt;
 The Faroe Islands also fish in the Greater North Sea, but ICES does not have information on this fleet.&lt;br&gt;&lt;br&gt;</t>
   </si>
-  <si>
-    <t>test</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +284,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -264,26 +321,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="9">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -294,10 +366,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -335,71 +407,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -427,7 +499,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -450,11 +522,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -463,13 +535,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -479,7 +551,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -488,7 +560,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -497,7 +569,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -505,10 +577,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -573,52 +645,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" style="8" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="255.57642857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="162" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="120.75" customFormat="1" s="3">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="303" customFormat="1" s="3">
+      <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="1666.5" customFormat="1" s="3">
+      <c r="A4" s="6" t="s">
         <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -627,40 +697,50 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE4E976-B447-4DEF-A85E-11D6D9966CA4}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="255.5703125" customWidth="1"/>
+    <col min="1" max="1" style="8" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="198.29071428571427" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="343.5" customFormat="1" s="3">
+      <c r="A2" s="5" t="s">
         <v>9</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="462" customFormat="1" s="3">
+      <c r="A3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="409.6000000000001" customFormat="1" s="3">
+      <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -669,29 +749,42 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D916A7BB-8321-4345-8DD6-BD18062EF575}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="255.57642857142858" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="210.75" customFormat="1" s="3">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -700,29 +793,34 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8086C30E-32C2-4F68-82C0-7284FD30F32C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -731,29 +829,34 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54640D34-6F2C-4FD7-AC14-D9115ECC0B2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -762,32 +865,70 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE2A7A1-C07D-40E0-A9E9-3CF06E261156}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="159.42578125" customWidth="1"/>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="159.4335714285714" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: implement floating glossary UI and server functionality (still need to clean up and expand to other modules
</commit_message>
<xml_diff>
--- a/data-raw/texts.xlsx
+++ b/data-raw/texts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icesit-my.sharepoint.com/personal/luca_lamoni_ices_dk/Documents/Profile/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_2023\fisheriesXplorer\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="11_3B97B444F62EC743AD03632361AC6BA5D546EF5D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{931718E8-809C-4422-B643-B9648C4752C2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5342848-33A2-4B57-8F54-1C3B1C7DF1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview_NrS" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="overview_CS" sheetId="12" r:id="rId7"/>
     <sheet name="overview_FO" sheetId="13" r:id="rId8"/>
     <sheet name="overview_GS" sheetId="14" r:id="rId9"/>
-    <sheet name="overview_IS" sheetId="15" r:id="rId10"/>
-    <sheet name="overview_ONA" sheetId="16" r:id="rId11"/>
-    <sheet name="landings_discards" sheetId="3" r:id="rId12"/>
-    <sheet name="status" sheetId="4" r:id="rId13"/>
-    <sheet name="mixfish" sheetId="5" r:id="rId14"/>
-    <sheet name="vms" sheetId="6" r:id="rId15"/>
-    <sheet name="bycatch" sheetId="7" r:id="rId16"/>
+    <sheet name="glossary" sheetId="17" r:id="rId10"/>
+    <sheet name="overview_IS" sheetId="15" r:id="rId11"/>
+    <sheet name="overview_ONA" sheetId="16" r:id="rId12"/>
+    <sheet name="landings_discards" sheetId="3" r:id="rId13"/>
+    <sheet name="status" sheetId="4" r:id="rId14"/>
+    <sheet name="mixfish" sheetId="5" r:id="rId15"/>
+    <sheet name="vms" sheetId="6" r:id="rId16"/>
+    <sheet name="bycatch" sheetId="7" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="100">
   <si>
     <t>section</t>
   </si>
@@ -653,12 +654,180 @@
   <si>
     <t>&lt;b&gt;Bycatch of protected, endangered, and threatened species&lt;/b&gt;&lt;br&gt;&lt;br&gt; All fisheries have the potential to catch protected, endangered, or threatened species, such as seabirds and marine mammals, as non-targeted bycatch. Data submitted to ICES through annual data calls indicated that between 2017–2021 ten ICES Member Countries had fisheries operating in the Greater North Sea ecoregion (ICES, 2022a). During the same period approximately 13 000 monitoring days were undertaken, primarily by at-sea observers, in a variety of static and mobile gears and on vessels ranging from under 8 m to over 40 m. Most bycatch data collection in the ecoregion is carried out within multipurpose programmes under the DCF and through dedicated bycatch monitoring programmes.&lt;br&gt;&lt;br&gt;&lt;b&gt; Bycatch records in 2021&lt;/b&gt;&lt;br&gt;&lt;br&gt; In 2021, 47 marine mammals from at least four species were recorded as bycatch, mostly in net métiers. Forty-two seabirds from at least five species were recorded as bycatch in bottom trawl, longline, purse-seine and net fisheries (Table 1). Over 13 000 specimens of fish of potential conservation interest were recorded from a wide mix of static and mobile gears. Most of the fish records were tub gurnard (Chelidonichthys lucerna) in bottom trawls. No turtles were reported as bycatch.</t>
   </si>
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>ICES ecoregion</t>
+  </si>
+  <si>
+    <t>Large marine area used by ICES to organise advice, assessments, and reporting across ecosystem products.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/advice/ESD/Pages/Ecosystem-overviews.aspx</t>
+  </si>
+  <si>
+    <t>Fisheries overview</t>
+  </si>
+  <si>
+    <t>ICES advice product summarising fishing activities, fleets, catches, and pressures for each ecoregion.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/advice/Fisheries-overviews/Pages/Introduction.aspx</t>
+  </si>
+  <si>
+    <t>Catch</t>
+  </si>
+  <si>
+    <t>Total fish removals used in advice (landings plus discards), as framed in ICES guidance on catches and landings.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.17895/ices.advice.8341</t>
+  </si>
+  <si>
+    <t>Landings</t>
+  </si>
+  <si>
+    <t>Portion of the catch retained and brought ashore; distinguished from discards in ICES guidance.</t>
+  </si>
+  <si>
+    <t>Discards</t>
+  </si>
+  <si>
+    <t>Components of a fish stock thrown back after capture (e.g., below minimum size or due to exhausted quota); most are unlikely to survive.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/community/documents/advice/acronyms_and_terminology.pdf</t>
+  </si>
+  <si>
+    <t>Fisheries guilds</t>
+  </si>
+  <si>
+    <t>Broad groupings (e.g., pelagic, demersal, benthic, elasmobranch) used in ecosystem and fisheries overviews to summarise stock groups and trends.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/advice/ESD/Pages/Bay-of-Biscay-and-the-Iberian-Coast_Landing.aspx</t>
+  </si>
+  <si>
+    <t>Maximum Sustainable Yield (MSY)</t>
+  </si>
+  <si>
+    <t>Largest average catch that can be continuously taken from a stock under existing environmental conditions.</t>
+  </si>
+  <si>
+    <t>FMSY</t>
+  </si>
+  <si>
+    <t>Fishing mortality consistent with achieving MSY.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/Lists/Glossary/ICES%20Glossary.aspx?PageFirstRow=361&amp;Paged=TRUE&amp;View=%7BE4199C10-9657-46B2-BF8B-E7DE42FF06A6%7D&amp;p_Acronyms0=FEAP&amp;p_ID=421</t>
+  </si>
+  <si>
+    <t>MSY Btrigger</t>
+  </si>
+  <si>
+    <t>Spawning-stock biomass reference point that triggers a more cautious response within the ICES MSY approach.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/Lists/Glossary/ICES%20Glossary.aspx?PageFirstRow=691&amp;Paged=TRUE&amp;View=%7BE4199C10-9657-46B2-BF8B-E7DE42FF06A6%7D&amp;p_Acronyms0=MSY&amp;p_ID=386</t>
+  </si>
+  <si>
+    <t>Blim / Bpa</t>
+  </si>
+  <si>
+    <t>Blim: limit SSB below which recruitment is impaired; Bpa: precautionary SSB set to keep SSB above Blim with high probability.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/Lists/Glossary/ICES%20Glossary.aspx?PageFirstRow=151&amp;Paged=TRUE&amp;PagedPrev=TRUE&amp;View=%7BE4199C10-9657-46B2-BF8B-E7DE42FF06A6%7D&amp;p_Acronyms0=CEFAS&amp;p_ID=451</t>
+  </si>
+  <si>
+    <t>Mixed fisheries</t>
+  </si>
+  <si>
+    <t>Fisheries where several stocks are caught together; advice and scenarios consider trade-offs across fleets and species.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/advice/Pages/technical_guidelines.aspx</t>
+  </si>
+  <si>
+    <t>Technical interactions</t>
+  </si>
+  <si>
+    <t>Consequences of species being caught together due to the non-selective nature of many gears; catches in one stock constrain catches in others.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/community/Documents/Advice/General_context_of_ICES_advice_2012.pdf</t>
+  </si>
+  <si>
+    <t>Métier / fleet grouping</t>
+  </si>
+  <si>
+    <t>Métier: homogeneous subdivision of a fishery by gear/area/mesh/target; used with fishery and fleet to describe activity categories.</t>
+  </si>
+  <si>
+    <t>Vessel Monitoring System (VMS)</t>
+  </si>
+  <si>
+    <t>Satellite-based system providing fishing vessel positions (speed and course) to support monitoring, control, surveillance and scientific analyses.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/about-ICES/projects/EU-RFP/EU%20Repository/PROTECT/FP6%20PROTECT%20Final%20Report%20Project%20Synthesis.pdf</t>
+  </si>
+  <si>
+    <t>Swept Area Ratio (SAR)</t>
+  </si>
+  <si>
+    <t>Ratio of seabed area swept by bottom-contacting gear to the area of a grid cell (a measure of fishing intensity from VMS-based analyses).</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/sites/pub/Publication%20Reports/Expert%20Group%20Report/SSGSUE/2014/01%20WGSFD%20-%20Report%20of%20the%20Working%20Group%20on%20Spatial%20Fisheries%20Data.pdf</t>
+  </si>
+  <si>
+    <t>Logbook</t>
+  </si>
+  <si>
+    <t>Official record of a vessel’s fishing operations (trip, gear, effort, catches); in ICES workflows commonly exchanged in EFLALO format.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/sites/pub/CM%20Doccuments/CM-2010/SSGSUE/sgvms10.pdf</t>
+  </si>
+  <si>
+    <t>Bycatch</t>
+  </si>
+  <si>
+    <t>Incidental capture of non-target species or sizes during fishing; addressed through ICES bycatch guidelines and advice.</t>
+  </si>
+  <si>
+    <t>ETP species</t>
+  </si>
+  <si>
+    <t>Endangered, Threatened, and Protected species considered in ICES bycatch work and advice.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/advice/pages/latest-advice.aspx</t>
+  </si>
+  <si>
+    <t>WGBYC</t>
+  </si>
+  <si>
+    <t>ICES Working Group on Bycatch of Protected Species; collates and assesses bycatch data and supports ICES advice.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/community/groups/Pages/WGbyc.aspx</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -700,6 +869,20 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -731,11 +914,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -756,10 +944,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{D9F166C1-85FC-4494-BE8A-7B590342AC69}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{5EAEE845-076B-4CD4-90B1-733697066B05}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1068,13 +1260,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1082,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1090,7 +1282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="303" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="303" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1098,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1112,6 +1304,267 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5EC4FE-E411-4E36-B8C3-47DB4028DB0F}">
+  <dimension ref="O1:Q20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X20" sqref="X20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="15" max="15" width="29.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37.81640625" customWidth="1"/>
+    <col min="17" max="17" width="9.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O7" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O8" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q8" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q9" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q10" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O11" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q11" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O12" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q12" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O13" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q13" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O14" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q14" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O15" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q15" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O16" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q16" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O17" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="P17" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q17" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O18" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q18" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O19" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="P19" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q19" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="15:17" x14ac:dyDescent="0.35">
+      <c r="O20" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="P20" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q20" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Q2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="Q3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="Q4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="Q5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="Q6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="Q7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="Q8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="Q9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="Q10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="Q11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="Q12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="Q13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="Q14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="Q15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="Q16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="Q17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="Q18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="Q19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="Q20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A026B00C-E4B3-4E36-BEA1-AD93DF3D486F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1119,12 +1572,12 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="135.5546875" customWidth="1"/>
+    <col min="2" max="2" width="135.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1140,7 +1593,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="348" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1148,7 +1601,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1161,7 +1614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{744F2D0C-79DF-4FE3-924E-E680015F9291}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1169,13 +1622,13 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
-    <col min="2" max="2" width="229.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="229.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1183,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1191,7 +1644,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1199,7 +1652,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1212,7 +1665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1221,13 +1674,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1235,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1243,7 +1696,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -1256,7 +1709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1265,12 +1718,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1278,7 +1731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1291,7 +1744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1300,12 +1753,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1313,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1326,7 +1779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1335,12 +1788,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1348,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1361,7 +1814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1370,13 +1823,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="159.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="159.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1408,13 +1861,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="198.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="198.36328125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1422,7 +1875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="343.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="343.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1430,7 +1883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1438,7 +1891,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1459,13 +1912,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
-    <col min="2" max="2" width="152.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="2" max="2" width="152.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1473,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="258.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="258.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1481,7 +1934,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1489,7 +1942,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1510,13 +1963,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" customWidth="1"/>
-    <col min="2" max="2" width="253.88671875" customWidth="1"/>
+    <col min="1" max="1" width="32.90625" customWidth="1"/>
+    <col min="2" max="2" width="253.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1524,7 +1977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="279" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="279" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1532,7 +1985,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1540,7 +1993,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1557,17 +2010,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D16401-415E-4611-9BEF-C11909718B5A}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.21875" customWidth="1"/>
-    <col min="2" max="2" width="223.88671875" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="223.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1575,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1583,7 +2036,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1591,7 +2044,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1612,12 +2065,12 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="181.44140625" customWidth="1"/>
+    <col min="2" max="2" width="181.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1625,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1633,7 +2086,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1641,7 +2094,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1662,13 +2115,13 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="149.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="149.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1676,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="216" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1684,7 +2137,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1692,7 +2145,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1713,13 +2166,13 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" customWidth="1"/>
-    <col min="2" max="2" width="137.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.453125" customWidth="1"/>
+    <col min="2" max="2" width="137.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1727,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="280.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="288" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1735,7 +2188,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="390" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="400" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1743,7 +2196,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="390" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="400" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1751,13 +2204,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.4">
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="7"/>
     </row>
   </sheetData>
@@ -1773,13 +2226,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="114.88671875" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" customWidth="1"/>
+    <col min="2" max="2" width="114.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1787,7 +2240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1795,7 +2248,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="360" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1803,7 +2256,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
chore: update documentation and clean up code structure in helper functions
</commit_message>
<xml_diff>
--- a/data-raw/texts.xlsx
+++ b/data-raw/texts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_2023\fisheriesXplorer\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5342848-33A2-4B57-8F54-1C3B1C7DF1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA926C9D-1088-41FB-A0FD-EFBBBCAE6AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview_NrS" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
   <si>
     <t>section</t>
   </si>
@@ -727,27 +727,15 @@
     <t>Fishing mortality consistent with achieving MSY.</t>
   </si>
   <si>
-    <t>https://www.ices.dk/Lists/Glossary/ICES%20Glossary.aspx?PageFirstRow=361&amp;Paged=TRUE&amp;View=%7BE4199C10-9657-46B2-BF8B-E7DE42FF06A6%7D&amp;p_Acronyms0=FEAP&amp;p_ID=421</t>
-  </si>
-  <si>
     <t>MSY Btrigger</t>
   </si>
   <si>
     <t>Spawning-stock biomass reference point that triggers a more cautious response within the ICES MSY approach.</t>
   </si>
   <si>
-    <t>https://www.ices.dk/Lists/Glossary/ICES%20Glossary.aspx?PageFirstRow=691&amp;Paged=TRUE&amp;View=%7BE4199C10-9657-46B2-BF8B-E7DE42FF06A6%7D&amp;p_Acronyms0=MSY&amp;p_ID=386</t>
-  </si>
-  <si>
     <t>Blim / Bpa</t>
   </si>
   <si>
-    <t>Blim: limit SSB below which recruitment is impaired; Bpa: precautionary SSB set to keep SSB above Blim with high probability.</t>
-  </si>
-  <si>
-    <t>https://www.ices.dk/Lists/Glossary/ICES%20Glossary.aspx?PageFirstRow=151&amp;Paged=TRUE&amp;PagedPrev=TRUE&amp;View=%7BE4199C10-9657-46B2-BF8B-E7DE42FF06A6%7D&amp;p_Acronyms0=CEFAS&amp;p_ID=451</t>
-  </si>
-  <si>
     <t>Mixed fisheries</t>
   </si>
   <si>
@@ -821,6 +809,18 @@
   </si>
   <si>
     <t>https://www.ices.dk/community/groups/Pages/WGbyc.aspx</t>
+  </si>
+  <si>
+    <t>Blim: limit reference point for spawning stock biomass (SSB); Bpa: precautionary reference point for spawning stock biomass (SSB).</t>
+  </si>
+  <si>
+    <t>Sustainable</t>
+  </si>
+  <si>
+    <t>Can be sustained; in the light of the ICES interpretation of precautionary approach: fisheries management that keeps stock(s) above Bpa and fishing mortality below Fpa</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/lists/glossary/ices%20glossary.aspx</t>
   </si>
 </sst>
 </file>
@@ -1260,13 +1260,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="303" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="303" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1305,20 +1305,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5EC4FE-E411-4E36-B8C3-47DB4028DB0F}">
-  <dimension ref="O1:Q20"/>
+  <dimension ref="O1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="29.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="37.81640625" customWidth="1"/>
-    <col min="17" max="17" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="140" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="15:17" x14ac:dyDescent="0.3">
       <c r="O1" t="s">
         <v>44</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="15:17" x14ac:dyDescent="0.3">
       <c r="O2" s="10" t="s">
         <v>47</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="15:17" x14ac:dyDescent="0.3">
       <c r="O3" s="10" t="s">
         <v>50</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="15:17" x14ac:dyDescent="0.3">
       <c r="O4" s="10" t="s">
         <v>53</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="15:17" x14ac:dyDescent="0.3">
       <c r="O5" s="10" t="s">
         <v>56</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="15:17" x14ac:dyDescent="0.3">
       <c r="O6" s="10" t="s">
         <v>58</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="15:17" x14ac:dyDescent="0.3">
       <c r="O7" s="10" t="s">
         <v>61</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="15:17" x14ac:dyDescent="0.3">
       <c r="O8" s="10" t="s">
         <v>64</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="15:17" x14ac:dyDescent="0.3">
       <c r="O9" s="10" t="s">
         <v>66</v>
       </c>
@@ -1414,127 +1414,138 @@
         <v>67</v>
       </c>
       <c r="Q9" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O10" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="10" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O10" s="10" t="s">
+      <c r="P10" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="Q10" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O11" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="Q10" s="11" t="s">
+      <c r="P11" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q11" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O12" s="10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="11" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O11" s="10" t="s">
+      <c r="P12" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="P11" s="10" t="s">
+      <c r="Q12" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="Q11" s="11" t="s">
+    </row>
+    <row r="13" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O13" s="10" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="12" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O12" s="10" t="s">
+      <c r="P13" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="P12" s="10" t="s">
+      <c r="Q13" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="Q12" s="11" t="s">
+    </row>
+    <row r="14" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O14" s="10" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="13" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O13" s="10" t="s">
+      <c r="P14" s="10" t="s">
         <v>78</v>
-      </c>
-      <c r="P13" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q13" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O14" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="P14" s="10" t="s">
-        <v>82</v>
       </c>
       <c r="Q14" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="15:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="15:17" x14ac:dyDescent="0.3">
       <c r="O15" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q15" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O16" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="P16" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="P15" s="10" t="s">
+      <c r="Q16" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="Q15" s="11" t="s">
+    </row>
+    <row r="17" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O17" s="10" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="16" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O16" s="10" t="s">
+      <c r="P17" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="P16" s="10" t="s">
+      <c r="Q17" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="Q16" s="11" t="s">
+    </row>
+    <row r="18" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O18" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="17" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O17" s="10" t="s">
+      <c r="P18" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="P17" s="10" t="s">
+      <c r="Q18" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O19" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="Q17" s="11" t="s">
+      <c r="P19" s="10" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O18" s="10" t="s">
+      <c r="Q19" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="P18" s="10" t="s">
+    </row>
+    <row r="20" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O20" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="Q18" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O19" s="10" t="s">
+      <c r="P20" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="P19" s="10" t="s">
+      <c r="Q20" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="Q19" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="15:17" x14ac:dyDescent="0.35">
-      <c r="O20" s="10" t="s">
+    </row>
+    <row r="21" spans="15:17" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
         <v>97</v>
       </c>
-      <c r="P20" s="10" t="s">
+      <c r="P21" t="s">
         <v>98</v>
       </c>
-      <c r="Q20" s="11" t="s">
+      <c r="Q21" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1547,18 +1558,15 @@
     <hyperlink ref="Q6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="Q7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="Q8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="Q9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="Q10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="Q11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="Q12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="Q13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="Q14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="Q15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="Q16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="Q17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="Q18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="Q19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="Q20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="Q12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="Q13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="Q14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="Q15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="Q16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="Q17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="Q18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="Q19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="Q20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1572,12 +1580,12 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="135.54296875" customWidth="1"/>
+    <col min="2" max="2" width="135.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1585,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1593,7 +1601,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="348" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1601,7 +1609,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1622,13 +1630,13 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="229.6328125" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="229.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1636,7 +1644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1644,7 +1652,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1652,7 +1660,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1674,13 +1682,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1688,7 +1696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1696,7 +1704,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -1718,12 +1726,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1731,7 +1739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1753,12 +1761,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1766,7 +1774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1788,12 +1796,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1801,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1823,13 +1831,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="159.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="159.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1837,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1861,13 +1869,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="198.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="198.33203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1875,7 +1883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="343.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="343.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1883,7 +1891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1891,7 +1899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1912,13 +1920,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="2" max="2" width="152.36328125" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="152.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1926,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="258.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="258.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1934,7 +1942,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1942,7 +1950,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1963,13 +1971,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.90625" customWidth="1"/>
-    <col min="2" max="2" width="253.90625" customWidth="1"/>
+    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+    <col min="2" max="2" width="253.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1977,7 +1985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="279" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="279" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1985,7 +1993,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1993,7 +2001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2014,13 +2022,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
-    <col min="2" max="2" width="223.90625" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
+    <col min="2" max="2" width="223.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2028,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2036,7 +2044,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2044,7 +2052,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2065,12 +2073,12 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="181.453125" customWidth="1"/>
+    <col min="2" max="2" width="181.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2078,7 +2086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2086,7 +2094,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2094,7 +2102,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2115,13 +2123,13 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" customWidth="1"/>
-    <col min="2" max="2" width="149.08984375" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="149.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2129,7 +2137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2137,7 +2145,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2145,7 +2153,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2166,13 +2174,13 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.453125" customWidth="1"/>
-    <col min="2" max="2" width="137.36328125" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
+    <col min="2" max="2" width="137.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2180,7 +2188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="288" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" ht="280.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2188,7 +2196,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="400" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" ht="390" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2196,7 +2204,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="400" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" ht="390" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2204,13 +2212,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
     </row>
   </sheetData>
@@ -2226,13 +2234,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.54296875" customWidth="1"/>
-    <col min="2" max="2" width="114.90625" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="114.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2240,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2248,7 +2256,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="360" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2256,7 +2264,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Revert "chore: update documentation and clean up code structure in helper functions"
</commit_message>
<xml_diff>
--- a/data-raw/texts.xlsx
+++ b/data-raw/texts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_2023\fisheriesXplorer\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA926C9D-1088-41FB-A0FD-EFBBBCAE6AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5342848-33A2-4B57-8F54-1C3B1C7DF1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview_NrS" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="100">
   <si>
     <t>section</t>
   </si>
@@ -727,15 +727,27 @@
     <t>Fishing mortality consistent with achieving MSY.</t>
   </si>
   <si>
+    <t>https://www.ices.dk/Lists/Glossary/ICES%20Glossary.aspx?PageFirstRow=361&amp;Paged=TRUE&amp;View=%7BE4199C10-9657-46B2-BF8B-E7DE42FF06A6%7D&amp;p_Acronyms0=FEAP&amp;p_ID=421</t>
+  </si>
+  <si>
     <t>MSY Btrigger</t>
   </si>
   <si>
     <t>Spawning-stock biomass reference point that triggers a more cautious response within the ICES MSY approach.</t>
   </si>
   <si>
+    <t>https://www.ices.dk/Lists/Glossary/ICES%20Glossary.aspx?PageFirstRow=691&amp;Paged=TRUE&amp;View=%7BE4199C10-9657-46B2-BF8B-E7DE42FF06A6%7D&amp;p_Acronyms0=MSY&amp;p_ID=386</t>
+  </si>
+  <si>
     <t>Blim / Bpa</t>
   </si>
   <si>
+    <t>Blim: limit SSB below which recruitment is impaired; Bpa: precautionary SSB set to keep SSB above Blim with high probability.</t>
+  </si>
+  <si>
+    <t>https://www.ices.dk/Lists/Glossary/ICES%20Glossary.aspx?PageFirstRow=151&amp;Paged=TRUE&amp;PagedPrev=TRUE&amp;View=%7BE4199C10-9657-46B2-BF8B-E7DE42FF06A6%7D&amp;p_Acronyms0=CEFAS&amp;p_ID=451</t>
+  </si>
+  <si>
     <t>Mixed fisheries</t>
   </si>
   <si>
@@ -809,18 +821,6 @@
   </si>
   <si>
     <t>https://www.ices.dk/community/groups/Pages/WGbyc.aspx</t>
-  </si>
-  <si>
-    <t>Blim: limit reference point for spawning stock biomass (SSB); Bpa: precautionary reference point for spawning stock biomass (SSB).</t>
-  </si>
-  <si>
-    <t>Sustainable</t>
-  </si>
-  <si>
-    <t>Can be sustained; in the light of the ICES interpretation of precautionary approach: fisheries management that keeps stock(s) above Bpa and fishing mortality below Fpa</t>
-  </si>
-  <si>
-    <t>https://www.ices.dk/lists/glossary/ices%20glossary.aspx</t>
   </si>
 </sst>
 </file>
@@ -1260,13 +1260,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="303" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="303" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1305,20 +1305,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5EC4FE-E411-4E36-B8C3-47DB4028DB0F}">
-  <dimension ref="O1:Q21"/>
+  <dimension ref="O1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="15" max="15" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="140" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37.81640625" customWidth="1"/>
+    <col min="17" max="17" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="15:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O1" t="s">
         <v>44</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="15:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O2" s="10" t="s">
         <v>47</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="15:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O3" s="10" t="s">
         <v>50</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="15:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O4" s="10" t="s">
         <v>53</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="15:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O5" s="10" t="s">
         <v>56</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="15:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O6" s="10" t="s">
         <v>58</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="15:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O7" s="10" t="s">
         <v>61</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="15:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O8" s="10" t="s">
         <v>64</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="15:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O9" s="10" t="s">
         <v>66</v>
       </c>
@@ -1414,138 +1414,127 @@
         <v>67</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="15:17" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O10" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="15:17" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O11" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P11" s="10" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="15:17" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O12" s="10" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="Q12" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="15:17" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O13" s="10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="P13" s="10" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="Q13" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="15:17" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O14" s="10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="Q14" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="15:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O15" s="10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="P15" s="10" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Q15" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="15:17" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O16" s="10" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="Q16" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="15:17" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O17" s="10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="P17" s="10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="Q17" s="11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="15:17" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O18" s="10" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="Q18" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="15:17" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O19" s="10" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="P19" s="10" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="Q19" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="15:17" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="15:17" x14ac:dyDescent="0.35">
       <c r="O20" s="10" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="Q20" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="15:17" x14ac:dyDescent="0.3">
-      <c r="O21" t="s">
-        <v>97</v>
-      </c>
-      <c r="P21" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q21" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1558,15 +1547,18 @@
     <hyperlink ref="Q6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="Q7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="Q8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="Q12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="Q13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="Q14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="Q15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="Q16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="Q17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="Q18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="Q19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="Q20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="Q9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="Q10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="Q11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="Q12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="Q13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="Q14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="Q15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="Q16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="Q17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="Q18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="Q19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="Q20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1580,12 +1572,12 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="135.5546875" customWidth="1"/>
+    <col min="2" max="2" width="135.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1593,7 +1585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1601,7 +1593,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="348" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1609,7 +1601,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1630,13 +1622,13 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
-    <col min="2" max="2" width="229.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="229.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1644,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1652,7 +1644,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1660,7 +1652,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1682,13 +1674,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1696,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1704,7 +1696,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -1726,12 +1718,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1739,7 +1731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1761,12 +1753,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1774,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1796,12 +1788,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1809,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1831,13 +1823,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="159.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="159.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1845,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1869,13 +1861,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="198.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="198.36328125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1883,7 +1875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="343.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="343.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1891,7 +1883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1899,7 +1891,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1920,13 +1912,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
-    <col min="2" max="2" width="152.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="2" max="2" width="152.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1934,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="258.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="258.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1942,7 +1934,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1950,7 +1942,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1971,13 +1963,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" customWidth="1"/>
-    <col min="2" max="2" width="253.88671875" customWidth="1"/>
+    <col min="1" max="1" width="32.90625" customWidth="1"/>
+    <col min="2" max="2" width="253.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1985,7 +1977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="279" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="279" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1993,7 +1985,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2001,7 +1993,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2022,13 +2014,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.21875" customWidth="1"/>
-    <col min="2" max="2" width="223.88671875" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="223.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2036,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2044,7 +2036,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2052,7 +2044,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2073,12 +2065,12 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="181.44140625" customWidth="1"/>
+    <col min="2" max="2" width="181.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2086,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2094,7 +2086,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2102,7 +2094,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2123,13 +2115,13 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="149.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="149.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2137,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="216" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2145,7 +2137,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2153,7 +2145,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2174,13 +2166,13 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" customWidth="1"/>
-    <col min="2" max="2" width="137.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.453125" customWidth="1"/>
+    <col min="2" max="2" width="137.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2188,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="280.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="288" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2196,7 +2188,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="390" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="400" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2204,7 +2196,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="390" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="400" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2212,13 +2204,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.4">
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="7"/>
     </row>
   </sheetData>
@@ -2234,13 +2226,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="114.88671875" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" customWidth="1"/>
+    <col min="2" max="2" width="114.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2248,7 +2240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2256,7 +2248,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="360" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2264,7 +2256,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
feat: update glossary and overview UI components; modify glossary term sorting and adjust tab panel label
</commit_message>
<xml_diff>
--- a/data-raw/texts.xlsx
+++ b/data-raw/texts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_2023\fisheriesXplorer\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3B536C-51C3-4EAD-A704-1379031F30C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272E1236-BB0B-465C-BE1E-C43353D135CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview_NrS" sheetId="1" r:id="rId1"/>
@@ -3450,7 +3450,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3474,9 +3474,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3838,8 +3835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5EC4FE-E411-4E36-B8C3-47DB4028DB0F}">
   <dimension ref="A1:C292"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3864,24 +3861,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -3897,24 +3894,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -3930,13 +3927,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -3952,46 +3949,46 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -4007,57 +4004,57 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -7064,6 +7061,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C20">
+    <sortCondition ref="A2:A20"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="C37" r:id="rId1" xr:uid="{22C4024E-F5EE-4C14-B35D-9A99EB6AF0F4}"/>
   </hyperlinks>
@@ -7097,7 +7097,7 @@
       <c r="A2" s="2" t="s">
         <v>912</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="1" t="s">
         <v>917</v>
       </c>
     </row>
@@ -7266,7 +7266,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -7632,7 +7632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>912</v>
       </c>
@@ -7798,11 +7798,11 @@
       <c r="A2" s="2" t="s">
         <v>912</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="1" t="s">
         <v>916</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="348" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
refactor: update sidebar text rendering for landings and discards in UI module
</commit_message>
<xml_diff>
--- a/data-raw/texts.xlsx
+++ b/data-raw/texts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_2023\fisheriesXplorer\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701AB6A6-9436-44E1-9E26-3214948285F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEAFFCB-83A8-4DBE-AC33-4A364A541CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28932" yWindow="768" windowWidth="59172" windowHeight="12072" tabRatio="826" firstSheet="10" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="826" firstSheet="18" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="glossary" sheetId="17" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="929">
   <si>
     <t>section</t>
   </si>
@@ -4383,7 +4383,104 @@
 &lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Main patterns and Trends: &lt;/p&gt;
+    <t>trends</t>
+  </si>
+  <si>
+    <t>cld</t>
+  </si>
+  <si>
+    <t>annex</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;MSY &amp; Precautionary Approach&lt;/h4&gt;
+&lt;p&gt;
+Summary of fishing mortality and stock size status relative to ICES maximum sustainable yield (MSY) approach and 
+precautionary approach (PA).
+&lt;/p&gt;
+&lt;p&gt;For the MSY: green represents stocks that are fished at or below F&lt;sub&gt;MSY&lt;/sub&gt; and whose sizes are equal to or greater than MSY B&lt;sub&gt;trigger&lt;/sub&gt;; 
+red represents stocks that are fished above F MSY or whose sizes are lower than MSY B&lt;sub&gt;trigger&lt;/sub&gt;.&lt;/p&gt;
+&lt;p&gt;For the PA: green represents stocks that are fished ator below F&lt;sub&gt;pa&lt;/sub&gt; and whose sizes are equal to or greater than B&lt;sub&gt;pa&lt;/sub&gt;; 
+orange represents stocks that are fished between F&lt;sub&gt;pa&lt;/sub&gt; and F&lt;sub&gt;lim&lt;/sub&gt; or whose sizes are between B&lt;sub&gt;lim&lt;/sub&gt; and B&lt;sub&gt;pa&lt;/sub&gt;; 
+red represents stocks that are fished above F&lt;sub&gt;lim&lt;/sub&gt; or whose sizes are lower than B&lt;sub&gt;lim&lt;/sub&gt;.&lt;/p&gt;
+&lt;p&gt;
+Grey represents stocks with unknown reference points.
+&lt;/p&gt;
+&lt;h4&gt;Catches in relation to MSY status&lt;/h4&gt;
+&lt;p&gt;
+Status summary of catches from stocks in the ecoregion relative to their latest stock assessment; the total
+catch of the stocks including catches taken outside the ecoregion.&lt;/p&gt;
+&lt;p&gt;Green represents the proportion of catch fished below F&lt;sub&gt;MSY&lt;/sub&gt; or whose stock size is greater than MSY B&lt;sub&gt;trigger&lt;/sub&gt;. 
+Red represents the proportion of catch fished above F&lt;sub&gt;MSY&lt;/sub&gt; or whose stock size is lower than MSY B&lt;sub&gt;trigger&lt;/sub&gt;. 
+Grey represents the proportion of catch lacking MSY reference points.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;MSY &amp; Precautionary Approach&lt;/h4&gt;
+&lt;p&gt;
+Summary of fishing mortality and stock size status relative to ICES maximum sustainable yield (MSY) approach and 
+precautionary approach (PA).
+&lt;/p&gt;
+&lt;p&gt;For the MSY: green represents stocks that are fished at or below F&lt;sub&gt;MSY&lt;/sub&gt; and whose sizes are equal to or greater than MSY B&lt;sub&gt;trigger&lt;/sub&gt;; 
+red represents stocks that are fished above F MSY or whose sizes are lower than MSY B&lt;sub&gt;trigger&lt;/sub&gt;.&lt;/p&gt;
+&lt;p&gt;For the PA: green represents stocks that are fished ator below F&lt;sub&gt;pa&lt;/sub&gt; and whose sizes are equal to or greater than B&lt;sub&gt;pa&lt;/sub&gt;; 
+orange represents stocks that are fished between F&lt;sub&gt;pa&lt;/sub&gt; and F&lt;sub&gt;lim&lt;/sub&gt; or whose sizes are between B&lt;sub&gt;lim&lt;/sub&gt; and B&lt;sub&gt;pa&lt;/sub&gt;; 
+red represents stocks that are fished above F&lt;sub&gt;lim&lt;/sub&gt; or whose sizes are lower than B&lt;sub&gt;lim&lt;/sub&gt;.&lt;/p&gt;
+&lt;p&gt;
+Grey represents stocks with unknown reference points.
+&lt;/p&gt;
+&lt;h4&gt;Catches in relation to MSY status&lt;/h4&gt;
+&lt;p&gt;
+Status summary of catches from stocks in the ecoregion relative to their latest stock assessment; the total
+catch of the stocks including catches taken outside the ecoregion.&lt;/p&gt;
+&lt;p&gt;Green represents the proportion of catch fished below F&lt;sub&gt;MSY&lt;/sub&gt; or whose stock size is greater than MSY B&lt;sub&gt;trigger&lt;/sub&gt;. 
+Red represents the proportion of catch fished above F&lt;sub&gt;MSY&lt;/sub&gt; or whose stock size is lower than MSY B&lt;sub&gt;trigger&lt;/sub&gt;. 
+Grey represents the proportion of catch lacking MSY reference points.&lt;/p&gt;
+&lt;h4&gt;Results description&lt;/h4&gt;
+&lt;p&gt;ICES currently provides advice for 112 stocks in the ecoregion. Of these, 9 (8%) benthic, 7 (6.2 %) pelagic, 10 (8.9 %) shellfish (Nephrops), 1 (0.8%) elasmobranch, and 17 (15.2%) demersal stocks have an ICES category 1 quantitative stock assessments. Demersal stocks include the three substocks of cod.27.46a7d20 (Northwestern, Viking, and Southern). Stock status is evaluated in terms of fishing mortality (F) and spawning-stock biomass (SSB) levels relative to the maximum sustainable yield (MSY) (F &lt; FMSY and SSB &gt; MSY Btrigger) and precautionary approach (PA) reference points (F &lt; FPA and SSB &gt; BPA).&lt;/p&gt;
+&lt;p&gt;In 2024, 39 (34.8%) of the assessed stocks are fished at or below FMSY levels, and 41 (36.6%) have a stock size equal to or above MSY Btrigger. These stocks account for 66.5% of total landings over the assessment area, which extends beyond the ecoregion. 24 (21.4%) of the assessed stocks are currently fished above FMSY and account for 90% of total landings over the assessment area.&lt;/p&gt;
+&lt;p&gt;Assessed stocks with unknown status relative to MSY and BPA represent 43% and 68%, respectively, of the stocks in the ecoregion. Stocks with unknown status relative to MSY account for 1.5% of total landings (although the assessment area for some stocks extends beyond the ecoregion)&lt;/p&gt;
+&lt;p&gt;Of the ten stocks that currently contribute most of the catch and landings in the ecoregion, haddock (had.27.46a20), boarfish (boc.27.6-8), hake (hke.27.3a46-abd), and anglerfish (mon.27.78abd) have a stock status above MSY Btrigger and fishing pressure below the FMSY, while mackerel (mac.27.nea), herring (her.27.nirs), cod (cod.27.7e-k), cod (cod.27.46a7d20 (all 3 sub-stocks)) and whiting (whg.27.7a) and (whg.27.7b-ce-k) are below MSY Btrigger and are currently fished above FMSY.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Status trends plots&lt;/h4&gt;
+&lt;p&gt;
+Temporal trends in F/F&lt;sub&gt;MSY&lt;/sub&gt; and SSB/MSY B&lt;sub&gt;trigger&lt;/sub&gt; for all available stocks. Stocks with proxy reference points are indicated with dotted lines.
+&lt;/p&gt;
+&lt;h4&gt;Results description&lt;/h4&gt;
+&lt;p&gt;On average, the spawning-stock size in all guilds (mean SSB/MSYBtrigger ratio) is currently above one, although it ranges from 3.2 to 1.3 among stocks. Fishing pressure for the elasmobranch, benthic, shellfish and pelagic guilds on average is currently below FMSY (range from 0.5 to 0.89 among stocks), while demersal species are fished above FMSY (mean F/FMSY ratio of 1.3).&lt;/p&gt;
+&lt;p&gt;For the elasmobranch guild, the mean F/FMSY ratio has declined since the 1990s and is currently below one. The mean SSB/MSY Btrigger ratio has increased since the 1980s and is currently above one.&lt;/p&gt;
+&lt;p&gt;For the benthic guild, the mean F/FMSY ratio has declined since the mid-1990s and is currently below one. The mean SSB/MSY Btrigger ratio has gradually increased since 2000 and is currently above one.&lt;/p&gt;
+&lt;p&gt;For the shellfish guild, the mean F/FMSY ratio shows strong fluctuations about a gradual decline from the mid-2000s and is currently below one. The mean SSB/MSY Btrigger ratio has remained above one and fairly stable throughout the time-series and is currently above one.&lt;/p&gt;
+&lt;p&gt;For the demersal guild, the mean F/FMSY ratio has declined since the 1990s and is currently above one. The mean SSB/MSY Btrigger ratio shows a small, gradual increase since 2000 and is currently above one.&lt;/p&gt;
+&lt;p&gt;For the pelagic guild, the mean F/FMSY ratio has fluctuated (mostly above one) since the 1990s and is currently below one. The mean SSB/MSY Btrigger ratio has remained fairly stable above one since the mid-1990s and is currently above one.&lt;/p&gt;
+&lt;p&gt;Not all species with catch advice are assessed against any PA or MSY reference points because these points are undefined; this includes European eel, salmon, and category 3 and 4 stocks.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Catches &amp; Kobe plots&lt;/h4&gt;
+&lt;p&gt;
+Status of stocks relative to the joint distribution of F/F&lt;sub&gt;MSY&lt;/sub&gt; and SSB/ MSY B&lt;sub&gt;trigger&lt;/sub&gt; (Kobe plot on the right/bottom) and 
+catches (triangles)/landings (circles) from the stocks latest advice (left/top plot). 
+Stocks in green are exploited at or below F&lt;sub&gt;MSY&lt;/sub&gt; while their sizes are also at or above MSY B&lt;sub&gt;trigger&lt;/sub&gt;. 
+Stocks in red are either exploited above F&lt;sub&gt;MSY&lt;/sub&gt; or have sizes below MSY B&lt;sub&gt;trigger&lt;/sub&gt;, or both. 
+Stocks in grey have unknown/undefined statuses in relation to at least one reference point.
+Stocks with proxy reference points are indicated with empty symbols (circles or triangles).
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h4&gt;Status trends plots&lt;/h4&gt;
+&lt;p&gt;
+Temporal trends in F/F&lt;sub&gt;MSY&lt;/sub&gt; and SSB/MSY B&lt;sub&gt;trigger&lt;/sub&gt; for all available stocks. Stocks with proxy reference points are indicated with dotted lines.
+&lt;/p&gt;
+</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Landings trends&lt;/h4&gt;
+&lt;p&gt;
+Landings (thousand tonnes) grouped by species common name &amp; fisheries guild, by fisheries guild and by country. 
+Group Undefined groups species that have not been assigned to a specific fisheries guild.
+When grouped by fisheries guild, total ladings are displayed with a dashed line.
+&lt;/p&gt; 
+&lt;h4&gt;Results description&lt;/h4&gt;
+&lt;p&gt;Main patterns and Trends: &lt;/p&gt;
 &lt;p&gt;Pelagic fisheries dominate landings (by volume) in the ecoregion. Blue whiting constitutes the highest proportion of pelagic landings, followed by mackerel. &lt;/p&gt;
 &lt;p&gt;Pelagic landings peaked in 1998 and in 2018 and ranged from [534] to [835] thousand tonnes in 2019-2023. &lt;/p&gt;
 &lt;p&gt;Annual mackerel landings have been below 200 thousand tonnes since 2018. Landings of herring and horse mackerel have been declining since the mid/late 1990s. &lt;/p&gt;
@@ -4396,101 +4493,52 @@
 &lt;p&gt;Otter trawling and seining is the dominant fishing effort, though has decline significantly over the time-series. Fishing effort by most other gears have also declined over the period, though more recently there has been a small increase in beam trawling (Figure 4). There are fluctuations in pelagic landings (Figure 5). Landings by demersal otter trawls, beam trawlers, pots, and static gears (mostly gillnet) have been relatively stable.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;The average discard rate among pelagic stocks is estimated to be very low. &lt;/p&gt;
+    <t>&lt;h4&gt;Landings trends&lt;/h4&gt;
+&lt;p&gt;
+Landings (thousand tonnes) grouped by species common name &amp; fisheries guild, by fisheries guild and by country. 
+Group Undefined groups species that have not been assigned to a specific fisheries guild.
+When grouped by fisheries guild, total ladings are displayed with a dashed line.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Discard trends&lt;/h4&gt;
+&lt;p&gt;
+Discard trends by fish fisheries guild shown as percentages (%) of the total annual catch in that
+category. 
+Some catches may occur outside the ecoregion and not all stock catches are disaggregated between landings
+and discards.
+&lt;/p&gt;
+&lt;h4&gt;Current discards&lt;/h4&gt;
+&lt;p&gt;
+Left/top panel: landings (green) and discards (orange) by fisheries guild
+(in thousand tonnes) only of the stocks with recorded discards. 
+Right/bottom panel: landings (green) and discards (orange) by fisheries guild (in thousand tonnes) of all
+stocks that have some catches in the ecoregion.
+&lt;/p&gt;
+&lt;p&gt;Elasmobranch discard data might highly uncertain, precaution is advised when interpreting the results.&lt;/p&gt;
+&lt;h4&gt;Results description&lt;/h4&gt;
+&lt;p&gt;The average discard rate among pelagic stocks is estimated to be very low. &lt;/p&gt;
 &lt;p&gt;The estimated average discard rate for elasmobranchs stocks is high and ranges 30% to 75%. &lt;/p&gt;
 &lt;p&gt;The average discard rate among demersal stocks ranges from 9% to 22% and is generally around 15%. &lt;/p&gt;
 &lt;p&gt;Crustacean and benthic stocks have an estimated average discard rate of around 10%. &lt;/p&gt;
 &lt;p&gt;Discard rates for some species are very high in the ecoregion, for example plaice (around 60% of tonnage) and whiting (50–99% of tonnage).&lt;/p&gt;</t>
   </si>
   <si>
-    <t>trends</t>
-  </si>
-  <si>
-    <t>cld</t>
-  </si>
-  <si>
-    <t>annex</t>
-  </si>
-  <si>
-    <t>&lt;h4&gt;MSY &amp; Precautionary Approach&lt;/h4&gt;
-&lt;p&gt;
-Summary of fishing mortality and stock size status relative to ICES maximum sustainable yield (MSY) approach and 
-precautionary approach (PA).
-&lt;/p&gt;
-&lt;p&gt;For the MSY: green represents stocks that are fished at or below F&lt;sub&gt;MSY&lt;/sub&gt; and whose sizes are equal to or greater than MSY B&lt;sub&gt;trigger&lt;/sub&gt;; 
-red represents stocks that are fished above F MSY or whose sizes are lower than MSY B&lt;sub&gt;trigger&lt;/sub&gt;.&lt;/p&gt;
-&lt;p&gt;For the PA: green represents stocks that are fished ator below F&lt;sub&gt;pa&lt;/sub&gt; and whose sizes are equal to or greater than B&lt;sub&gt;pa&lt;/sub&gt;; 
-orange represents stocks that are fished between F&lt;sub&gt;pa&lt;/sub&gt; and F&lt;sub&gt;lim&lt;/sub&gt; or whose sizes are between B&lt;sub&gt;lim&lt;/sub&gt; and B&lt;sub&gt;pa&lt;/sub&gt;; 
-red represents stocks that are fished above F&lt;sub&gt;lim&lt;/sub&gt; or whose sizes are lower than B&lt;sub&gt;lim&lt;/sub&gt;.&lt;/p&gt;
-&lt;p&gt;
-Grey represents stocks with unknown reference points.
-&lt;/p&gt;
-&lt;h4&gt;Catches in relation to MSY status&lt;/h4&gt;
-&lt;p&gt;
-Status summary of catches from stocks in the ecoregion relative to their latest stock assessment; the total
-catch of the stocks including catches taken outside the ecoregion.&lt;/p&gt;
-&lt;p&gt;Green represents the proportion of catch fished below F&lt;sub&gt;MSY&lt;/sub&gt; or whose stock size is greater than MSY B&lt;sub&gt;trigger&lt;/sub&gt;. 
-Red represents the proportion of catch fished above F&lt;sub&gt;MSY&lt;/sub&gt; or whose stock size is lower than MSY B&lt;sub&gt;trigger&lt;/sub&gt;. 
-Grey represents the proportion of catch lacking MSY reference points.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;h4&gt;MSY &amp; Precautionary Approach&lt;/h4&gt;
-&lt;p&gt;
-Summary of fishing mortality and stock size status relative to ICES maximum sustainable yield (MSY) approach and 
-precautionary approach (PA).
-&lt;/p&gt;
-&lt;p&gt;For the MSY: green represents stocks that are fished at or below F&lt;sub&gt;MSY&lt;/sub&gt; and whose sizes are equal to or greater than MSY B&lt;sub&gt;trigger&lt;/sub&gt;; 
-red represents stocks that are fished above F MSY or whose sizes are lower than MSY B&lt;sub&gt;trigger&lt;/sub&gt;.&lt;/p&gt;
-&lt;p&gt;For the PA: green represents stocks that are fished ator below F&lt;sub&gt;pa&lt;/sub&gt; and whose sizes are equal to or greater than B&lt;sub&gt;pa&lt;/sub&gt;; 
-orange represents stocks that are fished between F&lt;sub&gt;pa&lt;/sub&gt; and F&lt;sub&gt;lim&lt;/sub&gt; or whose sizes are between B&lt;sub&gt;lim&lt;/sub&gt; and B&lt;sub&gt;pa&lt;/sub&gt;; 
-red represents stocks that are fished above F&lt;sub&gt;lim&lt;/sub&gt; or whose sizes are lower than B&lt;sub&gt;lim&lt;/sub&gt;.&lt;/p&gt;
-&lt;p&gt;
-Grey represents stocks with unknown reference points.
-&lt;/p&gt;
-&lt;h4&gt;Catches in relation to MSY status&lt;/h4&gt;
-&lt;p&gt;
-Status summary of catches from stocks in the ecoregion relative to their latest stock assessment; the total
-catch of the stocks including catches taken outside the ecoregion.&lt;/p&gt;
-&lt;p&gt;Green represents the proportion of catch fished below F&lt;sub&gt;MSY&lt;/sub&gt; or whose stock size is greater than MSY B&lt;sub&gt;trigger&lt;/sub&gt;. 
-Red represents the proportion of catch fished above F&lt;sub&gt;MSY&lt;/sub&gt; or whose stock size is lower than MSY B&lt;sub&gt;trigger&lt;/sub&gt;. 
-Grey represents the proportion of catch lacking MSY reference points.&lt;/p&gt;
-&lt;h4&gt;Results description&lt;/h4&gt;
-&lt;p&gt;ICES currently provides advice for 112 stocks in the ecoregion. Of these, 9 (8%) benthic, 7 (6.2 %) pelagic, 10 (8.9 %) shellfish (Nephrops), 1 (0.8%) elasmobranch, and 17 (15.2%) demersal stocks have an ICES category 1 quantitative stock assessments. Demersal stocks include the three substocks of cod.27.46a7d20 (Northwestern, Viking, and Southern). Stock status is evaluated in terms of fishing mortality (F) and spawning-stock biomass (SSB) levels relative to the maximum sustainable yield (MSY) (F &lt; FMSY and SSB &gt; MSY Btrigger) and precautionary approach (PA) reference points (F &lt; FPA and SSB &gt; BPA).&lt;/p&gt;
-&lt;p&gt;In 2024, 39 (34.8%) of the assessed stocks are fished at or below FMSY levels, and 41 (36.6%) have a stock size equal to or above MSY Btrigger. These stocks account for 66.5% of total landings over the assessment area, which extends beyond the ecoregion. 24 (21.4%) of the assessed stocks are currently fished above FMSY and account for 90% of total landings over the assessment area.&lt;/p&gt;
-&lt;p&gt;Assessed stocks with unknown status relative to MSY and BPA represent 43% and 68%, respectively, of the stocks in the ecoregion. Stocks with unknown status relative to MSY account for 1.5% of total landings (although the assessment area for some stocks extends beyond the ecoregion)&lt;/p&gt;
-&lt;p&gt;Of the ten stocks that currently contribute most of the catch and landings in the ecoregion, haddock (had.27.46a20), boarfish (boc.27.6-8), hake (hke.27.3a46-abd), and anglerfish (mon.27.78abd) have a stock status above MSY Btrigger and fishing pressure below the FMSY, while mackerel (mac.27.nea), herring (her.27.nirs), cod (cod.27.7e-k), cod (cod.27.46a7d20 (all 3 sub-stocks)) and whiting (whg.27.7a) and (whg.27.7b-ce-k) are below MSY Btrigger and are currently fished above FMSY.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;h4&gt;Status trends plots&lt;/h4&gt;
-&lt;p&gt;
-Temporal trends in F/F&lt;sub&gt;MSY&lt;/sub&gt; and SSB/MSY B&lt;sub&gt;trigger&lt;/sub&gt; for all available stocks. Stocks with proxy reference points are indicated with dotted lines.
-&lt;/p&gt;
-&lt;h4&gt;Results description&lt;/h4&gt;
-&lt;p&gt;On average, the spawning-stock size in all guilds (mean SSB/MSYBtrigger ratio) is currently above one, although it ranges from 3.2 to 1.3 among stocks. Fishing pressure for the elasmobranch, benthic, shellfish and pelagic guilds on average is currently below FMSY (range from 0.5 to 0.89 among stocks), while demersal species are fished above FMSY (mean F/FMSY ratio of 1.3).&lt;/p&gt;
-&lt;p&gt;For the elasmobranch guild, the mean F/FMSY ratio has declined since the 1990s and is currently below one. The mean SSB/MSY Btrigger ratio has increased since the 1980s and is currently above one.&lt;/p&gt;
-&lt;p&gt;For the benthic guild, the mean F/FMSY ratio has declined since the mid-1990s and is currently below one. The mean SSB/MSY Btrigger ratio has gradually increased since 2000 and is currently above one.&lt;/p&gt;
-&lt;p&gt;For the shellfish guild, the mean F/FMSY ratio shows strong fluctuations about a gradual decline from the mid-2000s and is currently below one. The mean SSB/MSY Btrigger ratio has remained above one and fairly stable throughout the time-series and is currently above one.&lt;/p&gt;
-&lt;p&gt;For the demersal guild, the mean F/FMSY ratio has declined since the 1990s and is currently above one. The mean SSB/MSY Btrigger ratio shows a small, gradual increase since 2000 and is currently above one.&lt;/p&gt;
-&lt;p&gt;For the pelagic guild, the mean F/FMSY ratio has fluctuated (mostly above one) since the 1990s and is currently below one. The mean SSB/MSY Btrigger ratio has remained fairly stable above one since the mid-1990s and is currently above one.&lt;/p&gt;
-&lt;p&gt;Not all species with catch advice are assessed against any PA or MSY reference points because these points are undefined; this includes European eel, salmon, and category 3 and 4 stocks.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;h4&gt;Catches &amp; Kobe plots&lt;/h4&gt;
-&lt;p&gt;
-Status of stocks relative to the joint distribution of F/F&lt;sub&gt;MSY&lt;/sub&gt; and SSB/ MSY B&lt;sub&gt;trigger&lt;/sub&gt; (Kobe plot on the right/bottom) and 
-catches (triangles)/landings (circles) from the stocks latest advice (left/top plot). 
-Stocks in green are exploited at or below F&lt;sub&gt;MSY&lt;/sub&gt; while their sizes are also at or above MSY B&lt;sub&gt;trigger&lt;/sub&gt;. 
-Stocks in red are either exploited above F&lt;sub&gt;MSY&lt;/sub&gt; or have sizes below MSY B&lt;sub&gt;trigger&lt;/sub&gt;, or both. 
-Stocks in grey have unknown/undefined statuses in relation to at least one reference point.
-Stocks with proxy reference points are indicated with empty symbols (circles or triangles).
-&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h4&gt;Status trends plots&lt;/h4&gt;
-&lt;p&gt;
-Temporal trends in F/F&lt;sub&gt;MSY&lt;/sub&gt; and SSB/MSY B&lt;sub&gt;trigger&lt;/sub&gt; for all available stocks. Stocks with proxy reference points are indicated with dotted lines.
-&lt;/p&gt;
-</t>
+    <t>&lt;h4&gt;Discard trends&lt;/h4&gt;
+&lt;p&gt;
+Discard trends by fish fisheries guild shown as percentages (%) of the total annual catch in that
+category. 
+Some catches may occur outside the ecoregion and not all stock catches are disaggregated between landings
+and discards.
+&lt;/p&gt;
+&lt;h4&gt;Current discards&lt;/h4&gt;
+&lt;p&gt;
+Left/top panel: landings (green) and discards (orange) by fisheries guild
+(in thousand tonnes) only of the stocks with recorded discards. 
+Right/bottom panel: landings (green) and discards (orange) by fisheries guild (in thousand tonnes) of all
+stocks that have some catches in the ecoregion.
+&lt;/p&gt;
+&lt;p&gt;Elasmobranch discard data might highly uncertain, precaution is advised when interpreting the results.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -4930,16 +4978,16 @@
       <selection activeCell="A2" sqref="A2:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="168.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="37.77734375" customWidth="1"/>
-    <col min="17" max="17" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="168.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37.81640625" customWidth="1"/>
+    <col min="17" max="17" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -4950,7 +4998,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>29</v>
       </c>
@@ -4961,7 +5009,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>43</v>
       </c>
@@ -4972,7 +5020,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -4983,7 +5031,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
@@ -4994,7 +5042,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>45</v>
       </c>
@@ -5005,7 +5053,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
@@ -5016,7 +5064,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
@@ -5027,7 +5075,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>25</v>
       </c>
@@ -5038,7 +5086,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>49</v>
       </c>
@@ -5049,7 +5097,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
@@ -5060,7 +5108,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>41</v>
       </c>
@@ -5071,7 +5119,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>23</v>
       </c>
@@ -5082,7 +5130,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>35</v>
       </c>
@@ -5093,7 +5141,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>31</v>
       </c>
@@ -5104,7 +5152,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -5115,7 +5163,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>39</v>
       </c>
@@ -5126,7 +5174,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>33</v>
       </c>
@@ -5137,7 +5185,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>37</v>
       </c>
@@ -5148,7 +5196,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>47</v>
       </c>
@@ -5159,7 +5207,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
         <v>66</v>
       </c>
@@ -5170,7 +5218,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>69</v>
       </c>
@@ -5181,7 +5229,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
         <v>72</v>
       </c>
@@ -5192,7 +5240,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>75</v>
       </c>
@@ -5203,7 +5251,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>78</v>
       </c>
@@ -5214,7 +5262,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>81</v>
       </c>
@@ -5225,7 +5273,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>84</v>
       </c>
@@ -5236,7 +5284,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>87</v>
       </c>
@@ -5247,7 +5295,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>90</v>
       </c>
@@ -5258,7 +5306,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>93</v>
       </c>
@@ -5269,7 +5317,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>96</v>
       </c>
@@ -5280,7 +5328,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
         <v>99</v>
       </c>
@@ -5291,7 +5339,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
         <v>102</v>
       </c>
@@ -5302,7 +5350,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
         <v>105</v>
       </c>
@@ -5313,7 +5361,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
         <v>108</v>
       </c>
@@ -5324,7 +5372,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
         <v>111</v>
       </c>
@@ -5335,7 +5383,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="10" t="s">
         <v>114</v>
       </c>
@@ -5346,7 +5394,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
         <v>117</v>
       </c>
@@ -5357,7 +5405,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="s">
         <v>120</v>
       </c>
@@ -5368,7 +5416,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="10" t="s">
         <v>123</v>
       </c>
@@ -5379,7 +5427,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
         <v>126</v>
       </c>
@@ -5390,7 +5438,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
         <v>129</v>
       </c>
@@ -5401,7 +5449,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="s">
         <v>132</v>
       </c>
@@ -5412,7 +5460,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="10" t="s">
         <v>135</v>
       </c>
@@ -5423,7 +5471,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="s">
         <v>138</v>
       </c>
@@ -5434,7 +5482,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="s">
         <v>141</v>
       </c>
@@ -5445,7 +5493,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="s">
         <v>144</v>
       </c>
@@ -5456,7 +5504,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
         <v>147</v>
       </c>
@@ -5467,7 +5515,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
         <v>150</v>
       </c>
@@ -5478,7 +5526,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="s">
         <v>153</v>
       </c>
@@ -5489,7 +5537,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="10" t="s">
         <v>156</v>
       </c>
@@ -5500,7 +5548,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="10" t="s">
         <v>159</v>
       </c>
@@ -5511,7 +5559,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="10" t="s">
         <v>162</v>
       </c>
@@ -5522,7 +5570,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
         <v>165</v>
       </c>
@@ -5533,7 +5581,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="10" t="s">
         <v>168</v>
       </c>
@@ -5544,7 +5592,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
         <v>171</v>
       </c>
@@ -5555,7 +5603,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
         <v>174</v>
       </c>
@@ -5566,7 +5614,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="s">
         <v>177</v>
       </c>
@@ -5577,7 +5625,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
         <v>180</v>
       </c>
@@ -5588,7 +5636,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="10" t="s">
         <v>183</v>
       </c>
@@ -5599,7 +5647,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="10" t="s">
         <v>186</v>
       </c>
@@ -5610,7 +5658,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
         <v>189</v>
       </c>
@@ -5621,7 +5669,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
         <v>192</v>
       </c>
@@ -5632,7 +5680,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
         <v>195</v>
       </c>
@@ -5643,7 +5691,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="s">
         <v>198</v>
       </c>
@@ -5654,7 +5702,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
         <v>201</v>
       </c>
@@ -5665,7 +5713,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="10" t="s">
         <v>204</v>
       </c>
@@ -5676,7 +5724,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="10" t="s">
         <v>207</v>
       </c>
@@ -5687,7 +5735,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="s">
         <v>210</v>
       </c>
@@ -5698,7 +5746,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
         <v>213</v>
       </c>
@@ -5709,7 +5757,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="10" t="s">
         <v>216</v>
       </c>
@@ -5720,7 +5768,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
         <v>219</v>
       </c>
@@ -5731,7 +5779,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="10" t="s">
         <v>222</v>
       </c>
@@ -5742,7 +5790,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="10" t="s">
         <v>225</v>
       </c>
@@ -5753,7 +5801,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="10" t="s">
         <v>228</v>
       </c>
@@ -5764,7 +5812,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="10" t="s">
         <v>231</v>
       </c>
@@ -5775,7 +5823,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="10" t="s">
         <v>234</v>
       </c>
@@ -5786,7 +5834,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="10" t="s">
         <v>237</v>
       </c>
@@ -5797,7 +5845,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="10" t="s">
         <v>240</v>
       </c>
@@ -5808,7 +5856,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="10" t="s">
         <v>243</v>
       </c>
@@ -5819,7 +5867,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="10" t="s">
         <v>246</v>
       </c>
@@ -5830,7 +5878,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="10" t="s">
         <v>249</v>
       </c>
@@ -5841,7 +5889,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="10" t="s">
         <v>252</v>
       </c>
@@ -5852,7 +5900,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="10" t="s">
         <v>255</v>
       </c>
@@ -5863,7 +5911,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="10" t="s">
         <v>258</v>
       </c>
@@ -5874,7 +5922,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="10" t="s">
         <v>261</v>
       </c>
@@ -5885,7 +5933,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="10" t="s">
         <v>264</v>
       </c>
@@ -5896,7 +5944,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="10" t="s">
         <v>267</v>
       </c>
@@ -5907,7 +5955,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="10" t="s">
         <v>270</v>
       </c>
@@ -5918,7 +5966,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="10" t="s">
         <v>273</v>
       </c>
@@ -5929,7 +5977,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="10" t="s">
         <v>276</v>
       </c>
@@ -5940,7 +5988,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="10" t="s">
         <v>279</v>
       </c>
@@ -5951,7 +5999,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="10" t="s">
         <v>282</v>
       </c>
@@ -5962,7 +6010,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="10" t="s">
         <v>285</v>
       </c>
@@ -5973,7 +6021,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="10" t="s">
         <v>288</v>
       </c>
@@ -5984,7 +6032,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="10" t="s">
         <v>291</v>
       </c>
@@ -5995,7 +6043,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="10" t="s">
         <v>294</v>
       </c>
@@ -6006,7 +6054,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="10" t="s">
         <v>297</v>
       </c>
@@ -6017,7 +6065,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="10" t="s">
         <v>300</v>
       </c>
@@ -6028,7 +6076,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="10" t="s">
         <v>303</v>
       </c>
@@ -6039,7 +6087,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="10" t="s">
         <v>306</v>
       </c>
@@ -6050,7 +6098,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="10" t="s">
         <v>309</v>
       </c>
@@ -6061,7 +6109,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="10" t="s">
         <v>312</v>
       </c>
@@ -6072,7 +6120,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="10" t="s">
         <v>315</v>
       </c>
@@ -6083,7 +6131,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="10" t="s">
         <v>318</v>
       </c>
@@ -6094,7 +6142,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="10" t="s">
         <v>321</v>
       </c>
@@ -6105,7 +6153,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="10" t="s">
         <v>324</v>
       </c>
@@ -6116,7 +6164,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="10" t="s">
         <v>327</v>
       </c>
@@ -6127,7 +6175,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="10" t="s">
         <v>330</v>
       </c>
@@ -6138,7 +6186,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="10" t="s">
         <v>333</v>
       </c>
@@ -6149,7 +6197,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="10" t="s">
         <v>336</v>
       </c>
@@ -6160,7 +6208,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="10" t="s">
         <v>339</v>
       </c>
@@ -6171,7 +6219,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="10" t="s">
         <v>342</v>
       </c>
@@ -6182,7 +6230,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="10" t="s">
         <v>345</v>
       </c>
@@ -6193,7 +6241,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="10" t="s">
         <v>348</v>
       </c>
@@ -6204,7 +6252,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="10" t="s">
         <v>351</v>
       </c>
@@ -6215,7 +6263,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="10" t="s">
         <v>354</v>
       </c>
@@ -6226,7 +6274,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="10" t="s">
         <v>357</v>
       </c>
@@ -6237,7 +6285,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="10" t="s">
         <v>360</v>
       </c>
@@ -6248,7 +6296,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="10" t="s">
         <v>363</v>
       </c>
@@ -6259,7 +6307,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="10" t="s">
         <v>366</v>
       </c>
@@ -6270,7 +6318,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="10" t="s">
         <v>369</v>
       </c>
@@ -6281,7 +6329,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="10" t="s">
         <v>372</v>
       </c>
@@ -6292,7 +6340,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="10" t="s">
         <v>375</v>
       </c>
@@ -6303,7 +6351,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="10" t="s">
         <v>378</v>
       </c>
@@ -6314,7 +6362,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="10" t="s">
         <v>381</v>
       </c>
@@ -6325,7 +6373,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="10" t="s">
         <v>384</v>
       </c>
@@ -6336,7 +6384,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="10" t="s">
         <v>387</v>
       </c>
@@ -6347,7 +6395,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="10" t="s">
         <v>390</v>
       </c>
@@ -6358,7 +6406,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="10" t="s">
         <v>393</v>
       </c>
@@ -6369,7 +6417,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="10" t="s">
         <v>396</v>
       </c>
@@ -6380,7 +6428,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="10" t="s">
         <v>399</v>
       </c>
@@ -6391,7 +6439,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="10" t="s">
         <v>402</v>
       </c>
@@ -6402,7 +6450,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="10" t="s">
         <v>405</v>
       </c>
@@ -6413,7 +6461,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="10" t="s">
         <v>408</v>
       </c>
@@ -6424,7 +6472,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="10" t="s">
         <v>411</v>
       </c>
@@ -6435,7 +6483,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="10" t="s">
         <v>414</v>
       </c>
@@ -6446,7 +6494,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="10" t="s">
         <v>417</v>
       </c>
@@ -6457,7 +6505,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="10" t="s">
         <v>420</v>
       </c>
@@ -6468,7 +6516,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" s="10" t="s">
         <v>423</v>
       </c>
@@ -6479,7 +6527,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="10" t="s">
         <v>426</v>
       </c>
@@ -6490,7 +6538,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="10" t="s">
         <v>429</v>
       </c>
@@ -6501,7 +6549,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="10" t="s">
         <v>432</v>
       </c>
@@ -6512,7 +6560,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="10" t="s">
         <v>435</v>
       </c>
@@ -6523,7 +6571,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="10" t="s">
         <v>438</v>
       </c>
@@ -6534,7 +6582,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="10" t="s">
         <v>441</v>
       </c>
@@ -6545,7 +6593,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="10" t="s">
         <v>444</v>
       </c>
@@ -6556,7 +6604,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="10" t="s">
         <v>447</v>
       </c>
@@ -6567,7 +6615,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" s="10" t="s">
         <v>450</v>
       </c>
@@ -6578,7 +6626,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="10" t="s">
         <v>453</v>
       </c>
@@ -6589,7 +6637,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="10" t="s">
         <v>456</v>
       </c>
@@ -6600,7 +6648,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="10" t="s">
         <v>459</v>
       </c>
@@ -6611,7 +6659,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="10" t="s">
         <v>462</v>
       </c>
@@ -6622,7 +6670,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="10" t="s">
         <v>465</v>
       </c>
@@ -6633,7 +6681,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="10" t="s">
         <v>468</v>
       </c>
@@ -6644,7 +6692,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" s="10" t="s">
         <v>471</v>
       </c>
@@ -6655,7 +6703,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="10" t="s">
         <v>474</v>
       </c>
@@ -6666,7 +6714,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="10" t="s">
         <v>477</v>
       </c>
@@ -6677,7 +6725,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="10" t="s">
         <v>480</v>
       </c>
@@ -6688,7 +6736,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="10" t="s">
         <v>483</v>
       </c>
@@ -6699,7 +6747,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="10" t="s">
         <v>486</v>
       </c>
@@ -6710,7 +6758,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="10" t="s">
         <v>489</v>
       </c>
@@ -6721,7 +6769,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="10" t="s">
         <v>492</v>
       </c>
@@ -6732,7 +6780,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="10" t="s">
         <v>495</v>
       </c>
@@ -6743,7 +6791,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="10" t="s">
         <v>498</v>
       </c>
@@ -6754,7 +6802,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="10" t="s">
         <v>501</v>
       </c>
@@ -6765,7 +6813,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="10" t="s">
         <v>504</v>
       </c>
@@ -6776,7 +6824,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="10" t="s">
         <v>507</v>
       </c>
@@ -6787,7 +6835,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="10" t="s">
         <v>510</v>
       </c>
@@ -6798,7 +6846,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" s="10" t="s">
         <v>513</v>
       </c>
@@ -6809,7 +6857,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" s="10" t="s">
         <v>516</v>
       </c>
@@ -6820,7 +6868,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" s="10" t="s">
         <v>519</v>
       </c>
@@ -6831,7 +6879,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="10" t="s">
         <v>522</v>
       </c>
@@ -6842,7 +6890,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" s="10" t="s">
         <v>525</v>
       </c>
@@ -6853,7 +6901,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" s="10" t="s">
         <v>528</v>
       </c>
@@ -6864,7 +6912,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" s="10" t="s">
         <v>531</v>
       </c>
@@ -6875,7 +6923,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" s="10" t="s">
         <v>534</v>
       </c>
@@ -6886,7 +6934,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" s="10" t="s">
         <v>537</v>
       </c>
@@ -6897,7 +6945,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" s="10" t="s">
         <v>540</v>
       </c>
@@ -6908,7 +6956,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" s="10" t="s">
         <v>543</v>
       </c>
@@ -6919,7 +6967,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" s="10" t="s">
         <v>546</v>
       </c>
@@ -6930,7 +6978,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" s="10" t="s">
         <v>549</v>
       </c>
@@ -6941,7 +6989,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" s="10" t="s">
         <v>552</v>
       </c>
@@ -6952,7 +7000,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" s="10" t="s">
         <v>555</v>
       </c>
@@ -6963,7 +7011,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" s="10" t="s">
         <v>558</v>
       </c>
@@ -6974,7 +7022,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" s="10" t="s">
         <v>561</v>
       </c>
@@ -6985,7 +7033,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" s="10" t="s">
         <v>564</v>
       </c>
@@ -6996,7 +7044,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" s="10" t="s">
         <v>567</v>
       </c>
@@ -7007,7 +7055,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" s="10" t="s">
         <v>570</v>
       </c>
@@ -7018,7 +7066,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" s="10" t="s">
         <v>573</v>
       </c>
@@ -7029,7 +7077,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" s="10" t="s">
         <v>576</v>
       </c>
@@ -7040,7 +7088,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" s="10" t="s">
         <v>579</v>
       </c>
@@ -7051,7 +7099,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" s="10" t="s">
         <v>582</v>
       </c>
@@ -7062,7 +7110,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" s="10" t="s">
         <v>585</v>
       </c>
@@ -7073,7 +7121,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" s="10" t="s">
         <v>588</v>
       </c>
@@ -7084,7 +7132,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" s="10" t="s">
         <v>591</v>
       </c>
@@ -7095,7 +7143,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" s="10" t="s">
         <v>594</v>
       </c>
@@ -7106,7 +7154,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198" s="10" t="s">
         <v>597</v>
       </c>
@@ -7117,7 +7165,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" s="10" t="s">
         <v>600</v>
       </c>
@@ -7128,7 +7176,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200" s="10" t="s">
         <v>603</v>
       </c>
@@ -7139,7 +7187,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201" s="10" t="s">
         <v>606</v>
       </c>
@@ -7150,7 +7198,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" s="10" t="s">
         <v>609</v>
       </c>
@@ -7161,7 +7209,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203" s="10" t="s">
         <v>612</v>
       </c>
@@ -7172,7 +7220,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204" s="10" t="s">
         <v>615</v>
       </c>
@@ -7183,7 +7231,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205" s="10" t="s">
         <v>618</v>
       </c>
@@ -7194,7 +7242,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206" s="10" t="s">
         <v>621</v>
       </c>
@@ -7205,7 +7253,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207" s="10" t="s">
         <v>624</v>
       </c>
@@ -7216,7 +7264,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A208" s="10" t="s">
         <v>627</v>
       </c>
@@ -7227,7 +7275,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A209" s="10" t="s">
         <v>630</v>
       </c>
@@ -7238,7 +7286,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A210" s="10" t="s">
         <v>633</v>
       </c>
@@ -7249,7 +7297,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A211" s="10" t="s">
         <v>636</v>
       </c>
@@ -7260,7 +7308,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A212" s="10" t="s">
         <v>639</v>
       </c>
@@ -7271,7 +7319,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A213" s="10" t="s">
         <v>642</v>
       </c>
@@ -7282,7 +7330,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A214" s="10" t="s">
         <v>645</v>
       </c>
@@ -7293,7 +7341,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A215" s="10" t="s">
         <v>648</v>
       </c>
@@ -7304,7 +7352,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A216" s="10" t="s">
         <v>651</v>
       </c>
@@ -7315,7 +7363,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A217" s="10" t="s">
         <v>654</v>
       </c>
@@ -7326,7 +7374,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A218" s="10" t="s">
         <v>657</v>
       </c>
@@ -7337,7 +7385,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A219" s="10" t="s">
         <v>660</v>
       </c>
@@ -7348,7 +7396,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A220" s="10" t="s">
         <v>663</v>
       </c>
@@ -7359,7 +7407,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A221" s="10" t="s">
         <v>666</v>
       </c>
@@ -7370,7 +7418,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A222" s="10" t="s">
         <v>669</v>
       </c>
@@ -7381,7 +7429,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A223" s="10" t="s">
         <v>672</v>
       </c>
@@ -7392,7 +7440,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A224" s="10" t="s">
         <v>675</v>
       </c>
@@ -7403,7 +7451,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225" s="10" t="s">
         <v>678</v>
       </c>
@@ -7414,7 +7462,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A226" s="10" t="s">
         <v>681</v>
       </c>
@@ -7425,7 +7473,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227" s="10" t="s">
         <v>684</v>
       </c>
@@ -7436,7 +7484,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228" s="10" t="s">
         <v>687</v>
       </c>
@@ -7447,7 +7495,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229" s="10" t="s">
         <v>690</v>
       </c>
@@ -7458,7 +7506,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230" s="10" t="s">
         <v>693</v>
       </c>
@@ -7469,7 +7517,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231" s="10" t="s">
         <v>696</v>
       </c>
@@ -7480,7 +7528,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232" s="10" t="s">
         <v>699</v>
       </c>
@@ -7491,7 +7539,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233" s="10" t="s">
         <v>702</v>
       </c>
@@ -7502,7 +7550,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234" s="10" t="s">
         <v>705</v>
       </c>
@@ -7513,7 +7561,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235" s="10" t="s">
         <v>708</v>
       </c>
@@ -7524,7 +7572,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236" s="10" t="s">
         <v>711</v>
       </c>
@@ -7535,7 +7583,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237" s="10" t="s">
         <v>714</v>
       </c>
@@ -7546,7 +7594,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238" s="10" t="s">
         <v>717</v>
       </c>
@@ -7557,7 +7605,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" s="10" t="s">
         <v>720</v>
       </c>
@@ -7568,7 +7616,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240" s="10" t="s">
         <v>723</v>
       </c>
@@ -7579,7 +7627,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241" s="10" t="s">
         <v>726</v>
       </c>
@@ -7590,7 +7638,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242" s="10" t="s">
         <v>729</v>
       </c>
@@ -7601,7 +7649,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243" s="10" t="s">
         <v>732</v>
       </c>
@@ -7612,7 +7660,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244" s="10" t="s">
         <v>735</v>
       </c>
@@ -7623,7 +7671,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245" s="10" t="s">
         <v>738</v>
       </c>
@@ -7634,7 +7682,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246" s="10" t="s">
         <v>741</v>
       </c>
@@ -7645,7 +7693,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247" s="10" t="s">
         <v>744</v>
       </c>
@@ -7656,7 +7704,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248" s="10" t="s">
         <v>747</v>
       </c>
@@ -7667,7 +7715,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249" s="10" t="s">
         <v>750</v>
       </c>
@@ -7678,7 +7726,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250" s="10" t="s">
         <v>753</v>
       </c>
@@ -7689,7 +7737,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A251" s="10" t="s">
         <v>756</v>
       </c>
@@ -7700,7 +7748,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A252" s="10" t="s">
         <v>759</v>
       </c>
@@ -7711,7 +7759,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A253" s="10" t="s">
         <v>762</v>
       </c>
@@ -7722,7 +7770,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A254" s="10" t="s">
         <v>765</v>
       </c>
@@ -7733,7 +7781,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A255" s="10" t="s">
         <v>768</v>
       </c>
@@ -7744,7 +7792,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A256" s="10" t="s">
         <v>771</v>
       </c>
@@ -7755,7 +7803,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A257" s="10" t="s">
         <v>774</v>
       </c>
@@ -7766,7 +7814,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A258" s="10" t="s">
         <v>777</v>
       </c>
@@ -7777,7 +7825,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A259" s="10" t="s">
         <v>780</v>
       </c>
@@ -7788,7 +7836,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A260" s="10" t="s">
         <v>783</v>
       </c>
@@ -7799,7 +7847,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A261" s="10" t="s">
         <v>786</v>
       </c>
@@ -7810,7 +7858,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A262" s="10" t="s">
         <v>789</v>
       </c>
@@ -7821,7 +7869,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A263" s="10" t="s">
         <v>792</v>
       </c>
@@ -7832,7 +7880,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A264" s="10" t="s">
         <v>795</v>
       </c>
@@ -7843,7 +7891,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A265" s="10" t="s">
         <v>798</v>
       </c>
@@ -7854,7 +7902,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A266" s="10" t="s">
         <v>801</v>
       </c>
@@ -7865,7 +7913,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A267" s="10" t="s">
         <v>804</v>
       </c>
@@ -7876,7 +7924,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A268" s="10" t="s">
         <v>807</v>
       </c>
@@ -7887,7 +7935,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A269" s="10" t="s">
         <v>810</v>
       </c>
@@ -7898,7 +7946,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A270" s="10" t="s">
         <v>813</v>
       </c>
@@ -7909,7 +7957,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A271" s="10" t="s">
         <v>816</v>
       </c>
@@ -7920,7 +7968,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A272" s="10" t="s">
         <v>819</v>
       </c>
@@ -7931,7 +7979,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A273" s="10" t="s">
         <v>822</v>
       </c>
@@ -7942,7 +7990,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A274" s="10" t="s">
         <v>825</v>
       </c>
@@ -7953,7 +8001,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A275" s="10" t="s">
         <v>828</v>
       </c>
@@ -7964,7 +8012,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A276" s="10" t="s">
         <v>831</v>
       </c>
@@ -7975,7 +8023,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A277" s="10" t="s">
         <v>834</v>
       </c>
@@ -7986,7 +8034,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A278" s="10" t="s">
         <v>837</v>
       </c>
@@ -7997,7 +8045,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A279" s="10" t="s">
         <v>840</v>
       </c>
@@ -8008,7 +8056,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A280" s="10" t="s">
         <v>843</v>
       </c>
@@ -8019,7 +8067,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A281" s="10" t="s">
         <v>846</v>
       </c>
@@ -8030,7 +8078,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A282" s="10" t="s">
         <v>849</v>
       </c>
@@ -8041,7 +8089,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A283" s="10" t="s">
         <v>852</v>
       </c>
@@ -8052,7 +8100,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A284" s="10" t="s">
         <v>855</v>
       </c>
@@ -8063,7 +8111,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A285" s="10" t="s">
         <v>858</v>
       </c>
@@ -8074,7 +8122,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A286" s="10" t="s">
         <v>861</v>
       </c>
@@ -8085,7 +8133,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A287" s="10" t="s">
         <v>864</v>
       </c>
@@ -8096,7 +8144,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A288" s="10" t="s">
         <v>867</v>
       </c>
@@ -8107,7 +8155,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A289" s="10" t="s">
         <v>870</v>
       </c>
@@ -8118,7 +8166,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A290" s="10" t="s">
         <v>873</v>
       </c>
@@ -8129,7 +8177,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A291" s="10" t="s">
         <v>876</v>
       </c>
@@ -8140,7 +8188,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A292" s="10" t="s">
         <v>879</v>
       </c>
@@ -8173,13 +8221,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8187,7 +8235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
@@ -8195,7 +8243,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="303" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="303" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -8203,7 +8251,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -8227,13 +8275,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="198.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="198.36328125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8241,7 +8289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="343.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="343.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
@@ -8249,7 +8297,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -8257,7 +8305,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -8278,13 +8326,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="229.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="229.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8292,7 +8340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
@@ -8300,7 +8348,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -8308,7 +8356,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -8325,17 +8373,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2C24DB-5CFD-48C4-BB67-81838BA61C50}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8343,17 +8391,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>928</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8364,17 +8416,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176BBE4C-C868-422D-A432-89141BF78270}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8382,17 +8434,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>928</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8403,17 +8459,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537C8D36-44B6-40AB-B2F5-C278C8F38BBE}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8421,17 +8477,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>928</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8442,17 +8502,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1208CFA8-0BD4-4A00-92D8-FF2B69E34213}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8460,17 +8520,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>928</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8481,16 +8545,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D76C43-B7D3-42D3-B057-81CA4865142E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="125.5546875" customWidth="1"/>
+    <col min="2" max="2" width="125.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8498,20 +8562,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="319" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>918</v>
+        <v>927</v>
       </c>
     </row>
   </sheetData>
@@ -8523,17 +8587,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C668CA08-39B4-442C-BE86-54D5793A9F15}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8541,17 +8605,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>928</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8562,17 +8630,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82938685-CEEB-4659-B68E-B225C7C9053C}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8580,17 +8648,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>928</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8605,13 +8677,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="152.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="152.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8619,7 +8691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="258.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="258.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
@@ -8627,7 +8699,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -8635,7 +8707,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -8652,17 +8724,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2B002E-5D4B-4A97-8E05-ADA2BC7262BC}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8670,17 +8742,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>928</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8694,17 +8770,17 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8712,17 +8788,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>928</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8733,17 +8813,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35913B4E-3457-4352-AB64-7123F047E008}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8751,17 +8831,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>928</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8772,17 +8856,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FEA048-930A-43AC-A2F7-E864F3A29AEA}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8790,20 +8874,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>928</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8811,17 +8900,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDA5AB7-BD7F-4972-B610-8565F27586E1}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="199.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="199.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8829,33 +8918,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>886</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>918</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>919</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>920</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -8872,13 +8961,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="199.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="199.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8886,33 +8975,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>886</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>918</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>919</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>920</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -8928,13 +9017,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="199.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="199.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8942,33 +9031,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>886</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>918</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>919</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>920</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -8984,13 +9073,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="199.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="199.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8998,33 +9087,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>886</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>918</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>919</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>920</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -9043,13 +9132,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="199.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="199.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9057,33 +9146,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>886</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>918</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>923</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>919</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>920</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -9099,13 +9188,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="199.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="199.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9113,33 +9202,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>886</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>918</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>919</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>920</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -9155,13 +9244,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="253.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="253.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9169,7 +9258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="279" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="279" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
@@ -9177,7 +9266,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -9185,7 +9274,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -9206,13 +9295,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="199.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="199.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9220,33 +9309,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>886</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>918</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>919</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>920</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -9262,13 +9351,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="199.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="199.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9276,33 +9365,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>886</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>918</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>919</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>920</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -9318,13 +9407,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="199.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="199.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9332,33 +9421,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>886</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>918</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>919</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>920</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -9374,13 +9463,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="199.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="199.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9388,33 +9477,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>886</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>918</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>919</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>920</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -9430,13 +9519,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="199.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="199.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9444,33 +9533,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>886</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>917</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>918</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>919</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>920</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -9487,12 +9576,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9500,7 +9589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -9522,12 +9611,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9535,7 +9624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -9557,13 +9646,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="159.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="159.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9571,7 +9660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -9592,13 +9681,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="223.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="223.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9606,7 +9695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="319" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
@@ -9614,7 +9703,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -9622,7 +9711,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -9643,13 +9732,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="181.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="181.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9657,7 +9746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
@@ -9665,7 +9754,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -9673,7 +9762,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -9694,13 +9783,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="222.21875" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="222.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9708,7 +9797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="360" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
@@ -9716,7 +9805,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -9724,7 +9813,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -9745,13 +9834,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="137.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="137.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9759,7 +9848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="390" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="400" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
@@ -9767,7 +9856,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -9775,7 +9864,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -9783,13 +9872,13 @@
         <v>910</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.4">
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.4">
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="6"/>
     </row>
   </sheetData>
@@ -9805,13 +9894,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="135.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="135.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9819,7 +9908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
@@ -9827,7 +9916,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -9835,7 +9924,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -9856,13 +9945,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="114.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="114.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9870,7 +9959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
@@ -9878,7 +9967,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -9886,7 +9975,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
chore: update binary data files for texts
</commit_message>
<xml_diff>
--- a/data-raw/texts.xlsx
+++ b/data-raw/texts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icesit-my.sharepoint.com/personal/luca_lamoni_ices_dk/Documents/Microsoft Teams Chat Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_2023\fisheriesXplorer\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{6BF4C849-F593-4B1C-8AF3-FA9B6EBE9C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C57AD508-0290-482B-B014-B58113133AF6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E044A1-E485-4141-A302-B20CAAACF0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="826" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26160" yWindow="1440" windowWidth="47880" windowHeight="12996" tabRatio="826" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="glossary" sheetId="17" r:id="rId1"/>
@@ -2918,42 +2918,6 @@
   </si>
   <si>
     <t>&lt;p&gt;
-The Celtic Seas ecoregion covers the northwestern shelf seas of Europe (Figure 1). It includes areas of the deeper eastern
-Atlantic Ocean and coastal seas that are heavily influenced by oceanic inputs. The ecoregion ranges from north of Shetland
-to Brittany in the south. Three key areas constitute this ecoregion:
-&lt;/p&gt;
-&lt;ol&gt;
-  &lt;li&gt;
-    northern parts: the Malin shelf, west of Scotland, eastern Rockall Bank, and north of Scotland (parts of Subdivision
-    2.a.2, divisions 4.a and 6.a, and Subdivision 6.b.2);
-  &lt;/li&gt;
-  &lt;li&gt;
-    the Celtic Sea(*), Bristol Channel, Western English Channel, southwest and west of Ireland (Division 7.b and Subdivision
-    7.c.2; parts of divisions 7.e, 7.f, 7.g, 7.h, and subdivisions 7.j.2 and 7.k.2);
-  &lt;/li&gt;
-  &lt;li&gt;
-    the Irish Sea (Division 7.a).
-  &lt;/li&gt;
-&lt;/ol&gt;
-&lt;p&gt;
-In the north, there are strong links with the North Sea; in the southeast, a strong link with the channel area; and in the
-south a strong link with the Bay of Biscay. The eastern part of the Rockall Bank is within the geographic scope of the
-ecoregion, although it is separated from the western European shelf by the Rockall Trough.
-&lt;/p&gt;
-&lt;p&gt;
-The scientific names of all species described in this overview are listed in the Stock Status Lookup.
-&lt;/p&gt;
-&lt;p&gt;
-The overview covers ICES subareas 27.7 (excluding Division 27.7.d) and 27.6 (hereafter, the “27” area prefixes are omitted).
-Some fisheries statistics do not allow the full differentiation of sections of subareas 4 and 2 or (in earlier years) western
-sections of subareas 6 and 7, as well as the southeastern section of Division 7.e.
-&lt;/p&gt;
-&lt;p&gt;
-(*) Throughout this document ‘Celtic Seas’ refers to the ecoregion and ‘Celtic Sea’ refers to this southern area.
-&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;
 The Faroes ecoregion covers the shelf and surrounding waters inside the Faroe Islands Exclusive Economic Zone (EEZ) (Figure 1). 
 The waters around the Faroe Islands are in the upper 500 m dominated by the North Atlantic Current, which to the north of the 
 islands meets the East Icelandic Current. Clockwise current systems create retention areas on the Faroe Plateau (Faroe Shelf 
@@ -3524,106 +3488,6 @@
 &lt;p&gt;
 Historically, countries other than those bordering the Baltic Sea have made some landings. However, in recent decades
 landings are exclusively from the nine bordering countries.
-&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;
-Fourteen nations currently have fisheries targeting the many marine stocks in the ecoregion. These include (by decreasing
-order of contribution to total landings in the ecoregion): Scotland, Ireland, Denmark, the Netherlands, France, England,
-Germany, Poland, Northern Ireland, Lithuania, Spain, Belgium, Wales, and Sweden.
-&lt;/p&gt;
-&lt;h4&gt;France&lt;/h4&gt;
-&lt;p&gt;
-There were 309 French vessels with landings in the ecoregion. The number of vessels has decreased from 362 in 2021 to
-309 in 2024. The number of French vessels with 80% of their landings in the Celtic Seas ecoregion in 2024 was 94. Of these,
-11 were &amp;lt;12 m, 28 were 12–24 m, 49 were 24–40 m and 6 were &amp;gt; 40 m. The main species landed by volume are hake,
-anglerfish, blue whiting, saithe, and mackerel. In terms of landings value, the main species are anglerfish, hake, saithe, john
-dory, and albacore.
-&lt;/p&gt;
-&lt;h4&gt;Ireland&lt;/h4&gt;
-&lt;p&gt;
-There were 1 287 Irish vessels with landings in the ecoregion. The number of vessels has decreased from 1 313 in 2021 to
-1 287 in 2024. The number of Irish vessels with 80% of their catch in the Celtic Seas ecoregion in 2024 was 1 274. Of these,
-1 078 were &amp;lt;12 m, 118 were 12–24 m, 58 were 24–40 m and 20 were &amp;gt; 40 m. The main species landed by volume are
-mackerel, blue whiting, horse mackerel, sprat, and nephrops. In terms of landings value, the main species are nephrops,
-mackerel, blue whiting, brown crab, and horse mackerel.
-&lt;/p&gt;
-&lt;h4&gt;United Kingdom – Scotland&lt;/h4&gt;
-&lt;p&gt;
-There were 1 026 Scottish vessels with landings in the ecoregion. The number of vessels has decreased from 1 173 in 2021
-to 1 026 in 2024. The number of Scottish vessels with 80% of their catch in the Celtic Seas ecoregion in 2024 was 589. Of
-these, 472 were &amp;lt;12 m, 90 were 12–24 m, 23 were 24–40 m and 4 were &amp;gt; 40 m. The main species landed by volume are
-mackerel, blue whiting, herring, haddock, and Nephrops. In terms of value, the main species are mackerel, Nephrops,
-anglerfish, herring, and haddock.
-&lt;/p&gt;
-&lt;h4&gt;United Kingdom – Northern Ireland&lt;/h4&gt;
-&lt;p&gt;
-There were 180 Northern Ireland vessels with landings in the ecoregion. The number of vessels has decreased from 236 in
-2021 to 180 in 2024. The number of Northern Ireland vessels with 80% of their catch in the Celtic Seas ecoregion in 2024
-was 120. Of these, 63 were &amp;lt;12 m, 52 were 12–24 m, 4 were 24–40 m and 1 was &amp;gt; 40 m. The main species landed by volume
-are mackerel, herring, Nephrops, brown crab, and horse mackerel. In terms of value, the main species are Nephrops,
-mackerel, herring, brown crab, and scallops.
-&lt;/p&gt;
-&lt;h4&gt;United Kingdom – England and Wales&lt;/h4&gt;
-&lt;p&gt;
-There were 860 English vessels with landings in the ecoregion. The number of vessels has decreased from 924 in 2021 to
-860 in 2024. The number of English vessels with 80% of their catch in the Celtic Seas ecoregion in 2024 was 506. Of these,
-384 were &amp;lt;12 m, 88 were 12–24 m, 33 were 24–40 m and 1 was &amp;gt;40 m. The main species landed by volume are mackerel,
-blue whiting, pilchard, anglerfish, and brown crab. In terms of value, the main species are anglerfish, sole, brown crab,
-lobster, and hake.
-&lt;/p&gt;
-&lt;p&gt;
-There were 227 Welsh vessels with landings in the ecoregion. The number of vessels has decreased from 250 in 2021 to 227
-in 2024. The number of Welsh vessels with 80% of their catch in the Celtic Seas ecoregion in 2024 was 165. Of these, 155
-were &amp;lt;12 m, 8 were 12–24 m, 2 were 24–40 m and 0 were &amp;gt; 40 m. The main species landed by volume are whelk, anglerfish,
-scallop, megrim, and brown crab. In terms of value, the main species are whelk, lobster, anglerfish, seabass, and brown crab.
-&lt;/p&gt;
-&lt;h4&gt;Spain&lt;/h4&gt;
-&lt;p&gt;
-There were 146 Spanish vessels with landings in the ecoregion. The number of vessels has increased from 79 in 2021 to 146
-in 2024. The number of Spanish vessels with 80% of their catch in the Celtic Seas ecoregion in 2024 was 32. Of these, 0
-were &amp;lt;12 m, 0 were 12–24 m, 32 were 24–40 m and 0 were &amp;gt; 40 m. The main species landed by volume are hake, megrim,
-ling, blue shark, and witch. In terms of value, the main species are hake, megrim, Nephrops, ling, and greater forkbeard.
-&lt;/p&gt;
-&lt;h4&gt;Other countries&lt;/h4&gt;
-&lt;p&gt;
-About 60 Norwegian vessels operate in this ecoregion. Pelagic trawlers mainly target blue whiting but also target other
-pelagic species. There is also a demersal longline fishery that mainly targets ling and blue ling.
-&lt;/p&gt;
-&lt;p&gt;
-The Belgian fleet consists of about 65 active vessels, of which about 21 operate in the Irish Sea. The majority (89%) of the
-vessels operating in the Irish Sea are between 24 and 40 m, while the remainder are between 18 and 24 m. The Belgian fleet
-uses beam trawls and otter trawls for rays, plaice, sole, and anglerfish.
-&lt;/p&gt;
-&lt;p&gt;
-Seven German vessels operate in the Celtic Seas, one of which takes 80% of their catch in the ecoregion. This includes vessels
-that mainly target anglerfish and hake with gillnets and longline, as well as freezer trawlers that target blue whiting, horse
-mackerel, and mackerel.
-&lt;/p&gt;
-&lt;p&gt;
-One large (&amp;gt; 40 m) Lithuanian freezer trawler targets pelagic species in the ecoregion.
-&lt;/p&gt;
-&lt;p&gt;
-There are 16 large Dutch pelagic freezer trawlers operating in the ecoregion, mainly targeting blue whiting, horse mackerel,
-and mackerel.
-&lt;/p&gt;
-&lt;p&gt;
-The Danish fleet consists of sixteen vessels, one of which has more than 80% of their landings in the Celtic Seas. Blue whiting
-is the main species for the fleet by weight and mackerel is the main species by value.
-&lt;/p&gt;
-&lt;p&gt;
-Vessels from the Faroe Islands also operate in this ecoregion, targeting blue whiting with pelagic trawls.
-&lt;/p&gt;
-&lt;h4&gt;Recreational fisheries&lt;/h4&gt;
-&lt;p&gt;
-Recreational fishing is an important activity in the Celtic Sea that harvests a diverse range of species from a variety of
-platforms (e.g. shore, boat, charters) using many gears (e.g. rod and line, speargun, nets, pots, traps). The main countries with
-recreational fisheries are UK and Ireland, where no licence is required. Angling from shore and boat is the most popular
-method, with a number of charter boats offering trips. Catches can be significant, representing around 46% and 67% of total
-removals of sea bass and pollack, respectively, according to the latest ICES advice. The main target species include mackerel,
-pollack, sea bass, saithe, cod, spurdog (Squalus acanthias), flatfish (plaice, dab, flounder, sole), sea bream, wrasse, and whiting.
-Recreational fisheries data is included in the pollack and seabass stock assessments in the ecoregion. Sharks, skates, rays,
-shellfish, crustaceans, and cephalopods are also caught by recreational fishers.
 &lt;/p&gt;</t>
   </si>
   <si>
@@ -4487,21 +4351,6 @@
   </si>
   <si>
     <t>&lt;ul&gt;
-  &lt;li&gt;Vessel numbers have declined across the majority of the countries fishing in the ecoregion in the past decade.&lt;/li&gt;
-  &lt;li&gt;Total landings fluctuated around 1 million tonnes between 2014 and 2020, and have been lower, at 0.77–0.92 million tonnes, in 2021–2023. Pelagic fisheries continue to dominate landings by volume in the ecoregion.&lt;/li&gt;
-  &lt;li&gt;Discard rates of elasmobranch stocks are high (&amp;gt; 30%) in the ecoregion. Discard rates of other stocks remain stable.&lt;/li&gt;
-  &lt;li&gt;Average fishing mortalities have generally declined since the mid-1990s for stocks within the benthic, demersal and elasmobranch guilds. However, some stocks continue to be fished above FMSY, including mackerel and blue whiting in the pelagic guild.&lt;/li&gt;
-  &lt;li&gt;On average, the spawning stock size in all guilds is currently above the target (SSB/MSY Btrigger &amp;gt; 1), although some of the stocks including mackerel and gadoids in the Celtic Sea (cod, haddock and whiting) remain below target.&lt;/li&gt;
-  &lt;li&gt;Changes in species interactions, diets and fish distributions are affecting stock abundances and fisheries in the Celtic Sea.&lt;/li&gt;
-  &lt;li&gt;&lt;strong&gt;In relation to mixed fisheries:&lt;/strong&gt;&lt;/li&gt;
-  &lt;li&gt;Landings shares for individual stocks are dominated by demersal trawl métiers (demersal fish or Nephrops) and beam trawl métiers (benthic flatfish and skates and rays), though longlines and gillnets have a significant landing share for some stocks in the Celtic Sea (e.g. hake and ling), as do pots in the West of Scotland (Nephrops).&lt;/li&gt;
-  &lt;li&gt;Fleet landings compositions in the Celtic Sea have remained relatively stable since 2015, with some trends over time in some fleets towards dominant stocks. There can be significant differences in landings composition between gear type and country within the same gear type, reflecting different targeting and gear efficiencies.&lt;/li&gt;
-  &lt;li&gt;Annual mixed fisheries forecasts indicate that most fleets are limited by the zero catch advice for cod, haddock and whiting in the Celtic Sea. No forecasts are available for the Irish Sea or the West of Scotland.&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;The fisheries overview document (pdf) is accessible at   &lt;a href="https://doi.org/10.17895/ices.advice.30710879"&gt;ICES Library&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;
 &lt;li&gt;
 Vessel numbers have declined across the majority of the countries fishing in the ecoregion in the past decade.
 &lt;/li&gt;
@@ -4537,6 +4386,113 @@
 &lt;p&gt;
   The fisheries overview document (pdf) is accessible at   &lt;a href="https://doi.org/10.17895/ices.advice.30710897"&gt;ICES Library&lt;/a&gt;
 &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+The Celtic Seas ecoregion covers the northwestern shelf seas of Europe. It includes areas of the deeper eastern Atlantic Ocean and coastal seas that are heavily influenced by oceanic inputs. The ecoregion ranges from north of Shetland to Brittany in the south. Three key areas constitute this ecoregion:
+&lt;/p&gt;
+&lt;ol&gt;
+  &lt;li&gt;
+    northern parts: the Malin shelf, west of Scotland, eastern Rockall Bank, and north of Scotland (parts of Subdivision 2.a.2, divisions 4.a and 6.a, and Subdivision 6.b.2);
+  &lt;/li&gt;
+  &lt;li&gt;
+    the Celtic Sea, Bristol Channel, western English Channel, southwest and west of Ireland (Division 7.b and Subdivision 7.c.2; parts of divisions 7.e, 7.f, 7.g, and 7.h and subdivisions 7.j.2 and 7.k.2);
+  &lt;/li&gt;
+  &lt;li&gt;
+    the Irish Sea (Division 7.a).
+  &lt;/li&gt;
+&lt;/ol&gt;
+&lt;p&gt;
+In the north, there are strong links with the North Sea; in the southeast, a strong link with the English Channel area; and in the south a strong link with the Bay of Biscay. The eastern part of the Rockall Bank is within the geographic scope of the ecoregion, although it is separated from the western European shelf by the Rockall Trough.
+&lt;/p&gt;
+&lt;p&gt;
+The scientific names of all species described in this overview are listed in the Stock Status Lookup.
+&lt;/p&gt;
+&lt;p&gt;
+The overview covers ICES subareas 27.7 (excluding Division 27.7.d) and 27.6 (hereafter, the “27” area prefixes are omitted).
+Some fisheries statistics do not allow the full differentiation of sections of subareas 4 and 2 or (in earlier years) western sections of subareas 6 and 7, as well as the southeastern section of Division 7.e.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Fourteen nations currently have fisheries targeting the many marine stocks in the ecoregion. These include (by decreasing order of contribution to total landings in 2023): UK, Ireland, Norway, Denmark, Netherlands, France, Germany, Poland, Northern Ireland, Lithuania, Spain, Belgium, Wales, and Sweden.  
+&lt;/p&gt;
+&lt;h4&gt;France&lt;/h4&gt;
+&lt;p&gt;
+There were 309 French vessels with landings in the ecoregion in 2024, decreasing from 362 in 2021. The number of vessels with 80% of their landings in the ecoregion in 2024 was 94. Of these, 11 were &amp;lt;12 m, 28 were 12–24 m, 49 were 24–40 m and 6 were &amp;gt; 40 m. The main species landed by volume are hake, anglerfish, blue whiting, saithe, and mackerel. In terms of landings value, the main species are anglerfish, hake, saithe, john
+dory, and albacore.
+&lt;/p&gt;
+&lt;h4&gt;Ireland&lt;/h4&gt;
+&lt;p&gt;
+There were 1 287 Irish vessels with landings in the ecoregion in 2024, decreasing from 1 313 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 1 274. Of these, 1 078 were &amp;lt;12 m, 118 were 12–24 m, 58 were 24–40 m and 20 were &amp;gt; 40 m. The main species landed by volume are mackerel, blue whiting, horse mackerel, sprat, and nephrops. In terms of landings value, the main species are nephrops, mackerel, blue whiting, brown crab, and horse mackerel.
+&lt;/p&gt;
+&lt;h4&gt;United Kingdom – Scotland&lt;/h4&gt;
+&lt;p&gt;
+There were 1 026 Scottish vessels with landings in the ecoregion in 2024, decreasing from 1 173 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 589. Of these, 472 were &amp;lt;12 m, 90 were 12–24 m, 23 were 24–40 m and 4 were &amp;gt; 40 m. The main species landed by volume are mackerel, blue whiting, herring, haddock, and Nephrops. In terms of value, the main species are mackerel, Nephrops,
+anglerfish, herring, and haddock.
+&lt;/p&gt;
+&lt;h4&gt;United Kingdom – Northern Ireland&lt;/h4&gt;
+&lt;p&gt;
+There were 180 Northern Ireland vessels with landings in the ecoregion in 2024, decreasing from 236 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 120. Of these, 63 were &amp;lt;12 m, 52 were 12–24 m, 4 were 24–40 m and 1 was &amp;gt; 40 m. The main species landed by volume are mackerel, herring, Nephrops, brown crab, and horse mackerel. In terms of value, the main species are Nephrops, mackerel, herring, brown crab, and scallops.
+&lt;/p&gt;
+&lt;h4&gt;United Kingdom – England and Wales&lt;/h4&gt;
+&lt;p&gt;
+There were 860 English vessels with landings in the ecoregion in 2024, decreasing from 924 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 506. Of these, 384 were &amp;lt;12 m, 88 were 12–24 m, 33 were 24–40 m and 1 was &amp;gt;40 m. The main species landed by volume are mackerel, blue whiting, pilchard, anglerfish, and brown crab. In terms of value, the main species are anglerfish, sole, brown crab,
+lobster, and hake.
+&lt;/p&gt;
+&lt;p&gt;
+There were 227 Welsh vessels with landings in the ecoregion in 2024, decreasing from 250 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 165. Of these, 155 were &amp;lt;12 m, 8 were 12–24 m, 2 were 24–40 m and 0 were &amp;gt; 40 m. The main species landed by volume are whelk, anglerfish, scallop, megrim, and brown crab. In terms of value, the main species are whelk, lobster, anglerfish, seabass, and brown crab.
+&lt;/p&gt;
+&lt;h4&gt;Spain&lt;/h4&gt;
+&lt;p&gt;
+There were 146 Spanish vessels with landings in the ecoregion in 2024, increasing from 79 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 32. Of these, 0 were &amp;lt;12 m, 0 were 12–24 m, 32 were 24–40 m and 0 were &amp;gt; 40 m. The main species landed by volume are hake, megrim, ling, blue shark, and witch. In terms of value, the main species are hake, megrim, Nephrops, ling, and greater forkbeard.
+&lt;/p&gt;
+&lt;h4&gt;Other countries&lt;/h4&gt;
+&lt;p&gt;
+About 60 Norwegian vessels operate in the ecoregion. Pelagic trawlers mainly target blue whiting but also target other
+pelagic species. There is also a demersal longline fishery that mainly targets ling and blue ling.
+&lt;/p&gt;
+&lt;p&gt;
+The Belgian fleet consists of about 65 active vessels, of which about 21 operate in the Irish Sea. The majority (89%) of those operating in the Irish Sea are between 24 and 40 m, while the remainder are between 18 and 24 m. The Belgian fleet uses beam trawls and otter trawls for rays, plaice, sole, and anglerfish.
+&lt;/p&gt;
+&lt;p&gt;
+Seven German vessels operate in the Celtic Seas, one of which takes 80% of their catch in the ecoregion. This includes vessels that mainly target anglerfish and hake with gillnets and longline, as well as freezer trawlers that target blue whiting, horse
+mackerel, and mackerel.
+&lt;/p&gt;
+&lt;p&gt;
+One large (&amp;gt; 40 m) Lithuanian freezer trawler targets pelagic species.
+&lt;/p&gt;
+&lt;p&gt;
+There are 16 large Dutch pelagic freezer trawlers operating in the ecoregion, mainly targeting blue whiting, horse mackerel,
+and mackerel.
+&lt;/p&gt;
+&lt;p&gt;
+The Danish fleet consists of sixteen vessels, one of which has more than 80% of their landings in the ecoregion. Blue whiting
+is the main species for the fleet by weight and mackerel is the main species by value.
+&lt;/p&gt;
+&lt;p&gt;
+Vessels from the Faroe Islands also operate in this ecoregion, targeting blue whiting with pelagic trawls.
+&lt;/p&gt;
+&lt;h4&gt;Recreational fisheries&lt;/h4&gt;
+&lt;p&gt;
+Recreational fishing is an important activity in the Celtic Sea that harvests a diverse range of species from a variety of platforms (e.g. shore, boat, and charters) using many gears (e.g. rod and line, speargun, nets, pots, and traps). The main countries with recreational fisheries are UK and Ireland, where no licence is required. Angling from shore and boat is the most popular method, with a number of charter boats offering trips. Catches can be significant, representing around 46% and 67% of total removals of sea bass and Pollack, respectively, according to the latest ICES advice. The main target species include mackerel, pollack, sea bass, saithe, cod, spurdog, flatfish (plaice, dab, flounder, and sole), sea bream, wrasse, and whiting. Recreational fisheries data is included in the pollack and sea bass stock assessments in the ecoregion. Sharks, skates, rays, shellfish, crustaceans, and cephalopods are also caught by recreational fishers
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;
+  &lt;li&gt;Vessel numbers have declined across the majority of the countries fishing in the ecoregion in the past decade.&lt;/li&gt;
+  &lt;li&gt;Total landings fluctuated around 1 million tonnes between 2014 and 2020, and have been lower, at 0.77–0.92 million tonnes, in 2021–2023. Pelagic fisheries continue to dominate landings by volume.&lt;/li&gt;
+  &lt;li&gt;Discard rates of elasmobranch stocks are high (&amp;gt; 30%)&lt;/li&gt;
+  &lt;li&gt;Average fishing mortalities have generally declined since the mid-1990s for stocks within the benthic, demersal and elasmobranch guilds.&lt;/li&gt;
+&lt;li&gt; Some stocks continue to be fished above F&lt;sub&gt;MSY&lt;/sub&gt;, including mackerel and blue whiting in the pelagic guild. &lt;/li&gt;
+  &lt;li&gt;On average, the spawning stock size in all guilds is currently above the target (SSB/MSY B&lt;sub&gt;trigger&lt;/sub&gt; &amp;gt; 1), although some of the stocks including gadoids in the Celtic Sea (cod, haddock and whiting) remain below MSY B&lt;sub&gt;trigger&lt;/sub&gt;. The status of mackerel was below MSY B&lt;sub&gt;trigger&lt;/sub&gt; in 2024 and 2025.&lt;/li&gt;
+  &lt;li&gt;Changes in species interactions, diets and fish distributions are affecting stock abundances and fisheries in the Celtic Sea.&lt;/li&gt;
+  &lt;li&gt;In relation to mixed fisheries:&lt;/li&gt;&lt;ul&gt;
+  &lt;li&gt;Landings shares for individual stocks are dominated by demersal trawl métiers (demersal fish or Nephrops) and beam trawl métiers (benthic flatfish and skates and rays), though longlines and gillnets have a significant landing share for some stocks in the Celtic Sea (e.g. hake and ling), as do pots in the West of Scotland (Nephrops).&lt;/li&gt;
+  &lt;li&gt;Fleet landings compositions in the Celtic Sea have remained relatively stable since 2015, with some trends over time in some fleets towards dominant stocks. There can be significant differences in landings composition between gear type and country within the same gear type, reflecting different targeting and gear efficiencies.&lt;/li&gt;
+  &lt;li&gt;Annual mixed fisheries forecasts indicate that most fleets are limited by the zero catch advice for cod, haddock and whiting in the Celtic Sea. No forecasts are available for the Irish Sea or the West of Scotland.&lt;/li&gt;
+&lt;/ul&gt;&lt;/ul&gt;
+&lt;p&gt;The fisheries overview document (pdf) is accessible at   &lt;a href="https://doi.org/10.17895/ices.advice.30710879"&gt;ICES Library&lt;/a&gt;&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -4976,16 +4932,16 @@
       <selection activeCell="A2" sqref="A2:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="168.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="37.7109375" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="168.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37.6640625" customWidth="1"/>
+    <col min="17" max="17" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -4996,7 +4952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>29</v>
       </c>
@@ -5007,7 +4963,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>43</v>
       </c>
@@ -5018,7 +4974,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -5029,7 +4985,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
@@ -5040,7 +4996,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>45</v>
       </c>
@@ -5051,7 +5007,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
@@ -5062,7 +5018,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
@@ -5073,7 +5029,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>25</v>
       </c>
@@ -5084,7 +5040,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>49</v>
       </c>
@@ -5095,7 +5051,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
@@ -5106,7 +5062,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>41</v>
       </c>
@@ -5117,7 +5073,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>23</v>
       </c>
@@ -5128,7 +5084,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>35</v>
       </c>
@@ -5139,7 +5095,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>31</v>
       </c>
@@ -5150,7 +5106,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -5161,7 +5117,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>39</v>
       </c>
@@ -5172,7 +5128,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>33</v>
       </c>
@@ -5183,7 +5139,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>37</v>
       </c>
@@ -5194,7 +5150,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>47</v>
       </c>
@@ -5205,7 +5161,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>66</v>
       </c>
@@ -5216,7 +5172,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>69</v>
       </c>
@@ -5227,7 +5183,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>72</v>
       </c>
@@ -5238,7 +5194,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>75</v>
       </c>
@@ -5249,7 +5205,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>78</v>
       </c>
@@ -5260,7 +5216,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>81</v>
       </c>
@@ -5271,7 +5227,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>84</v>
       </c>
@@ -5282,7 +5238,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>87</v>
       </c>
@@ -5293,7 +5249,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>90</v>
       </c>
@@ -5304,7 +5260,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>93</v>
       </c>
@@ -5315,7 +5271,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>96</v>
       </c>
@@ -5326,7 +5282,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>99</v>
       </c>
@@ -5337,7 +5293,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>102</v>
       </c>
@@ -5348,7 +5304,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>105</v>
       </c>
@@ -5359,7 +5315,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>108</v>
       </c>
@@ -5370,7 +5326,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>111</v>
       </c>
@@ -5381,7 +5337,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>114</v>
       </c>
@@ -5392,7 +5348,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>117</v>
       </c>
@@ -5403,7 +5359,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>120</v>
       </c>
@@ -5414,7 +5370,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>123</v>
       </c>
@@ -5425,7 +5381,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>126</v>
       </c>
@@ -5436,7 +5392,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>129</v>
       </c>
@@ -5447,7 +5403,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>132</v>
       </c>
@@ -5458,7 +5414,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>135</v>
       </c>
@@ -5469,7 +5425,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>138</v>
       </c>
@@ -5480,7 +5436,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>141</v>
       </c>
@@ -5491,7 +5447,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>144</v>
       </c>
@@ -5502,7 +5458,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>147</v>
       </c>
@@ -5513,7 +5469,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>150</v>
       </c>
@@ -5524,7 +5480,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>153</v>
       </c>
@@ -5535,7 +5491,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>156</v>
       </c>
@@ -5546,7 +5502,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>159</v>
       </c>
@@ -5557,7 +5513,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>162</v>
       </c>
@@ -5568,7 +5524,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>165</v>
       </c>
@@ -5579,7 +5535,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>168</v>
       </c>
@@ -5590,7 +5546,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>171</v>
       </c>
@@ -5601,7 +5557,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>174</v>
       </c>
@@ -5612,7 +5568,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>177</v>
       </c>
@@ -5623,7 +5579,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>180</v>
       </c>
@@ -5634,7 +5590,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>183</v>
       </c>
@@ -5645,7 +5601,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>186</v>
       </c>
@@ -5656,7 +5612,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>189</v>
       </c>
@@ -5667,7 +5623,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>192</v>
       </c>
@@ -5678,7 +5634,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>195</v>
       </c>
@@ -5689,7 +5645,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>198</v>
       </c>
@@ -5700,7 +5656,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
         <v>201</v>
       </c>
@@ -5711,7 +5667,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="s">
         <v>204</v>
       </c>
@@ -5722,7 +5678,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
         <v>207</v>
       </c>
@@ -5733,7 +5689,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="s">
         <v>210</v>
       </c>
@@ -5744,7 +5700,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="10" t="s">
         <v>213</v>
       </c>
@@ -5755,7 +5711,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="s">
         <v>216</v>
       </c>
@@ -5766,7 +5722,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
         <v>219</v>
       </c>
@@ -5777,7 +5733,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="s">
         <v>222</v>
       </c>
@@ -5788,7 +5744,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
         <v>225</v>
       </c>
@@ -5799,7 +5755,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
         <v>228</v>
       </c>
@@ -5810,7 +5766,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="s">
         <v>231</v>
       </c>
@@ -5821,7 +5777,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="10" t="s">
         <v>234</v>
       </c>
@@ -5832,7 +5788,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="10" t="s">
         <v>237</v>
       </c>
@@ -5843,7 +5799,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="s">
         <v>240</v>
       </c>
@@ -5854,7 +5810,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="s">
         <v>243</v>
       </c>
@@ -5865,7 +5821,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="10" t="s">
         <v>246</v>
       </c>
@@ -5876,7 +5832,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="10" t="s">
         <v>249</v>
       </c>
@@ -5887,7 +5843,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="10" t="s">
         <v>252</v>
       </c>
@@ -5898,7 +5854,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="10" t="s">
         <v>255</v>
       </c>
@@ -5909,7 +5865,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="10" t="s">
         <v>258</v>
       </c>
@@ -5920,7 +5876,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="10" t="s">
         <v>261</v>
       </c>
@@ -5931,7 +5887,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="10" t="s">
         <v>264</v>
       </c>
@@ -5942,7 +5898,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="10" t="s">
         <v>267</v>
       </c>
@@ -5953,7 +5909,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="10" t="s">
         <v>270</v>
       </c>
@@ -5964,7 +5920,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="10" t="s">
         <v>273</v>
       </c>
@@ -5975,7 +5931,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="10" t="s">
         <v>276</v>
       </c>
@@ -5986,7 +5942,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
         <v>279</v>
       </c>
@@ -5997,7 +5953,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="10" t="s">
         <v>282</v>
       </c>
@@ -6008,7 +5964,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="10" t="s">
         <v>285</v>
       </c>
@@ -6019,7 +5975,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="10" t="s">
         <v>288</v>
       </c>
@@ -6030,7 +5986,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="10" t="s">
         <v>291</v>
       </c>
@@ -6041,7 +5997,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="10" t="s">
         <v>294</v>
       </c>
@@ -6052,7 +6008,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="10" t="s">
         <v>297</v>
       </c>
@@ -6063,7 +6019,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="10" t="s">
         <v>300</v>
       </c>
@@ -6074,7 +6030,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="10" t="s">
         <v>303</v>
       </c>
@@ -6085,7 +6041,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="10" t="s">
         <v>306</v>
       </c>
@@ -6096,7 +6052,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="10" t="s">
         <v>309</v>
       </c>
@@ -6107,7 +6063,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="10" t="s">
         <v>312</v>
       </c>
@@ -6118,7 +6074,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="10" t="s">
         <v>315</v>
       </c>
@@ -6129,7 +6085,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="10" t="s">
         <v>318</v>
       </c>
@@ -6140,7 +6096,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="10" t="s">
         <v>321</v>
       </c>
@@ -6151,7 +6107,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="10" t="s">
         <v>324</v>
       </c>
@@ -6162,7 +6118,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="10" t="s">
         <v>327</v>
       </c>
@@ -6173,7 +6129,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="10" t="s">
         <v>330</v>
       </c>
@@ -6184,7 +6140,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="10" t="s">
         <v>333</v>
       </c>
@@ -6195,7 +6151,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="10" t="s">
         <v>336</v>
       </c>
@@ -6206,7 +6162,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="10" t="s">
         <v>339</v>
       </c>
@@ -6217,7 +6173,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="10" t="s">
         <v>342</v>
       </c>
@@ -6228,7 +6184,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="10" t="s">
         <v>345</v>
       </c>
@@ -6239,7 +6195,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="10" t="s">
         <v>348</v>
       </c>
@@ -6250,7 +6206,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="10" t="s">
         <v>351</v>
       </c>
@@ -6261,7 +6217,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="10" t="s">
         <v>354</v>
       </c>
@@ -6272,7 +6228,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="10" t="s">
         <v>357</v>
       </c>
@@ -6283,7 +6239,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="10" t="s">
         <v>360</v>
       </c>
@@ -6294,7 +6250,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="10" t="s">
         <v>363</v>
       </c>
@@ -6305,7 +6261,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="10" t="s">
         <v>366</v>
       </c>
@@ -6316,7 +6272,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="10" t="s">
         <v>369</v>
       </c>
@@ -6327,7 +6283,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="10" t="s">
         <v>372</v>
       </c>
@@ -6338,7 +6294,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="10" t="s">
         <v>375</v>
       </c>
@@ -6349,7 +6305,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="10" t="s">
         <v>378</v>
       </c>
@@ -6360,7 +6316,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="10" t="s">
         <v>381</v>
       </c>
@@ -6371,7 +6327,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="10" t="s">
         <v>384</v>
       </c>
@@ -6382,7 +6338,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="10" t="s">
         <v>387</v>
       </c>
@@ -6393,7 +6349,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="10" t="s">
         <v>390</v>
       </c>
@@ -6404,7 +6360,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="10" t="s">
         <v>393</v>
       </c>
@@ -6415,7 +6371,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="10" t="s">
         <v>396</v>
       </c>
@@ -6426,7 +6382,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="10" t="s">
         <v>399</v>
       </c>
@@ -6437,7 +6393,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="10" t="s">
         <v>402</v>
       </c>
@@ -6448,7 +6404,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="10" t="s">
         <v>405</v>
       </c>
@@ -6459,7 +6415,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="10" t="s">
         <v>408</v>
       </c>
@@ -6470,7 +6426,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="10" t="s">
         <v>411</v>
       </c>
@@ -6481,7 +6437,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="10" t="s">
         <v>414</v>
       </c>
@@ -6492,7 +6448,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="10" t="s">
         <v>417</v>
       </c>
@@ -6503,7 +6459,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="10" t="s">
         <v>420</v>
       </c>
@@ -6514,7 +6470,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="10" t="s">
         <v>423</v>
       </c>
@@ -6525,7 +6481,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="10" t="s">
         <v>426</v>
       </c>
@@ -6536,7 +6492,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="10" t="s">
         <v>429</v>
       </c>
@@ -6547,7 +6503,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="10" t="s">
         <v>432</v>
       </c>
@@ -6558,7 +6514,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="10" t="s">
         <v>435</v>
       </c>
@@ -6569,7 +6525,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="10" t="s">
         <v>438</v>
       </c>
@@ -6580,7 +6536,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="10" t="s">
         <v>441</v>
       </c>
@@ -6591,7 +6547,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="10" t="s">
         <v>444</v>
       </c>
@@ -6602,7 +6558,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="10" t="s">
         <v>447</v>
       </c>
@@ -6613,7 +6569,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="10" t="s">
         <v>450</v>
       </c>
@@ -6624,7 +6580,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="10" t="s">
         <v>453</v>
       </c>
@@ -6635,7 +6591,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="10" t="s">
         <v>456</v>
       </c>
@@ -6646,7 +6602,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="10" t="s">
         <v>459</v>
       </c>
@@ -6657,7 +6613,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="10" t="s">
         <v>462</v>
       </c>
@@ -6668,7 +6624,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="10" t="s">
         <v>465</v>
       </c>
@@ -6679,7 +6635,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="10" t="s">
         <v>468</v>
       </c>
@@ -6690,7 +6646,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="10" t="s">
         <v>471</v>
       </c>
@@ -6701,7 +6657,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="10" t="s">
         <v>474</v>
       </c>
@@ -6712,7 +6668,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="10" t="s">
         <v>477</v>
       </c>
@@ -6723,7 +6679,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="10" t="s">
         <v>480</v>
       </c>
@@ -6734,7 +6690,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="10" t="s">
         <v>483</v>
       </c>
@@ -6745,7 +6701,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="10" t="s">
         <v>486</v>
       </c>
@@ -6756,7 +6712,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="10" t="s">
         <v>489</v>
       </c>
@@ -6767,7 +6723,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="10" t="s">
         <v>492</v>
       </c>
@@ -6778,7 +6734,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="10" t="s">
         <v>495</v>
       </c>
@@ -6789,7 +6745,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="10" t="s">
         <v>498</v>
       </c>
@@ -6800,7 +6756,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="10" t="s">
         <v>501</v>
       </c>
@@ -6811,7 +6767,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="10" t="s">
         <v>504</v>
       </c>
@@ -6822,7 +6778,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="10" t="s">
         <v>507</v>
       </c>
@@ -6833,7 +6789,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="10" t="s">
         <v>510</v>
       </c>
@@ -6844,7 +6800,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="10" t="s">
         <v>513</v>
       </c>
@@ -6855,7 +6811,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="10" t="s">
         <v>516</v>
       </c>
@@ -6866,7 +6822,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="10" t="s">
         <v>519</v>
       </c>
@@ -6877,7 +6833,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="10" t="s">
         <v>522</v>
       </c>
@@ -6888,7 +6844,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="10" t="s">
         <v>525</v>
       </c>
@@ -6899,7 +6855,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="10" t="s">
         <v>528</v>
       </c>
@@ -6910,7 +6866,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="10" t="s">
         <v>531</v>
       </c>
@@ -6921,7 +6877,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="10" t="s">
         <v>534</v>
       </c>
@@ -6932,7 +6888,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="10" t="s">
         <v>537</v>
       </c>
@@ -6943,7 +6899,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="10" t="s">
         <v>540</v>
       </c>
@@ -6954,7 +6910,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="10" t="s">
         <v>543</v>
       </c>
@@ -6965,7 +6921,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="10" t="s">
         <v>546</v>
       </c>
@@ -6976,7 +6932,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="10" t="s">
         <v>549</v>
       </c>
@@ -6987,7 +6943,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="10" t="s">
         <v>552</v>
       </c>
@@ -6998,7 +6954,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="10" t="s">
         <v>555</v>
       </c>
@@ -7009,7 +6965,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="10" t="s">
         <v>558</v>
       </c>
@@ -7020,7 +6976,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="10" t="s">
         <v>561</v>
       </c>
@@ -7031,7 +6987,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="10" t="s">
         <v>564</v>
       </c>
@@ -7042,7 +6998,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="10" t="s">
         <v>567</v>
       </c>
@@ -7053,7 +7009,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="10" t="s">
         <v>570</v>
       </c>
@@ -7064,7 +7020,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" s="10" t="s">
         <v>573</v>
       </c>
@@ -7075,7 +7031,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="10" t="s">
         <v>576</v>
       </c>
@@ -7086,7 +7042,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="10" t="s">
         <v>579</v>
       </c>
@@ -7097,7 +7053,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="10" t="s">
         <v>582</v>
       </c>
@@ -7108,7 +7064,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="10" t="s">
         <v>585</v>
       </c>
@@ -7119,7 +7075,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="10" t="s">
         <v>588</v>
       </c>
@@ -7130,7 +7086,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="10" t="s">
         <v>591</v>
       </c>
@@ -7141,7 +7097,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="10" t="s">
         <v>594</v>
       </c>
@@ -7152,7 +7108,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="10" t="s">
         <v>597</v>
       </c>
@@ -7163,7 +7119,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="10" t="s">
         <v>600</v>
       </c>
@@ -7174,7 +7130,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="10" t="s">
         <v>603</v>
       </c>
@@ -7185,7 +7141,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="10" t="s">
         <v>606</v>
       </c>
@@ -7196,7 +7152,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="10" t="s">
         <v>609</v>
       </c>
@@ -7207,7 +7163,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="10" t="s">
         <v>612</v>
       </c>
@@ -7218,7 +7174,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="10" t="s">
         <v>615</v>
       </c>
@@ -7229,7 +7185,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="10" t="s">
         <v>618</v>
       </c>
@@ -7240,7 +7196,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="10" t="s">
         <v>621</v>
       </c>
@@ -7251,7 +7207,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="10" t="s">
         <v>624</v>
       </c>
@@ -7262,7 +7218,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" s="10" t="s">
         <v>627</v>
       </c>
@@ -7273,7 +7229,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" s="10" t="s">
         <v>630</v>
       </c>
@@ -7284,7 +7240,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="10" t="s">
         <v>633</v>
       </c>
@@ -7295,7 +7251,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="10" t="s">
         <v>636</v>
       </c>
@@ -7306,7 +7262,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="10" t="s">
         <v>639</v>
       </c>
@@ -7317,7 +7273,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="10" t="s">
         <v>642</v>
       </c>
@@ -7328,7 +7284,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="10" t="s">
         <v>645</v>
       </c>
@@ -7339,7 +7295,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="10" t="s">
         <v>648</v>
       </c>
@@ -7350,7 +7306,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="10" t="s">
         <v>651</v>
       </c>
@@ -7361,7 +7317,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="10" t="s">
         <v>654</v>
       </c>
@@ -7372,7 +7328,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="10" t="s">
         <v>657</v>
       </c>
@@ -7383,7 +7339,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="10" t="s">
         <v>660</v>
       </c>
@@ -7394,7 +7350,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="10" t="s">
         <v>663</v>
       </c>
@@ -7405,7 +7361,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" s="10" t="s">
         <v>666</v>
       </c>
@@ -7416,7 +7372,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="10" t="s">
         <v>669</v>
       </c>
@@ -7427,7 +7383,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" s="10" t="s">
         <v>672</v>
       </c>
@@ -7438,7 +7394,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" s="10" t="s">
         <v>675</v>
       </c>
@@ -7449,7 +7405,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" s="10" t="s">
         <v>678</v>
       </c>
@@ -7460,7 +7416,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="10" t="s">
         <v>681</v>
       </c>
@@ -7471,7 +7427,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="10" t="s">
         <v>684</v>
       </c>
@@ -7482,7 +7438,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="10" t="s">
         <v>687</v>
       </c>
@@ -7493,7 +7449,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="10" t="s">
         <v>690</v>
       </c>
@@ -7504,7 +7460,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="10" t="s">
         <v>693</v>
       </c>
@@ -7515,7 +7471,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="10" t="s">
         <v>696</v>
       </c>
@@ -7526,7 +7482,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="10" t="s">
         <v>699</v>
       </c>
@@ -7537,7 +7493,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="10" t="s">
         <v>702</v>
       </c>
@@ -7548,7 +7504,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="10" t="s">
         <v>705</v>
       </c>
@@ -7559,7 +7515,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="10" t="s">
         <v>708</v>
       </c>
@@ -7570,7 +7526,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="10" t="s">
         <v>711</v>
       </c>
@@ -7581,7 +7537,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="10" t="s">
         <v>714</v>
       </c>
@@ -7592,7 +7548,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="10" t="s">
         <v>717</v>
       </c>
@@ -7603,7 +7559,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="10" t="s">
         <v>720</v>
       </c>
@@ -7614,7 +7570,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="10" t="s">
         <v>723</v>
       </c>
@@ -7625,7 +7581,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" s="10" t="s">
         <v>726</v>
       </c>
@@ -7636,7 +7592,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" s="10" t="s">
         <v>729</v>
       </c>
@@ -7647,7 +7603,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" s="10" t="s">
         <v>732</v>
       </c>
@@ -7658,7 +7614,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" s="10" t="s">
         <v>735</v>
       </c>
@@ -7669,7 +7625,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" s="10" t="s">
         <v>738</v>
       </c>
@@ -7680,7 +7636,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" s="10" t="s">
         <v>741</v>
       </c>
@@ -7691,7 +7647,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" s="10" t="s">
         <v>744</v>
       </c>
@@ -7702,7 +7658,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" s="10" t="s">
         <v>747</v>
       </c>
@@ -7713,7 +7669,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" s="10" t="s">
         <v>750</v>
       </c>
@@ -7724,7 +7680,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" s="10" t="s">
         <v>753</v>
       </c>
@@ -7735,7 +7691,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" s="10" t="s">
         <v>756</v>
       </c>
@@ -7746,7 +7702,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" s="10" t="s">
         <v>759</v>
       </c>
@@ -7757,7 +7713,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" s="10" t="s">
         <v>762</v>
       </c>
@@ -7768,7 +7724,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" s="10" t="s">
         <v>765</v>
       </c>
@@ -7779,7 +7735,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" s="10" t="s">
         <v>768</v>
       </c>
@@ -7790,7 +7746,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" s="10" t="s">
         <v>771</v>
       </c>
@@ -7801,7 +7757,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" s="10" t="s">
         <v>774</v>
       </c>
@@ -7812,7 +7768,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" s="10" t="s">
         <v>777</v>
       </c>
@@ -7823,7 +7779,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" s="10" t="s">
         <v>780</v>
       </c>
@@ -7834,7 +7790,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" s="10" t="s">
         <v>783</v>
       </c>
@@ -7845,7 +7801,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" s="10" t="s">
         <v>786</v>
       </c>
@@ -7856,7 +7812,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" s="10" t="s">
         <v>789</v>
       </c>
@@ -7867,7 +7823,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" s="10" t="s">
         <v>792</v>
       </c>
@@ -7878,7 +7834,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" s="10" t="s">
         <v>795</v>
       </c>
@@ -7889,7 +7845,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" s="10" t="s">
         <v>798</v>
       </c>
@@ -7900,7 +7856,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" s="10" t="s">
         <v>801</v>
       </c>
@@ -7911,7 +7867,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" s="10" t="s">
         <v>804</v>
       </c>
@@ -7922,7 +7878,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" s="10" t="s">
         <v>807</v>
       </c>
@@ -7933,7 +7889,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" s="10" t="s">
         <v>810</v>
       </c>
@@ -7944,7 +7900,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" s="10" t="s">
         <v>813</v>
       </c>
@@ -7955,7 +7911,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" s="10" t="s">
         <v>816</v>
       </c>
@@ -7966,7 +7922,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" s="10" t="s">
         <v>819</v>
       </c>
@@ -7977,7 +7933,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" s="10" t="s">
         <v>822</v>
       </c>
@@ -7988,7 +7944,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" s="10" t="s">
         <v>825</v>
       </c>
@@ -7999,7 +7955,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" s="10" t="s">
         <v>828</v>
       </c>
@@ -8010,7 +7966,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" s="10" t="s">
         <v>831</v>
       </c>
@@ -8021,7 +7977,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" s="10" t="s">
         <v>834</v>
       </c>
@@ -8032,7 +7988,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" s="10" t="s">
         <v>837</v>
       </c>
@@ -8043,7 +7999,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" s="10" t="s">
         <v>840</v>
       </c>
@@ -8054,7 +8010,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" s="10" t="s">
         <v>843</v>
       </c>
@@ -8065,7 +8021,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" s="10" t="s">
         <v>846</v>
       </c>
@@ -8076,7 +8032,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" s="10" t="s">
         <v>849</v>
       </c>
@@ -8087,7 +8043,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" s="10" t="s">
         <v>852</v>
       </c>
@@ -8098,7 +8054,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" s="10" t="s">
         <v>855</v>
       </c>
@@ -8109,7 +8065,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" s="10" t="s">
         <v>858</v>
       </c>
@@ -8120,7 +8076,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286" s="10" t="s">
         <v>861</v>
       </c>
@@ -8131,7 +8087,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" s="10" t="s">
         <v>864</v>
       </c>
@@ -8142,7 +8098,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" s="10" t="s">
         <v>867</v>
       </c>
@@ -8153,7 +8109,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289" s="10" t="s">
         <v>870</v>
       </c>
@@ -8164,7 +8120,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290" s="10" t="s">
         <v>873</v>
       </c>
@@ -8175,7 +8131,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291" s="10" t="s">
         <v>876</v>
       </c>
@@ -8186,7 +8142,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292" s="10" t="s">
         <v>879</v>
       </c>
@@ -8215,17 +8171,17 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="255.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8233,28 +8189,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="303" customHeight="1" x14ac:dyDescent="0.25">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="303" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
   </sheetData>
@@ -8273,13 +8229,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="198.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="198.33203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8287,15 +8243,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="343.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="343.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -8303,12 +8259,12 @@
         <v>886</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
   </sheetData>
@@ -8324,13 +8280,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="229.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="229.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8338,28 +8294,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
   </sheetData>
@@ -8375,13 +8331,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8389,20 +8345,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="328.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="328.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -8418,13 +8374,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8432,20 +8388,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="286.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="286.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -8461,13 +8417,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8475,20 +8431,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="288" customHeight="1" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="288" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -8504,13 +8460,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8518,20 +8474,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="294" customHeight="1" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="294" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -8547,12 +8503,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="125.5703125" customWidth="1"/>
+    <col min="2" max="2" width="125.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8560,20 +8516,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
   </sheetData>
@@ -8589,13 +8545,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8603,20 +8559,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="260.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="260.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -8632,13 +8588,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8646,20 +8602,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="308.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="308.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -8675,13 +8631,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="152.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="152.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8689,15 +8645,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="258.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="258.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -8705,7 +8661,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -8726,13 +8682,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8740,20 +8696,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="348" customHeight="1" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="348" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -8772,13 +8728,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8786,20 +8742,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="244.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="244.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -8815,13 +8771,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8829,20 +8785,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="243.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -8858,13 +8814,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8872,20 +8828,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="210.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="276" customHeight="1" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="276" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -8902,13 +8858,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="199.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="199.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8916,33 +8872,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>884</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>907</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>908</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>909</v>
       </c>
     </row>
   </sheetData>
@@ -8959,13 +8915,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="199.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="199.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8973,33 +8929,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>884</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>907</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>908</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>909</v>
       </c>
     </row>
   </sheetData>
@@ -9015,13 +8971,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="199.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="199.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9029,33 +8985,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>884</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>907</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>908</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>909</v>
       </c>
     </row>
   </sheetData>
@@ -9071,13 +9027,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="199.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="199.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9085,33 +9041,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>884</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>907</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>908</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>909</v>
       </c>
     </row>
   </sheetData>
@@ -9130,13 +9086,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="199.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="199.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9144,33 +9100,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>884</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="315" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>907</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>908</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>909</v>
       </c>
     </row>
   </sheetData>
@@ -9186,13 +9142,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="199.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="199.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9200,33 +9156,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>884</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>907</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>908</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>909</v>
       </c>
     </row>
   </sheetData>
@@ -9242,13 +9198,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="253.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="253.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9256,15 +9212,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="279" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="279" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -9272,12 +9228,12 @@
         <v>888</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
   </sheetData>
@@ -9293,13 +9249,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="199.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="199.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9307,33 +9263,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>884</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>907</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>908</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>909</v>
       </c>
     </row>
   </sheetData>
@@ -9349,13 +9305,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="199.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="199.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9363,33 +9319,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>884</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>907</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>908</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>909</v>
       </c>
     </row>
   </sheetData>
@@ -9405,13 +9361,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="199.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="199.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9419,33 +9375,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>884</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>907</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>908</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>909</v>
       </c>
     </row>
   </sheetData>
@@ -9461,13 +9417,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="199.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="199.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9475,33 +9431,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>884</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>907</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>908</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>909</v>
       </c>
     </row>
   </sheetData>
@@ -9517,13 +9473,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="199.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="199.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9531,33 +9487,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>884</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>905</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>907</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>908</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>909</v>
       </c>
     </row>
   </sheetData>
@@ -9574,12 +9530,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9587,7 +9543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -9609,12 +9565,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9622,7 +9578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -9644,13 +9600,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="159.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="159.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9658,7 +9614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -9679,13 +9635,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="223.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="223.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9693,15 +9649,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -9709,12 +9665,12 @@
         <v>889</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
   </sheetData>
@@ -9730,13 +9686,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="181.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="181.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9744,15 +9700,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -9760,12 +9716,12 @@
         <v>890</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
   </sheetData>
@@ -9777,17 +9733,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB1D8E1-BE83-467E-ABE2-EB20A46DABB5}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="222.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="222.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9795,28 +9751,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>900</v>
+        <v>927</v>
       </c>
     </row>
   </sheetData>
@@ -9832,13 +9788,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="137.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="137.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9846,37 +9802,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="393.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="390" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" s="6"/>
     </row>
   </sheetData>
@@ -9892,13 +9848,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="135.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="135.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9906,28 +9862,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
   </sheetData>
@@ -9943,13 +9899,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="114.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="114.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9957,7 +9913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>882</v>
       </c>
@@ -9965,20 +9921,20 @@
         <v>883</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated excel file with generic descriptions; modified mod_vms to account for text; added links to vms inventory
</commit_message>
<xml_diff>
--- a/data-raw/texts.xlsx
+++ b/data-raw/texts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_2023\fisheriesXplorer\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E044A1-E485-4141-A302-B20CAAACF0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A829B5C2-27E4-4438-97AD-536DFD91552E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26160" yWindow="1440" windowWidth="47880" windowHeight="12996" tabRatio="826" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="826" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="glossary" sheetId="17" r:id="rId1"/>
@@ -47,9 +47,19 @@
     <sheet name="status_NrS" sheetId="35" r:id="rId32"/>
     <sheet name="status_NwS" sheetId="36" r:id="rId33"/>
     <sheet name="status_ONA" sheetId="37" r:id="rId34"/>
-    <sheet name="mixfish" sheetId="5" r:id="rId35"/>
-    <sheet name="vms" sheetId="6" r:id="rId36"/>
-    <sheet name="bycatch" sheetId="7" r:id="rId37"/>
+    <sheet name="vms_AZ" sheetId="6" r:id="rId35"/>
+    <sheet name="vms_BI" sheetId="38" r:id="rId36"/>
+    <sheet name="vms_BrS" sheetId="39" r:id="rId37"/>
+    <sheet name="vms_BtS" sheetId="40" r:id="rId38"/>
+    <sheet name="vms_CS" sheetId="41" r:id="rId39"/>
+    <sheet name="vms_FO" sheetId="42" r:id="rId40"/>
+    <sheet name="vms_IS" sheetId="43" r:id="rId41"/>
+    <sheet name="vms_GS" sheetId="44" r:id="rId42"/>
+    <sheet name="vms_NrS" sheetId="45" r:id="rId43"/>
+    <sheet name="vms_NwS" sheetId="46" r:id="rId44"/>
+    <sheet name="vms_ONA" sheetId="47" r:id="rId45"/>
+    <sheet name="mixfish" sheetId="5" r:id="rId46"/>
+    <sheet name="bycatch" sheetId="7" r:id="rId47"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -72,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="931">
   <si>
     <t>section</t>
   </si>
@@ -4155,6 +4165,152 @@
 &lt;p&gt;Elasmobranch discard data might be highly uncertain, precaution is advised when interpreting the results.&lt;/p&gt;</t>
   </si>
   <si>
+    <t>&lt;h4&gt;Discard trends&lt;/h4&gt;
+&lt;p&gt;
+Discard trends by fish fisheries guild shown as percentages (%) of the total annual catch in that
+category. 
+Some catches may occur outside the ecoregion and not all stock catches are disaggregated between landings
+and discards.
+&lt;/p&gt;
+&lt;h4&gt;Current discards&lt;/h4&gt;
+&lt;p&gt;
+Left/top panel: landings (green) and discards (orange) by fisheries guild
+(in thousand tonnes) only of the stocks with recorded discards. 
+Right/bottom panel: landings (green) and discards (orange) by fisheries guild (in thousand tonnes) of all
+stocks that have some catches in the ecoregion.
+&lt;/p&gt;
+&lt;p&gt;Elasmobranch discard data might be highly uncertain, precaution is advised when interpreting the results.&lt;/p&gt;
+&lt;h4&gt;Results description&lt;/h4&gt;
+&lt;p&gt;The average discard rate among pelagic stocks is estimated to be very low. &lt;/p&gt;
+&lt;p&gt;The estimated average discard rate for elasmobranchs stocks is high and ranges 30% to 75%. &lt;/p&gt;
+&lt;p&gt;The average discard rate among demersal stocks ranges from 9% to 22% and is generally around 15%. &lt;/p&gt;
+&lt;p&gt;Crustacean and benthic stocks have an estimated average discard rate of around 10%. &lt;/p&gt;
+&lt;p&gt;Discard rates for some species are very high in the ecoregion, for example plaice (around 60% of tonnage) and whiting (50–99% of tonnage).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;
+  &lt;li&gt;Fisheries management measures for major stocks (e.g. cod, haddock, saithe, and herring) have resulted in decreased fishing pressure – close to or at F&lt;sub&gt;MSY&lt;/sub&gt; or HR&lt;sub&gt;MSY&lt;/sub&gt; – and increased SSBs for the past two decades.&lt;/li&gt;
+  &lt;li&gt;There has been an overall reduction in fishing effort since 1991 for all fisheries – except those using handlines, where it has increased. The decrease in trawl effort is likely to have reduced pressure on benthic habitats.&lt;/li&gt;
+  &lt;li&gt;Three pelagic fisheries have seen increased effort and landings due to changes in migration patterns linked to prey availability, oceanographic conditions, and stock abundance: a blue whiting fishery (starting in the late 1990s), the Atlantic mackerel fishery (commencing mid-2000s), and the Norwegian spring-spawning herring fishery (recommencing at the turn of the century).&lt;/li&gt;
+  &lt;li&gt;Fishing grounds of several species (e.g. haddock, anglerfish, ling, lemon sole, and witch) have expanded to the northern part of the ecoregion due to species redistribution associated with increased water temperature.&lt;/li&gt;
+  &lt;li&gt;Several species—including Atlantic halibut, spotted wolfish, Norway lobster, and northern shrimp—have shown substantial decreases in stock sizes due to factors such as high fishing pressure and reduced productivity. Directed fisheries for Atlantic halibut and Norway lobster are currently prohibited.&lt;/li&gt;
+  &lt;li&gt;Legislation to recommence hunting of fin and minke whales was passed in 2009. However, catches are not made every year.&lt;/li&gt;
+  &lt;li&gt;The highest cumulative multiannual bycatch rate of protected, endangered, and threatened species was recorded in set gillnets. At species level, the highest seabird bycatch rates were for guillemot and common eider, and the highest marine mammal bycatch rates for harbour porpoise and harbour seal. The estimated annual seabird bycatch in the gillnet lumpfish fishery has decreased in recent years, though the driver is unclear.&lt;/li&gt;
+  &lt;li&gt;The summer feeding grounds of capelin have shifted from the Icelandic Waters ecoregion to the Greenland Sea ecoregion. While this does not directly affect the Icelandic winter capelin fishery, it may indirectly influence the distribution and growth of predator stocks on which other fisheries depend.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;
+  The fisheries overview document (pdf) is accessible at:  
+  &lt;a href="https://doi.org/10.17895/ices.advice.27879909" target="_blank"&gt;ICES Library&lt;/a&gt;
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+The Celtic Seas ecoregion covers the northwestern shelf seas of Europe. It includes areas of the deeper eastern Atlantic Ocean and coastal seas that are heavily influenced by oceanic inputs. The ecoregion ranges from north of Shetland to Brittany in the south. Three key areas constitute this ecoregion:
+&lt;/p&gt;
+&lt;ol&gt;
+  &lt;li&gt;
+    northern parts: the Malin shelf, west of Scotland, eastern Rockall Bank, and north of Scotland (parts of Subdivision 2.a.2, divisions 4.a and 6.a, and Subdivision 6.b.2);
+  &lt;/li&gt;
+  &lt;li&gt;
+    the Celtic Sea, Bristol Channel, western English Channel, southwest and west of Ireland (Division 7.b and Subdivision 7.c.2; parts of divisions 7.e, 7.f, 7.g, and 7.h and subdivisions 7.j.2 and 7.k.2);
+  &lt;/li&gt;
+  &lt;li&gt;
+    the Irish Sea (Division 7.a).
+  &lt;/li&gt;
+&lt;/ol&gt;
+&lt;p&gt;
+In the north, there are strong links with the North Sea; in the southeast, a strong link with the English Channel area; and in the south a strong link with the Bay of Biscay. The eastern part of the Rockall Bank is within the geographic scope of the ecoregion, although it is separated from the western European shelf by the Rockall Trough.
+&lt;/p&gt;
+&lt;p&gt;
+The scientific names of all species described in this overview are listed in the Stock Status Lookup.
+&lt;/p&gt;
+&lt;p&gt;
+The overview covers ICES subareas 27.7 (excluding Division 27.7.d) and 27.6 (hereafter, the “27” area prefixes are omitted).
+Some fisheries statistics do not allow the full differentiation of sections of subareas 4 and 2 or (in earlier years) western sections of subareas 6 and 7, as well as the southeastern section of Division 7.e.
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+Fourteen nations currently have fisheries targeting the many marine stocks in the ecoregion. These include (by decreasing order of contribution to total landings in 2023): UK, Ireland, Norway, Denmark, Netherlands, France, Germany, Poland, Northern Ireland, Lithuania, Spain, Belgium, Wales, and Sweden.  
+&lt;/p&gt;
+&lt;h4&gt;France&lt;/h4&gt;
+&lt;p&gt;
+There were 309 French vessels with landings in the ecoregion in 2024, decreasing from 362 in 2021. The number of vessels with 80% of their landings in the ecoregion in 2024 was 94. Of these, 11 were &amp;lt;12 m, 28 were 12–24 m, 49 were 24–40 m and 6 were &amp;gt; 40 m. The main species landed by volume are hake, anglerfish, blue whiting, saithe, and mackerel. In terms of landings value, the main species are anglerfish, hake, saithe, john
+dory, and albacore.
+&lt;/p&gt;
+&lt;h4&gt;Ireland&lt;/h4&gt;
+&lt;p&gt;
+There were 1 287 Irish vessels with landings in the ecoregion in 2024, decreasing from 1 313 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 1 274. Of these, 1 078 were &amp;lt;12 m, 118 were 12–24 m, 58 were 24–40 m and 20 were &amp;gt; 40 m. The main species landed by volume are mackerel, blue whiting, horse mackerel, sprat, and nephrops. In terms of landings value, the main species are nephrops, mackerel, blue whiting, brown crab, and horse mackerel.
+&lt;/p&gt;
+&lt;h4&gt;United Kingdom – Scotland&lt;/h4&gt;
+&lt;p&gt;
+There were 1 026 Scottish vessels with landings in the ecoregion in 2024, decreasing from 1 173 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 589. Of these, 472 were &amp;lt;12 m, 90 were 12–24 m, 23 were 24–40 m and 4 were &amp;gt; 40 m. The main species landed by volume are mackerel, blue whiting, herring, haddock, and Nephrops. In terms of value, the main species are mackerel, Nephrops,
+anglerfish, herring, and haddock.
+&lt;/p&gt;
+&lt;h4&gt;United Kingdom – Northern Ireland&lt;/h4&gt;
+&lt;p&gt;
+There were 180 Northern Ireland vessels with landings in the ecoregion in 2024, decreasing from 236 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 120. Of these, 63 were &amp;lt;12 m, 52 were 12–24 m, 4 were 24–40 m and 1 was &amp;gt; 40 m. The main species landed by volume are mackerel, herring, Nephrops, brown crab, and horse mackerel. In terms of value, the main species are Nephrops, mackerel, herring, brown crab, and scallops.
+&lt;/p&gt;
+&lt;h4&gt;United Kingdom – England and Wales&lt;/h4&gt;
+&lt;p&gt;
+There were 860 English vessels with landings in the ecoregion in 2024, decreasing from 924 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 506. Of these, 384 were &amp;lt;12 m, 88 were 12–24 m, 33 were 24–40 m and 1 was &amp;gt;40 m. The main species landed by volume are mackerel, blue whiting, pilchard, anglerfish, and brown crab. In terms of value, the main species are anglerfish, sole, brown crab,
+lobster, and hake.
+&lt;/p&gt;
+&lt;p&gt;
+There were 227 Welsh vessels with landings in the ecoregion in 2024, decreasing from 250 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 165. Of these, 155 were &amp;lt;12 m, 8 were 12–24 m, 2 were 24–40 m and 0 were &amp;gt; 40 m. The main species landed by volume are whelk, anglerfish, scallop, megrim, and brown crab. In terms of value, the main species are whelk, lobster, anglerfish, seabass, and brown crab.
+&lt;/p&gt;
+&lt;h4&gt;Spain&lt;/h4&gt;
+&lt;p&gt;
+There were 146 Spanish vessels with landings in the ecoregion in 2024, increasing from 79 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 32. Of these, 0 were &amp;lt;12 m, 0 were 12–24 m, 32 were 24–40 m and 0 were &amp;gt; 40 m. The main species landed by volume are hake, megrim, ling, blue shark, and witch. In terms of value, the main species are hake, megrim, Nephrops, ling, and greater forkbeard.
+&lt;/p&gt;
+&lt;h4&gt;Other countries&lt;/h4&gt;
+&lt;p&gt;
+About 60 Norwegian vessels operate in the ecoregion. Pelagic trawlers mainly target blue whiting but also target other
+pelagic species. There is also a demersal longline fishery that mainly targets ling and blue ling.
+&lt;/p&gt;
+&lt;p&gt;
+The Belgian fleet consists of about 65 active vessels, of which about 21 operate in the Irish Sea. The majority (89%) of those operating in the Irish Sea are between 24 and 40 m, while the remainder are between 18 and 24 m. The Belgian fleet uses beam trawls and otter trawls for rays, plaice, sole, and anglerfish.
+&lt;/p&gt;
+&lt;p&gt;
+Seven German vessels operate in the Celtic Seas, one of which takes 80% of their catch in the ecoregion. This includes vessels that mainly target anglerfish and hake with gillnets and longline, as well as freezer trawlers that target blue whiting, horse
+mackerel, and mackerel.
+&lt;/p&gt;
+&lt;p&gt;
+One large (&amp;gt; 40 m) Lithuanian freezer trawler targets pelagic species.
+&lt;/p&gt;
+&lt;p&gt;
+There are 16 large Dutch pelagic freezer trawlers operating in the ecoregion, mainly targeting blue whiting, horse mackerel,
+and mackerel.
+&lt;/p&gt;
+&lt;p&gt;
+The Danish fleet consists of sixteen vessels, one of which has more than 80% of their landings in the ecoregion. Blue whiting
+is the main species for the fleet by weight and mackerel is the main species by value.
+&lt;/p&gt;
+&lt;p&gt;
+Vessels from the Faroe Islands also operate in this ecoregion, targeting blue whiting with pelagic trawls.
+&lt;/p&gt;
+&lt;h4&gt;Recreational fisheries&lt;/h4&gt;
+&lt;p&gt;
+Recreational fishing is an important activity in the Celtic Sea that harvests a diverse range of species from a variety of platforms (e.g. shore, boat, and charters) using many gears (e.g. rod and line, speargun, nets, pots, and traps). The main countries with recreational fisheries are UK and Ireland, where no licence is required. Angling from shore and boat is the most popular method, with a number of charter boats offering trips. Catches can be significant, representing around 46% and 67% of total removals of sea bass and Pollack, respectively, according to the latest ICES advice. The main target species include mackerel, pollack, sea bass, saithe, cod, spurdog, flatfish (plaice, dab, flounder, and sole), sea bream, wrasse, and whiting. Recreational fisheries data is included in the pollack and sea bass stock assessments in the ecoregion. Sharks, skates, rays, shellfish, crustaceans, and cephalopods are also caught by recreational fishers
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>effort_SAR</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Fishing effort&lt;/h4&gt;
+&lt;p&gt;
+Spatial distribution of average annual fishing effort (mW fishing hours) in the years 2021–2024, by gear type. Fishing effort data are only shown for vessels &gt; 12 m with vessel monitoring systems (VMS)‡; this will bias the distributions, particularly in coastal areas. In the legend, “n” gives the number of c-squares attributed to that level.
+&lt;/p&gt; 
+&lt;p&gt;
+‡ Details on countries submitting VMS and logbook data can be found at &lt;a href="https://data.ices.dk/vms/inventory" target="_blank"&gt;ICES VMS and Logbook DataBase&lt;/a&gt;
+&lt;/p&gt; 
+&lt;h4&gt;Swept Area Ratio&lt;/h4&gt;
+&lt;p&gt;
+Average annual (2021–2024) surface (left panel) and subsurface (right panel) disturbance by mobile
+bottom-contacting fishing gear (bottom otter trawls, bottom seines, dredges, and beam trawls) in the ecoregion, expressed as average swept-area ratios (SAR).&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>&lt;ul&gt;
   &lt;li&gt;
     The majority of the fisheries in the Azores ecoregion are targeted by Azorean vessels. Only a small proportion of catch is taken by surface longliners from mainland Portugal and Spain targeting swordfish and blue shark. The fisheries are classified as small scale because around 60% of the vessels are under nine metres in length and target many different species. The most important targets are tuna and tuna-like species (in weight), deep-water demersal species (in value), and small pelagic species. The most important fishing methods are handline and bottom longline, followed by pole and line (bait boats). Surface longline is also used but mainly by non-regional vessels that operate outside a 100 nautical mile area. The Azores Exclusive Economic Zone (EEZ) is recognized as a no take area for nets (including a trawl ban) excluding a few small coastal gillnets and purse seiners for small pelagics.
@@ -4168,7 +4324,40 @@
 &lt;/ul&gt;
 &lt;p&gt;
   The fisheries overview document (pdf) is accessible at:
-  &lt;a href="https://doi.org/10.17895/ices.advice.27880014"&gt;ICES Library&lt;/a&gt;
+  &lt;a href="https://doi.org/10.17895/ices.advice.27880014" target="_blank"&gt;ICES Library&lt;/a&gt;
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;
+  &lt;li&gt;
+    The commercial fisheries in the ecoregion target a wide variety of stocks, resulting in a diverse and spatially varied fishing industry. The countries with the largest landings and effort in the ecoregion are Spain, Portugal, and France, with minor landings from Ireland, Belgium, and UK. The most common gear used in the area is bottom trawls, which target demersal species. The highest landings, however, are taken by midwater trawls mainly targeting species such as blue whiting, mackerel, and to a lesser extent species such as sardine.
+  &lt;/li&gt;
+  &lt;li&gt;
+    Of the wide variety of stocks both targeted and caught as bycatch, 73 are evaluated by ICES for spawning stock biomass (SSB) size and fishing pressure. Twenty-two stocks have been evaluated against maximum sustainable yield (MSY) reference points for fishing mortality, and 86% of these are fished below FMSY.
+  &lt;/li&gt;
+  &lt;li&gt;
+    In addition to biomass removal, ecosystem effects of fisheries include abrasion, ghost fishing, damage to benthic fauna by demersal trawling, and bycatch of marine mammals, elasmobranchs, and seabirds. Several regulatory and research efforts are in place or are being developed that are aimed at reducing the impact of fishing on the ecosystem.
+  &lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;
+  The fisheries overview document (pdf) is accessible at:
+  &lt;a href="https://doi.org/10.17895/ices.advice.27879951" target="_blank"&gt;ICES Library&lt;/a&gt;
+&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;
+  &lt;li&gt;
+    The commercial fisheries in the Barents Sea Ecoregion target few stocks. The largest pelagic fishery targets capelin (cap.27.1-2) using midwater trawl. The largest demersal fisheries target cod (cod.27.1-2), haddock (had.27.1-2), and other gadoids, predominantly using trawls, gillnets, longlines, and handlines. The crustacean fisheries target deep-sea prawn, red king crab, and snow crab. Harp seals and minke whales are also hunted in the region.
+  &lt;/li&gt;
+  &lt;li&gt;
+    Twelve nations currently have fisheries targeting the stocks in this ecoregion. Norway and Russian Federation have the largest fleets and dominate the landings in the region. Total landings peaked in the mid-1970s and have been at a lower level for the last two decades. Catches of capelin have varied, from being the largest catches in the region (by weight) at some points in time to zero catches at others. Pelagic trawling in the ecoregion tends to catch only one species at a time, whereas demersal trawling normally catches several species simultaneously.
+  &lt;/li&gt;
+  &lt;li&gt;
+    In addition to biomass removal, the ecosystem effects of fisheries include abrasion, ghost fishing, damage to benthic fauna by demersal trawling, bycatch of elasmobranchs in demersal fisheries, bycatch of seabirds in gillnet and longline fisheries, and bycatch of harbour porpoise in gillnet fisheries. Several regulatory and research efforts to reduce the impact of fishing on the ecosystem are in place or being developed.
+  &lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;
+ The fisheries overview document (pdf) is accessible at   &lt;a href="https://doi.org/10.17895/ices.advice.18667634.v1" target="_blank"&gt;ICES Library&lt;/a&gt;
 &lt;/p&gt;</t>
   </si>
   <si>
@@ -4209,48 +4398,24 @@
 &lt;/ul&gt;
 &lt;p&gt;
   The fisheries overview document (pdf) is accessible at:
-  &lt;a href="https://doi.org/10.17895/ices.advice.27880068"&gt;ICES Library&lt;/a&gt;
+  &lt;a href="https://doi.org/10.17895/ices.advice.27880068" target="_blank"&gt;ICES Library&lt;/a&gt;
 &lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;
-  &lt;li&gt;
-    The commercial fisheries in the ecoregion target a wide variety of stocks, resulting in a diverse and spatially varied fishing industry. The countries with the largest landings and effort in the ecoregion are Spain, Portugal, and France, with minor landings from Ireland, Belgium, and UK. The most common gear used in the area is bottom trawls, which target demersal species. The highest landings, however, are taken by midwater trawls mainly targeting species such as blue whiting, mackerel, and to a lesser extent species such as sardine.
-  &lt;/li&gt;
-  &lt;li&gt;
-    Of the wide variety of stocks both targeted and caught as bycatch, 73 are evaluated by ICES for spawning stock biomass (SSB) size and fishing pressure. Twenty-two stocks have been evaluated against maximum sustainable yield (MSY) reference points for fishing mortality, and 86% of these are fished below FMSY.
-  &lt;/li&gt;
-  &lt;li&gt;
-    In addition to biomass removal, ecosystem effects of fisheries include abrasion, ghost fishing, damage to benthic fauna by demersal trawling, and bycatch of marine mammals, elasmobranchs, and seabirds. Several regulatory and research efforts are in place or are being developed that are aimed at reducing the impact of fishing on the ecosystem.
-  &lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;
-  The fisheries overview document (pdf) is accessible at:
-  &lt;a href="https://doi.org/10.17895/ices.advice.27879951"&gt;ICES Library&lt;/a&gt;
-&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;h4&gt;Discard trends&lt;/h4&gt;
-&lt;p&gt;
-Discard trends by fish fisheries guild shown as percentages (%) of the total annual catch in that
-category. 
-Some catches may occur outside the ecoregion and not all stock catches are disaggregated between landings
-and discards.
-&lt;/p&gt;
-&lt;h4&gt;Current discards&lt;/h4&gt;
-&lt;p&gt;
-Left/top panel: landings (green) and discards (orange) by fisheries guild
-(in thousand tonnes) only of the stocks with recorded discards. 
-Right/bottom panel: landings (green) and discards (orange) by fisheries guild (in thousand tonnes) of all
-stocks that have some catches in the ecoregion.
-&lt;/p&gt;
-&lt;p&gt;Elasmobranch discard data might be highly uncertain, precaution is advised when interpreting the results.&lt;/p&gt;
-&lt;h4&gt;Results description&lt;/h4&gt;
-&lt;p&gt;The average discard rate among pelagic stocks is estimated to be very low. &lt;/p&gt;
-&lt;p&gt;The estimated average discard rate for elasmobranchs stocks is high and ranges 30% to 75%. &lt;/p&gt;
-&lt;p&gt;The average discard rate among demersal stocks ranges from 9% to 22% and is generally around 15%. &lt;/p&gt;
-&lt;p&gt;Crustacean and benthic stocks have an estimated average discard rate of around 10%. &lt;/p&gt;
-&lt;p&gt;Discard rates for some species are very high in the ecoregion, for example plaice (around 60% of tonnage) and whiting (50–99% of tonnage).&lt;/p&gt;</t>
+  &lt;li&gt;Vessel numbers have declined across the majority of the countries fishing in the ecoregion in the past decade.&lt;/li&gt;
+  &lt;li&gt;Total landings fluctuated around 1 million tonnes between 2014 and 2020, and have been lower, at 0.77–0.92 million tonnes, in 2021–2023. Pelagic fisheries continue to dominate landings by volume.&lt;/li&gt;
+  &lt;li&gt;Discard rates of elasmobranch stocks are high (&amp;gt; 30%)&lt;/li&gt;
+  &lt;li&gt;Average fishing mortalities have generally declined since the mid-1990s for stocks within the benthic, demersal and elasmobranch guilds.&lt;/li&gt;
+&lt;li&gt; Some stocks continue to be fished above F&lt;sub&gt;MSY&lt;/sub&gt;, including mackerel and blue whiting in the pelagic guild. &lt;/li&gt;
+  &lt;li&gt;On average, the spawning stock size in all guilds is currently above the target (SSB/MSY B&lt;sub&gt;trigger&lt;/sub&gt; &amp;gt; 1), although some of the stocks including gadoids in the Celtic Sea (cod, haddock and whiting) remain below MSY B&lt;sub&gt;trigger&lt;/sub&gt;. The status of mackerel was below MSY B&lt;sub&gt;trigger&lt;/sub&gt; in 2024 and 2025.&lt;/li&gt;
+  &lt;li&gt;Changes in species interactions, diets and fish distributions are affecting stock abundances and fisheries in the Celtic Sea.&lt;/li&gt;
+  &lt;li&gt;In relation to mixed fisheries:&lt;/li&gt;&lt;ul&gt;
+  &lt;li&gt;Landings shares for individual stocks are dominated by demersal trawl métiers (demersal fish or Nephrops) and beam trawl métiers (benthic flatfish and skates and rays), though longlines and gillnets have a significant landing share for some stocks in the Celtic Sea (e.g. hake and ling), as do pots in the West of Scotland (Nephrops).&lt;/li&gt;
+  &lt;li&gt;Fleet landings compositions in the Celtic Sea have remained relatively stable since 2015, with some trends over time in some fleets towards dominant stocks. There can be significant differences in landings composition between gear type and country within the same gear type, reflecting different targeting and gear efficiencies.&lt;/li&gt;
+  &lt;li&gt;Annual mixed fisheries forecasts indicate that most fleets are limited by the zero catch advice for cod, haddock and whiting in the Celtic Sea. No forecasts are available for the Irish Sea or the West of Scotland.&lt;/li&gt;
+&lt;/ul&gt;&lt;/ul&gt;
+&lt;p&gt;The fisheries overview document (pdf) is accessible at   &lt;a href="https://doi.org/10.17895/ices.advice.30710879" target="_blank"&gt;ICES Library&lt;/a&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;
@@ -4259,95 +4424,8 @@
   &lt;li&gt;Discarding is prohibited in the pelagic fishery. Discarding in the demersal fisheries is considered negligible; however, there are no reliable estimates of potential discards.&lt;/li&gt;&lt;br&gt;
   &lt;li&gt;Stocks within the ecoregion are assessed for stock status and fishing pressure. Half of the stocks have a wider spatial distribution outside the ecoregion. The fishing pressure (in relation to FMSY) of demersal stocks has decreased since 2000 but is currently above sustainable limits. The biomass (in relation to MSY Btrigger) has increased in recent years. For the pelagic fisheries the fishing pressure has been around FMSY since 2010, but the stock size has decreased since 2017.&lt;/li&gt;&lt;br&gt;
   &lt;li&gt;Data on incidental bycatch of marine mammals and seabird species are scarce. Gillnets are banned in waters of less than 380 m depth around the Faroes, which might reduce both seabird and marine mammal bycatch in the region.&lt;/li&gt;&lt;br&gt;
-  &lt;li&gt;The fisheries overview document (pdf) is accessible at: &lt;a href="https://doi.org/10.17895/ices.advice.27879915"&gt;ICES Library&lt;/a&gt;&lt;/li&gt;&lt;br&gt;
+  &lt;li&gt;The fisheries overview document (pdf) is accessible at: &lt;a href="https://doi.org/10.17895/ices.advice.27879915" target="_blank"&gt;ICES Library&lt;/a&gt;&lt;/li&gt;&lt;br&gt;
 &lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;
-  &lt;li&gt;Fisheries management measures for major stocks (e.g. cod, haddock, saithe, and herring) have resulted in decreased fishing pressure – close to or at F&lt;sub&gt;MSY&lt;/sub&gt; or HR&lt;sub&gt;MSY&lt;/sub&gt; – and increased SSBs for the past two decades.&lt;/li&gt;
-  &lt;li&gt;There has been an overall reduction in fishing effort since 1991 for all fisheries – except those using handlines, where it has increased. The decrease in trawl effort is likely to have reduced pressure on benthic habitats.&lt;/li&gt;
-  &lt;li&gt;Three pelagic fisheries have seen increased effort and landings due to changes in migration patterns linked to prey availability, oceanographic conditions, and stock abundance: a blue whiting fishery (starting in the late 1990s), the Atlantic mackerel fishery (commencing mid-2000s), and the Norwegian spring-spawning herring fishery (recommencing at the turn of the century).&lt;/li&gt;
-  &lt;li&gt;Fishing grounds of several species (e.g. haddock, anglerfish, ling, lemon sole, and witch) have expanded to the northern part of the ecoregion due to species redistribution associated with increased water temperature.&lt;/li&gt;
-  &lt;li&gt;Several species—including Atlantic halibut, spotted wolfish, Norway lobster, and northern shrimp—have shown substantial decreases in stock sizes due to factors such as high fishing pressure and reduced productivity. Directed fisheries for Atlantic halibut and Norway lobster are currently prohibited.&lt;/li&gt;
-  &lt;li&gt;Legislation to recommence hunting of fin and minke whales was passed in 2009. However, catches are not made every year.&lt;/li&gt;
-  &lt;li&gt;The highest cumulative multiannual bycatch rate of protected, endangered, and threatened species was recorded in set gillnets. At species level, the highest seabird bycatch rates were for guillemot and common eider, and the highest marine mammal bycatch rates for harbour porpoise and harbour seal. The estimated annual seabird bycatch in the gillnet lumpfish fishery has decreased in recent years, though the driver is unclear.&lt;/li&gt;
-  &lt;li&gt;The summer feeding grounds of capelin have shifted from the Icelandic Waters ecoregion to the Greenland Sea ecoregion. While this does not directly affect the Icelandic winter capelin fishery, it may indirectly influence the distribution and growth of predator stocks on which other fisheries depend.&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;
-  The fisheries overview document (pdf) is accessible at:  
-  &lt;a href="https://doi.org/10.17895/ices.advice.27879909" target="_blank"&gt;ICES Library&lt;/a&gt;
-&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;
-  &lt;li&gt;
-    The largest landings in this ecoregion are by Norway, the Russian Federation (Russia henceforth), Faroe Islands, and Iceland, mainly by pelagic fisheries. Other nations also have fisheries in the area. The number of fishing vessels is declining while the size of the remaining vessels is increasing. The annual catch in the ecoregion has varied between 700 000 tonnes to over 2 million tonnes.
-  &lt;/li&gt;
-  &lt;li&gt;
-    The pelagic fisheries, using purse-seine and pelagic trawls, account for the largest catches by weight and target Norwegian spring-spawning (NSS) herring (her.27.1-24a514a), blue whiting (whb.27.1-91214), mackerel (mac.27.nea), and other pelagic species. The largest demersal fishery targets cod (cod.27.1-2), haddock (had.27.1-2), and saithe (pok.27.1-2) using bottom trawls, purse-seine, Danish seine and gillnets, and to a lesser extent hook and line gear. Smaller fisheries target other gadoid species, Greenland halibut (ghl.27.1-2), and beaked redfish (reb.27.1-2). Landings of pelagic species within the ecoregion in the last decades have been variable. The demersal fisheries, dominated by cod, display less pronounced fluctuations than the pelagic fisheries. Information about discards is sparse, but the total weight of discards is considered low in both the pelagic and the demersal fisheries. Harp seals and minke whales are hunted in the region.
-  &lt;/li&gt;
-  &lt;li&gt;
-    Status summaries of Norwegian Sea stocks relative to ICES maximum sustainable yield (MSY) approach and precautionary approach (PA) are known for about 42% of the 19 stocks assessed by ICES in this ecoregion. Only 21% of the stocks are fished below F MSY, accounting for less than 1% of the total catch. 21% of the stocks have a biomass above MSY Btrigger, accounting for 86% of the total catch. Demersal stocks have shown a trend of declining fishing mortality since the mid-1990s, followed by a sharp increase in 2019, largely driven by the exploitation pattern of redfish. In 2021 the average F/F MSY ratio was close to 1. The mean SSB/MSY Btrigger ratio of demersal stocks has been decreasing over the last decade, but mean SSB remains above MSY Btrigger and increased in 2021. The average F/F MSY ratio for pelagic stocks has fluctuated slightly above 1 since 2005. The mean SSB/MSY Btrigger ratio for pelagic species has been well above 1 the last two decades though followed by a recent sharp decline, but remains above 1.
-  &lt;/li&gt;
-  &lt;li&gt;
-    In addition to biomass removal, ecosystem effects of fisheries include abrasion, ghost fishing, and bycatch of protected, endangered, and threatened species.
-  &lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;
-  The fisheries overview document (pdf) is accessible at
-  &lt;a href="https://doi.org/10.17895/ices.advice.27879897"&gt;ICES Library&lt;/a&gt;.
-&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;
-  &lt;li&gt;
-    The commercial fisheries in the Oceanic Northeast Atlantic ecoregion target few
-    stocks. The main fisheries in the area are a multinational fishery on two pelagic
-    beaked redfish stocks in the northwestern part of the ecoregion and a fishery on
-    blue whiting on the Hatton-Rockall plateau and west of the Porcupine Bank using
-    midwater trawl. The demersal fisheries for haddock at Rockall account for only a
-    small proportion of the total catches of haddock taken in this ecoregion. Fishing
-    for tuna (bluefin, skipjack, bigeye, and albacore) and other large pelagic species
-    (swordfish) by long-distance longliners occurs across much of this ecoregion. Very
-    few deep-sea fisheries are conducted in the region.
-  &lt;/li&gt;
-  &lt;li&gt;
-    There are currently around 20 nations with fisheries targeting the stocks in the
-    ecoregion. Norway, Iceland, and the Russian Federation have the largest fleets and
-    dominate the landings in the region. Total landings have varied since the mid-1970s,
-    with a rise in the recent decade mainly due to increased blue whiting catches. Two
-    beaked redfish stocks dominated the catches (by weight) until 2000, but catches of
-    these stocks have decreased considerably since the peak of the fishery in the
-    mid-1990s.
-  &lt;/li&gt;
-  &lt;li&gt;
-    The Oceanic Northeast Atlantic ecoregion has 52 stocks for which ICES provided
-    advice in 2021. Around 13% of the assessed stocks are fished at or below F&lt;sub&gt;MSY&lt;/sub&gt;
-    target levels; around 19% of the stocks were assessed to be above MSY
-    B&lt;sub&gt;trigger&lt;/sub&gt;. The majority of the stocks have unknown stock and fishing
-    mortality statuses.
-  &lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;
- The fisheries overview document (pdf) is accessible at
-  &lt;a href="https://doi.org/10.17895/ices.advice.27880092"&gt;ICES Library&lt;/a&gt;.
-&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;
-  &lt;li&gt;
-    The commercial fisheries in the Barents Sea Ecoregion target few stocks. The largest pelagic fishery targets capelin (cap.27.1-2) using midwater trawl. The largest demersal fisheries target cod (cod.27.1-2), haddock (had.27.1-2), and other gadoids, predominantly using trawls, gillnets, longlines, and handlines. The crustacean fisheries target deep-sea prawn, red king crab, and snow crab. Harp seals and minke whales are also hunted in the region.
-  &lt;/li&gt;
-  &lt;li&gt;
-    Twelve nations currently have fisheries targeting the stocks in this ecoregion. Norway and Russian Federation have the largest fleets and dominate the landings in the region. Total landings peaked in the mid-1970s and have been at a lower level for the last two decades. Catches of capelin have varied, from being the largest catches in the region (by weight) at some points in time to zero catches at others. Pelagic trawling in the ecoregion tends to catch only one species at a time, whereas demersal trawling normally catches several species simultaneously.
-  &lt;/li&gt;
-  &lt;li&gt;
-    In addition to biomass removal, the ecosystem effects of fisheries include abrasion, ghost fishing, damage to benthic fauna by demersal trawling, bycatch of elasmobranchs in demersal fisheries, bycatch of seabirds in gillnet and longline fisheries, and bycatch of harbour porpoise in gillnet fisheries. Several regulatory and research efforts to reduce the impact of fishing on the ecosystem are in place or being developed.
-  &lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;
- The fisheries overview document (pdf) is accessible at   &lt;a href="https://doi.org/10.17895/ices.advice.18667634.v1"&gt;ICES Library&lt;/a&gt;
-&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;
@@ -4384,115 +4462,63 @@
 &lt;/li&gt;
 &lt;/ul&gt;
 &lt;p&gt;
-  The fisheries overview document (pdf) is accessible at   &lt;a href="https://doi.org/10.17895/ices.advice.30710897"&gt;ICES Library&lt;/a&gt;
+  The fisheries overview document (pdf) is accessible at   &lt;a href="https://doi.org/10.17895/ices.advice.30710897" target="_blank"&gt;ICES Library&lt;/a&gt;
 &lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;
-The Celtic Seas ecoregion covers the northwestern shelf seas of Europe. It includes areas of the deeper eastern Atlantic Ocean and coastal seas that are heavily influenced by oceanic inputs. The ecoregion ranges from north of Shetland to Brittany in the south. Three key areas constitute this ecoregion:
-&lt;/p&gt;
-&lt;ol&gt;
+    <t>&lt;ul&gt;
   &lt;li&gt;
-    northern parts: the Malin shelf, west of Scotland, eastern Rockall Bank, and north of Scotland (parts of Subdivision 2.a.2, divisions 4.a and 6.a, and Subdivision 6.b.2);
+    The largest landings in this ecoregion are by Norway, the Russian Federation (Russia henceforth), Faroe Islands, and Iceland, mainly by pelagic fisheries. Other nations also have fisheries in the area. The number of fishing vessels is declining while the size of the remaining vessels is increasing. The annual catch in the ecoregion has varied between 700 000 tonnes to over 2 million tonnes.
   &lt;/li&gt;
   &lt;li&gt;
-    the Celtic Sea, Bristol Channel, western English Channel, southwest and west of Ireland (Division 7.b and Subdivision 7.c.2; parts of divisions 7.e, 7.f, 7.g, and 7.h and subdivisions 7.j.2 and 7.k.2);
+    The pelagic fisheries, using purse-seine and pelagic trawls, account for the largest catches by weight and target Norwegian spring-spawning (NSS) herring (her.27.1-24a514a), blue whiting (whb.27.1-91214), mackerel (mac.27.nea), and other pelagic species. The largest demersal fishery targets cod (cod.27.1-2), haddock (had.27.1-2), and saithe (pok.27.1-2) using bottom trawls, purse-seine, Danish seine and gillnets, and to a lesser extent hook and line gear. Smaller fisheries target other gadoid species, Greenland halibut (ghl.27.1-2), and beaked redfish (reb.27.1-2). Landings of pelagic species within the ecoregion in the last decades have been variable. The demersal fisheries, dominated by cod, display less pronounced fluctuations than the pelagic fisheries. Information about discards is sparse, but the total weight of discards is considered low in both the pelagic and the demersal fisheries. Harp seals and minke whales are hunted in the region.
   &lt;/li&gt;
   &lt;li&gt;
-    the Irish Sea (Division 7.a).
+    Status summaries of Norwegian Sea stocks relative to ICES maximum sustainable yield (MSY) approach and precautionary approach (PA) are known for about 42% of the 19 stocks assessed by ICES in this ecoregion. Only 21% of the stocks are fished below F MSY, accounting for less than 1% of the total catch. 21% of the stocks have a biomass above MSY Btrigger, accounting for 86% of the total catch. Demersal stocks have shown a trend of declining fishing mortality since the mid-1990s, followed by a sharp increase in 2019, largely driven by the exploitation pattern of redfish. In 2021 the average F/F MSY ratio was close to 1. The mean SSB/MSY Btrigger ratio of demersal stocks has been decreasing over the last decade, but mean SSB remains above MSY Btrigger and increased in 2021. The average F/F MSY ratio for pelagic stocks has fluctuated slightly above 1 since 2005. The mean SSB/MSY Btrigger ratio for pelagic species has been well above 1 the last two decades though followed by a recent sharp decline, but remains above 1.
   &lt;/li&gt;
-&lt;/ol&gt;
-&lt;p&gt;
-In the north, there are strong links with the North Sea; in the southeast, a strong link with the English Channel area; and in the south a strong link with the Bay of Biscay. The eastern part of the Rockall Bank is within the geographic scope of the ecoregion, although it is separated from the western European shelf by the Rockall Trough.
-&lt;/p&gt;
-&lt;p&gt;
-The scientific names of all species described in this overview are listed in the Stock Status Lookup.
-&lt;/p&gt;
-&lt;p&gt;
-The overview covers ICES subareas 27.7 (excluding Division 27.7.d) and 27.6 (hereafter, the “27” area prefixes are omitted).
-Some fisheries statistics do not allow the full differentiation of sections of subareas 4 and 2 or (in earlier years) western sections of subareas 6 and 7, as well as the southeastern section of Division 7.e.
+  &lt;li&gt;
+    In addition to biomass removal, ecosystem effects of fisheries include abrasion, ghost fishing, and bycatch of protected, endangered, and threatened species.
+  &lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;
+  The fisheries overview document (pdf) is accessible at
+  &lt;a href="https://doi.org/10.17895/ices.advice.27879897" target="_blank"&gt;ICES Library&lt;/a&gt;.
 &lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;
-Fourteen nations currently have fisheries targeting the many marine stocks in the ecoregion. These include (by decreasing order of contribution to total landings in 2023): UK, Ireland, Norway, Denmark, Netherlands, France, Germany, Poland, Northern Ireland, Lithuania, Spain, Belgium, Wales, and Sweden.  
-&lt;/p&gt;
-&lt;h4&gt;France&lt;/h4&gt;
-&lt;p&gt;
-There were 309 French vessels with landings in the ecoregion in 2024, decreasing from 362 in 2021. The number of vessels with 80% of their landings in the ecoregion in 2024 was 94. Of these, 11 were &amp;lt;12 m, 28 were 12–24 m, 49 were 24–40 m and 6 were &amp;gt; 40 m. The main species landed by volume are hake, anglerfish, blue whiting, saithe, and mackerel. In terms of landings value, the main species are anglerfish, hake, saithe, john
-dory, and albacore.
-&lt;/p&gt;
-&lt;h4&gt;Ireland&lt;/h4&gt;
-&lt;p&gt;
-There were 1 287 Irish vessels with landings in the ecoregion in 2024, decreasing from 1 313 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 1 274. Of these, 1 078 were &amp;lt;12 m, 118 were 12–24 m, 58 were 24–40 m and 20 were &amp;gt; 40 m. The main species landed by volume are mackerel, blue whiting, horse mackerel, sprat, and nephrops. In terms of landings value, the main species are nephrops, mackerel, blue whiting, brown crab, and horse mackerel.
-&lt;/p&gt;
-&lt;h4&gt;United Kingdom – Scotland&lt;/h4&gt;
-&lt;p&gt;
-There were 1 026 Scottish vessels with landings in the ecoregion in 2024, decreasing from 1 173 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 589. Of these, 472 were &amp;lt;12 m, 90 were 12–24 m, 23 were 24–40 m and 4 were &amp;gt; 40 m. The main species landed by volume are mackerel, blue whiting, herring, haddock, and Nephrops. In terms of value, the main species are mackerel, Nephrops,
-anglerfish, herring, and haddock.
-&lt;/p&gt;
-&lt;h4&gt;United Kingdom – Northern Ireland&lt;/h4&gt;
-&lt;p&gt;
-There were 180 Northern Ireland vessels with landings in the ecoregion in 2024, decreasing from 236 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 120. Of these, 63 were &amp;lt;12 m, 52 were 12–24 m, 4 were 24–40 m and 1 was &amp;gt; 40 m. The main species landed by volume are mackerel, herring, Nephrops, brown crab, and horse mackerel. In terms of value, the main species are Nephrops, mackerel, herring, brown crab, and scallops.
-&lt;/p&gt;
-&lt;h4&gt;United Kingdom – England and Wales&lt;/h4&gt;
-&lt;p&gt;
-There were 860 English vessels with landings in the ecoregion in 2024, decreasing from 924 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 506. Of these, 384 were &amp;lt;12 m, 88 were 12–24 m, 33 were 24–40 m and 1 was &amp;gt;40 m. The main species landed by volume are mackerel, blue whiting, pilchard, anglerfish, and brown crab. In terms of value, the main species are anglerfish, sole, brown crab,
-lobster, and hake.
-&lt;/p&gt;
-&lt;p&gt;
-There were 227 Welsh vessels with landings in the ecoregion in 2024, decreasing from 250 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 165. Of these, 155 were &amp;lt;12 m, 8 were 12–24 m, 2 were 24–40 m and 0 were &amp;gt; 40 m. The main species landed by volume are whelk, anglerfish, scallop, megrim, and brown crab. In terms of value, the main species are whelk, lobster, anglerfish, seabass, and brown crab.
-&lt;/p&gt;
-&lt;h4&gt;Spain&lt;/h4&gt;
-&lt;p&gt;
-There were 146 Spanish vessels with landings in the ecoregion in 2024, increasing from 79 in 2021. The number of vessels with 80% of their catch in the ecoregion in 2024 was 32. Of these, 0 were &amp;lt;12 m, 0 were 12–24 m, 32 were 24–40 m and 0 were &amp;gt; 40 m. The main species landed by volume are hake, megrim, ling, blue shark, and witch. In terms of value, the main species are hake, megrim, Nephrops, ling, and greater forkbeard.
-&lt;/p&gt;
-&lt;h4&gt;Other countries&lt;/h4&gt;
-&lt;p&gt;
-About 60 Norwegian vessels operate in the ecoregion. Pelagic trawlers mainly target blue whiting but also target other
-pelagic species. There is also a demersal longline fishery that mainly targets ling and blue ling.
-&lt;/p&gt;
-&lt;p&gt;
-The Belgian fleet consists of about 65 active vessels, of which about 21 operate in the Irish Sea. The majority (89%) of those operating in the Irish Sea are between 24 and 40 m, while the remainder are between 18 and 24 m. The Belgian fleet uses beam trawls and otter trawls for rays, plaice, sole, and anglerfish.
-&lt;/p&gt;
-&lt;p&gt;
-Seven German vessels operate in the Celtic Seas, one of which takes 80% of their catch in the ecoregion. This includes vessels that mainly target anglerfish and hake with gillnets and longline, as well as freezer trawlers that target blue whiting, horse
-mackerel, and mackerel.
-&lt;/p&gt;
-&lt;p&gt;
-One large (&amp;gt; 40 m) Lithuanian freezer trawler targets pelagic species.
-&lt;/p&gt;
-&lt;p&gt;
-There are 16 large Dutch pelagic freezer trawlers operating in the ecoregion, mainly targeting blue whiting, horse mackerel,
-and mackerel.
-&lt;/p&gt;
-&lt;p&gt;
-The Danish fleet consists of sixteen vessels, one of which has more than 80% of their landings in the ecoregion. Blue whiting
-is the main species for the fleet by weight and mackerel is the main species by value.
-&lt;/p&gt;
-&lt;p&gt;
-Vessels from the Faroe Islands also operate in this ecoregion, targeting blue whiting with pelagic trawls.
-&lt;/p&gt;
-&lt;h4&gt;Recreational fisheries&lt;/h4&gt;
-&lt;p&gt;
-Recreational fishing is an important activity in the Celtic Sea that harvests a diverse range of species from a variety of platforms (e.g. shore, boat, and charters) using many gears (e.g. rod and line, speargun, nets, pots, and traps). The main countries with recreational fisheries are UK and Ireland, where no licence is required. Angling from shore and boat is the most popular method, with a number of charter boats offering trips. Catches can be significant, representing around 46% and 67% of total removals of sea bass and Pollack, respectively, according to the latest ICES advice. The main target species include mackerel, pollack, sea bass, saithe, cod, spurdog, flatfish (plaice, dab, flounder, and sole), sea bream, wrasse, and whiting. Recreational fisheries data is included in the pollack and sea bass stock assessments in the ecoregion. Sharks, skates, rays, shellfish, crustaceans, and cephalopods are also caught by recreational fishers
+    <t>&lt;ul&gt;
+  &lt;li&gt;
+    The commercial fisheries in the Oceanic Northeast Atlantic ecoregion target few
+    stocks. The main fisheries in the area are a multinational fishery on two pelagic
+    beaked redfish stocks in the northwestern part of the ecoregion and a fishery on
+    blue whiting on the Hatton-Rockall plateau and west of the Porcupine Bank using
+    midwater trawl. The demersal fisheries for haddock at Rockall account for only a
+    small proportion of the total catches of haddock taken in this ecoregion. Fishing
+    for tuna (bluefin, skipjack, bigeye, and albacore) and other large pelagic species
+    (swordfish) by long-distance longliners occurs across much of this ecoregion. Very
+    few deep-sea fisheries are conducted in the region.
+  &lt;/li&gt;
+  &lt;li&gt;
+    There are currently around 20 nations with fisheries targeting the stocks in the
+    ecoregion. Norway, Iceland, and the Russian Federation have the largest fleets and
+    dominate the landings in the region. Total landings have varied since the mid-1970s,
+    with a rise in the recent decade mainly due to increased blue whiting catches. Two
+    beaked redfish stocks dominated the catches (by weight) until 2000, but catches of
+    these stocks have decreased considerably since the peak of the fishery in the
+    mid-1990s.
+  &lt;/li&gt;
+  &lt;li&gt;
+    The Oceanic Northeast Atlantic ecoregion has 52 stocks for which ICES provided
+    advice in 2021. Around 13% of the assessed stocks are fished at or below F&lt;sub&gt;MSY&lt;/sub&gt;
+    target levels; around 19% of the stocks were assessed to be above MSY
+    B&lt;sub&gt;trigger&lt;/sub&gt;. The majority of the stocks have unknown stock and fishing
+    mortality statuses.
+  &lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;
+ The fisheries overview document (pdf) is accessible at
+  &lt;a href="https://doi.org/10.17895/ices.advice.27880092" target="_blank"&gt;ICES Library&lt;/a&gt;.
 &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;
-  &lt;li&gt;Vessel numbers have declined across the majority of the countries fishing in the ecoregion in the past decade.&lt;/li&gt;
-  &lt;li&gt;Total landings fluctuated around 1 million tonnes between 2014 and 2020, and have been lower, at 0.77–0.92 million tonnes, in 2021–2023. Pelagic fisheries continue to dominate landings by volume.&lt;/li&gt;
-  &lt;li&gt;Discard rates of elasmobranch stocks are high (&amp;gt; 30%)&lt;/li&gt;
-  &lt;li&gt;Average fishing mortalities have generally declined since the mid-1990s for stocks within the benthic, demersal and elasmobranch guilds.&lt;/li&gt;
-&lt;li&gt; Some stocks continue to be fished above F&lt;sub&gt;MSY&lt;/sub&gt;, including mackerel and blue whiting in the pelagic guild. &lt;/li&gt;
-  &lt;li&gt;On average, the spawning stock size in all guilds is currently above the target (SSB/MSY B&lt;sub&gt;trigger&lt;/sub&gt; &amp;gt; 1), although some of the stocks including gadoids in the Celtic Sea (cod, haddock and whiting) remain below MSY B&lt;sub&gt;trigger&lt;/sub&gt;. The status of mackerel was below MSY B&lt;sub&gt;trigger&lt;/sub&gt; in 2024 and 2025.&lt;/li&gt;
-  &lt;li&gt;Changes in species interactions, diets and fish distributions are affecting stock abundances and fisheries in the Celtic Sea.&lt;/li&gt;
-  &lt;li&gt;In relation to mixed fisheries:&lt;/li&gt;&lt;ul&gt;
-  &lt;li&gt;Landings shares for individual stocks are dominated by demersal trawl métiers (demersal fish or Nephrops) and beam trawl métiers (benthic flatfish and skates and rays), though longlines and gillnets have a significant landing share for some stocks in the Celtic Sea (e.g. hake and ling), as do pots in the West of Scotland (Nephrops).&lt;/li&gt;
-  &lt;li&gt;Fleet landings compositions in the Celtic Sea have remained relatively stable since 2015, with some trends over time in some fleets towards dominant stocks. There can be significant differences in landings composition between gear type and country within the same gear type, reflecting different targeting and gear efficiencies.&lt;/li&gt;
-  &lt;li&gt;Annual mixed fisheries forecasts indicate that most fleets are limited by the zero catch advice for cod, haddock and whiting in the Celtic Sea. No forecasts are available for the Irish Sea or the West of Scotland.&lt;/li&gt;
-&lt;/ul&gt;&lt;/ul&gt;
-&lt;p&gt;The fisheries overview document (pdf) is accessible at   &lt;a href="https://doi.org/10.17895/ices.advice.30710879"&gt;ICES Library&lt;/a&gt;&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -8194,7 +8220,7 @@
         <v>882</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>925</v>
+        <v>928</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" ht="303" customHeight="1" x14ac:dyDescent="0.3">
@@ -8225,7 +8251,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -8248,7 +8274,7 @@
         <v>882</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>922</v>
+        <v>929</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -8276,7 +8302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{744F2D0C-79DF-4FE3-924E-E680015F9291}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -8299,7 +8325,7 @@
         <v>882</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>923</v>
+        <v>930</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
@@ -8529,7 +8555,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
     </row>
   </sheetData>
@@ -8627,7 +8653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C69BDA-CBD4-4A20-96F1-D4184C7A4A9F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -8650,7 +8676,7 @@
         <v>882</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>916</v>
+        <v>922</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
@@ -9194,8 +9220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58BB4192-B3A0-40C4-9076-17E7860549D0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9217,7 +9243,7 @@
         <v>882</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>918</v>
+        <v>923</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
@@ -9469,8 +9495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051B8018-23E1-4D0A-B47D-B5B875F199B2}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9522,17 +9548,20 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -9543,12 +9572,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="271.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
+        <v>920</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -9557,17 +9586,17 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD5BEFF-ABF3-4924-AB24-FF61AF228C0E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -9578,12 +9607,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="271.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
+        <v>920</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -9592,18 +9621,17 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{924E1A3D-452D-420C-B25E-B5B00D9E4E1C}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="159.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -9614,12 +9642,82 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="271.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
+        <v>920</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>921</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D815AD19-E228-474C-9937-3BF8367B118E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="271.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>921</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D15E140-89C9-45F3-80F4-6B8F3C0CB47C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="271.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -9678,6 +9776,287 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE1070B-144A-405D-8FC5-7DE029CC4010}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="271.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>921</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F29691E-1FE6-43C9-8319-10047CCCEDC2}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="271.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>921</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44602A52-179B-4771-A428-8A5F60E9F4E5}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="271.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>921</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A8B149-F3B9-47FC-B67F-BAF2CCCF6F3A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="271.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>921</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407DE1E1-ED4A-4EC4-9635-4F064BD979D5}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="271.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>921</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD0BC59-9F8E-4902-8633-6FC5285FFBA9}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="271.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>921</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="159.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA59C6F2-69D0-4598-BA12-1B489ABE98B2}">
   <dimension ref="A1:B4"/>
@@ -9705,7 +10084,7 @@
         <v>882</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>917</v>
+        <v>925</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
@@ -9733,7 +10112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB1D8E1-BE83-467E-ABE2-EB20A46DABB5}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -9756,7 +10135,7 @@
         <v>882</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
@@ -9764,7 +10143,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>926</v>
+        <v>918</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
@@ -9772,7 +10151,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
     </row>
   </sheetData>
@@ -9784,7 +10163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{385D6F23-1F00-43DA-8201-777B854F56F6}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -9807,7 +10186,7 @@
         <v>882</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>920</v>
+        <v>927</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
@@ -9844,8 +10223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A026B00C-E4B3-4E36-BEA1-AD93DF3D486F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9867,7 +10246,7 @@
         <v>882</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
@@ -9896,7 +10275,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>